<commit_message>
Added formula to confidence level interval for sample standard deviation
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696FB9A2-F16D-0448-98EF-C49680A0FC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3A615C-B0CD-334E-95CB-093EC9309C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
@@ -802,15 +802,9 @@
     <t>sample mean</t>
   </si>
   <si>
-    <t>Proportion</t>
-  </si>
-  <si>
     <t>std dev proportion</t>
   </si>
   <si>
-    <t>Assignment #4 Question 8</t>
-  </si>
-  <si>
     <t>lower limit</t>
   </si>
   <si>
@@ -833,6 +827,12 @@
   </si>
   <si>
     <t>Normal Distribution Sampling</t>
+  </si>
+  <si>
+    <t>sample std dev</t>
+  </si>
+  <si>
+    <t>population</t>
   </si>
 </sst>
 </file>
@@ -847,7 +847,7 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -873,16 +873,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -904,17 +907,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -952,7 +950,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -974,12 +972,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,7 +1073,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1289,10 +1281,7 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1300,27 +1289,17 @@
     <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1336,7 +1315,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1349,11 +1327,63 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -12641,21 +12671,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="121">
+      <c r="C17" s="114">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="122"/>
+      <c r="D17" s="115"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="121">
+      <c r="C18" s="114">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="122"/>
+      <c r="D18" s="115"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -16723,7 +16753,7 @@
   <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16735,15 +16765,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="121" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
@@ -16937,15 +16967,15 @@
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="123" t="s">
+      <c r="A14" s="121" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -17114,13 +17144,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="125" t="s">
+      <c r="A26" s="117" t="s">
         <v>201</v>
       </c>
       <c r="B26" s="83">
         <v>29</v>
       </c>
-      <c r="C26" s="127">
+      <c r="C26" s="119">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17129,11 +17159,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="126"/>
+      <c r="A27" s="118"/>
       <c r="B27" s="81">
         <v>37</v>
       </c>
-      <c r="C27" s="128"/>
+      <c r="C27" s="120"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17149,15 +17179,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="124" t="s">
+      <c r="A30" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="124"/>
-      <c r="C30" s="124"/>
-      <c r="D30" s="124"/>
-      <c r="E30" s="124"/>
-      <c r="F30" s="124"/>
-      <c r="G30" s="124"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="116"/>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="116"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17190,7 +17220,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="83" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B34" s="84">
         <v>1</v>
@@ -17260,7 +17290,7 @@
         <v>8.4361799794053529E-27</v>
       </c>
       <c r="E38" s="85" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F38" s="95">
         <f>B32 - (B34 * B33)</f>
@@ -17282,7 +17312,7 @@
       </c>
       <c r="D39" s="94"/>
       <c r="E39" s="89" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F39" s="95">
         <f>B32 + (B34 * B33)</f>
@@ -17292,13 +17322,13 @@
       <c r="H39" s="79"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="125" t="s">
+      <c r="A40" s="117" t="s">
         <v>201</v>
       </c>
       <c r="B40" s="83">
         <v>3300</v>
       </c>
-      <c r="C40" s="127">
+      <c r="C40" s="119">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
         <v>0</v>
       </c>
@@ -17307,11 +17337,11 @@
       <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="126"/>
+      <c r="A41" s="118"/>
       <c r="B41" s="81">
         <v>4200</v>
       </c>
-      <c r="C41" s="128"/>
+      <c r="C41" s="120"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
       <c r="H41" s="79"/>
@@ -17338,15 +17368,15 @@
       <c r="H44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="124" t="s">
+      <c r="A46" s="116" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="124"/>
-      <c r="C46" s="124"/>
-      <c r="D46" s="124"/>
-      <c r="E46" s="124"/>
-      <c r="F46" s="124"/>
-      <c r="G46" s="124"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="116"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="83" t="s">
@@ -17439,23 +17469,23 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="125" t="s">
+      <c r="A58" s="117" t="s">
         <v>201</v>
       </c>
       <c r="B58" s="83">
         <v>2</v>
       </c>
-      <c r="C58" s="127">
+      <c r="C58" s="119">
         <f>_xlfn.BINOM.DIST(B59,$B$48,$B$49,TRUE) - _xlfn.BINOM.DIST(B58,$B$48,$B$49,TRUE)</f>
         <v>0.30165667656250023</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="126"/>
+      <c r="A59" s="118"/>
       <c r="B59" s="81">
         <v>6</v>
       </c>
-      <c r="C59" s="128"/>
+      <c r="C59" s="120"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="97"/>
@@ -17473,15 +17503,15 @@
       <c r="C62" s="94"/>
     </row>
     <row r="64" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A64" s="124" t="s">
+      <c r="A64" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="B64" s="124"/>
-      <c r="C64" s="124"/>
-      <c r="D64" s="124"/>
-      <c r="E64" s="124"/>
-      <c r="F64" s="124"/>
-      <c r="G64" s="124"/>
+      <c r="B64" s="116"/>
+      <c r="C64" s="116"/>
+      <c r="D64" s="116"/>
+      <c r="E64" s="116"/>
+      <c r="F64" s="116"/>
+      <c r="G64" s="116"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="83" t="s">
@@ -17548,23 +17578,23 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="125" t="s">
+      <c r="A73" s="117" t="s">
         <v>201</v>
       </c>
       <c r="B73" s="83">
         <v>2</v>
       </c>
-      <c r="C73" s="127">
+      <c r="C73" s="119">
         <f>_xlfn.POISSON.DIST(B74,$B$66,TRUE) - _xlfn.POISSON.DIST(B73,$B$66,TRUE)</f>
         <v>3.8791531399499785E-3</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="126"/>
+      <c r="A74" s="118"/>
       <c r="B74" s="81">
         <v>5</v>
       </c>
-      <c r="C74" s="128"/>
+      <c r="C74" s="120"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="97"/>
@@ -17587,15 +17617,15 @@
       <c r="C78" s="94"/>
     </row>
     <row r="79" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A79" s="124" t="s">
+      <c r="A79" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="B79" s="124"/>
-      <c r="C79" s="124"/>
-      <c r="D79" s="124"/>
-      <c r="E79" s="124"/>
-      <c r="F79" s="124"/>
-      <c r="G79" s="124"/>
+      <c r="B79" s="116"/>
+      <c r="C79" s="116"/>
+      <c r="D79" s="116"/>
+      <c r="E79" s="116"/>
+      <c r="F79" s="116"/>
+      <c r="G79" s="116"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B80" s="80"/>
@@ -17666,25 +17696,25 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="125" t="s">
+      <c r="A87" s="117" t="s">
         <v>201</v>
       </c>
       <c r="B87" s="84">
         <f>2.1/6</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="C87" s="127">
+      <c r="C87" s="119">
         <f>_xlfn.EXPON.DIST(B88,$B$81,TRUE) - _xlfn.EXPON.DIST(B87,$B$81,TRUE)</f>
         <v>0.25047716007445753</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="126"/>
+      <c r="A88" s="118"/>
       <c r="B88" s="81">
         <f>4.5/6</f>
         <v>0.75</v>
       </c>
-      <c r="C88" s="128"/>
+      <c r="C88" s="120"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="97"/>
@@ -17707,15 +17737,15 @@
       <c r="C92" s="94"/>
     </row>
     <row r="93" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A93" s="124" t="s">
+      <c r="A93" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="B93" s="124"/>
-      <c r="C93" s="124"/>
-      <c r="D93" s="124"/>
-      <c r="E93" s="124"/>
-      <c r="F93" s="124"/>
-      <c r="G93" s="124"/>
+      <c r="B93" s="116"/>
+      <c r="C93" s="116"/>
+      <c r="D93" s="116"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="116"/>
+      <c r="G93" s="116"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D94" s="75"/>
@@ -17871,7 +17901,7 @@
       <c r="G107" s="79"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="106"/>
+      <c r="A108" s="105"/>
       <c r="B108" s="79"/>
       <c r="C108" s="79"/>
       <c r="D108" s="79"/>
@@ -17883,7 +17913,7 @@
       <c r="A109" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="B109" s="103">
+      <c r="B109" s="102">
         <v>4</v>
       </c>
       <c r="C109" s="79"/>
@@ -17896,7 +17926,7 @@
       <c r="A110" s="83" t="s">
         <v>211</v>
       </c>
-      <c r="B110" s="103">
+      <c r="B110" s="102">
         <v>7</v>
       </c>
       <c r="C110" s="79"/>
@@ -17922,7 +17952,7 @@
       <c r="A112" s="83" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="103">
+      <c r="B112" s="102">
         <f>B111*B109</f>
         <v>300</v>
       </c>
@@ -17956,7 +17986,7 @@
       <c r="C115" s="95">
         <v>0.35</v>
       </c>
-      <c r="D115" s="104">
+      <c r="D115" s="103">
         <f>C115*($B$110*MIN($B$111, B115) - $B$112)</f>
         <v>-43.75</v>
       </c>
@@ -17971,7 +18001,7 @@
       <c r="C116" s="95">
         <v>0.2</v>
       </c>
-      <c r="D116" s="104">
+      <c r="D116" s="103">
         <f t="shared" ref="D116:D117" si="5">C116*($B$110*MIN($B$111, B116) - $B$112)</f>
         <v>10</v>
       </c>
@@ -17986,7 +18016,7 @@
       <c r="C117" s="95">
         <v>0.45</v>
       </c>
-      <c r="D117" s="104">
+      <c r="D117" s="103">
         <f t="shared" si="5"/>
         <v>101.25</v>
       </c>
@@ -17995,13 +18025,20 @@
       <c r="A118" s="79"/>
       <c r="B118" s="79"/>
       <c r="C118" s="79"/>
-      <c r="D118" s="105">
+      <c r="D118" s="104">
         <f>SUM(D115:D117)</f>
         <v>67.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="A93:G93"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
@@ -18012,13 +18049,6 @@
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="C87:C88"/>
     <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18027,10 +18057,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E279595A-CDC1-E441-A6DF-F172F4F13CC6}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18041,228 +18071,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="116" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="120" t="s">
-        <v>240</v>
+      <c r="B3" s="113" t="s">
+        <v>238</v>
       </c>
       <c r="C3" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="114">
+      <c r="D3" s="108">
         <f>AVERAGE(A4:A23)</f>
         <v>34.6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="115">
+      <c r="A4" s="109">
         <v>25</v>
       </c>
-      <c r="B4" s="120" cm="1">
+      <c r="B4" s="113" cm="1">
         <f t="array" ref="B4:B23">_xlfn._xlws.SORT(A4:A23)</f>
         <v>5</v>
       </c>
-      <c r="C4" s="120"/>
+      <c r="C4" s="113"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="115">
+      <c r="A5" s="109">
         <v>20</v>
       </c>
-      <c r="B5" s="120">
+      <c r="B5" s="113">
         <v>10</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="122" t="s">
         <v>217</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="123" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="122" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="115">
+      <c r="A6" s="109">
         <v>5</v>
       </c>
-      <c r="B6" s="120">
+      <c r="B6" s="113">
         <v>15</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="122">
         <v>5</v>
       </c>
-      <c r="D6" s="114">
+      <c r="D6" s="124">
         <f>AVERAGE(A4:A8)</f>
         <v>20</v>
       </c>
-      <c r="E6" s="116">
+      <c r="E6" s="125">
         <f>D6-$D$3</f>
         <v>-14.600000000000001</v>
       </c>
-      <c r="F6" s="117"/>
+      <c r="F6" s="110"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="115">
+      <c r="A7" s="109">
         <v>17</v>
       </c>
-      <c r="B7" s="120">
+      <c r="B7" s="113">
         <v>17</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="123">
         <v>10</v>
       </c>
-      <c r="D7" s="114">
+      <c r="D7" s="124">
         <f>AVERAGE(A4:A13)</f>
         <v>28.8</v>
       </c>
-      <c r="E7" s="116">
+      <c r="E7" s="125">
         <f>D7-$D$3</f>
         <v>-5.8000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="115">
+      <c r="A8" s="109">
         <v>33</v>
       </c>
-      <c r="B8" s="120">
+      <c r="B8" s="113">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="115">
+      <c r="A9" s="109">
         <v>20</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="113">
         <v>20</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="122" t="s">
         <v>217</v>
       </c>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="123" t="s">
         <v>233</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="122" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="115">
+      <c r="A10" s="109">
         <v>41</v>
       </c>
-      <c r="B10" s="120">
+      <c r="B10" s="113">
         <v>20</v>
       </c>
-      <c r="C10" s="78" t="s">
-        <v>242</v>
-      </c>
-      <c r="D10" s="114">
+      <c r="C10" s="122" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" s="124">
         <f>AVERAGE(B4:B8)</f>
         <v>13.4</v>
       </c>
-      <c r="E10" s="116">
+      <c r="E10" s="125">
         <f>D10-$D$3</f>
         <v>-21.200000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="115">
+      <c r="A11" s="109">
         <v>53</v>
       </c>
-      <c r="B11" s="120">
+      <c r="B11" s="113">
         <v>24</v>
       </c>
-      <c r="C11" s="77" t="s">
-        <v>243</v>
-      </c>
-      <c r="D11" s="114">
+      <c r="C11" s="123" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="124">
         <f>AVERAGE(B19:B23)</f>
         <v>58.8</v>
       </c>
-      <c r="E11" s="116">
+      <c r="E11" s="125">
         <f>D11-$D$3</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="115">
+      <c r="A12" s="109">
         <v>50</v>
       </c>
-      <c r="B12" s="120">
+      <c r="B12" s="113">
         <v>25</v>
       </c>
-      <c r="D12" s="83" t="s">
-        <v>241</v>
-      </c>
-      <c r="E12" s="95">
+      <c r="D12" s="126" t="s">
+        <v>239</v>
+      </c>
+      <c r="E12" s="127">
         <f>MAX(ABS(E10), ABS(E11))</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="115">
+      <c r="A13" s="109">
         <v>24</v>
       </c>
-      <c r="B13" s="120">
+      <c r="B13" s="113">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="115">
+      <c r="A14" s="109">
         <v>41</v>
       </c>
-      <c r="B14" s="120">
+      <c r="B14" s="113">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="115">
+      <c r="A15" s="109">
         <v>52</v>
       </c>
-      <c r="B15" s="120">
+      <c r="B15" s="113">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="115">
+      <c r="A16" s="109">
         <v>47</v>
       </c>
-      <c r="B16" s="120">
+      <c r="B16" s="113">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="115">
+      <c r="A17" s="109">
         <v>15</v>
       </c>
-      <c r="B17" s="120">
+      <c r="B17" s="113">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="115">
+      <c r="A18" s="109">
         <v>44</v>
       </c>
-      <c r="B18" s="120">
+      <c r="B18" s="113">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="118">
+      <c r="A19" s="111">
         <v>10</v>
       </c>
-      <c r="B19" s="120">
+      <c r="B19" s="113">
         <v>50</v>
       </c>
     </row>
@@ -18270,7 +18300,7 @@
       <c r="A20" s="76">
         <v>36</v>
       </c>
-      <c r="B20" s="120">
+      <c r="B20" s="113">
         <v>52</v>
       </c>
     </row>
@@ -18278,7 +18308,7 @@
       <c r="A21" s="76">
         <v>60</v>
       </c>
-      <c r="B21" s="120">
+      <c r="B21" s="113">
         <v>53</v>
       </c>
     </row>
@@ -18286,7 +18316,7 @@
       <c r="A22" s="76">
         <v>20</v>
       </c>
-      <c r="B22" s="120">
+      <c r="B22" s="113">
         <v>60</v>
       </c>
     </row>
@@ -18294,32 +18324,32 @@
       <c r="A23" s="76">
         <v>79</v>
       </c>
-      <c r="B23" s="120">
+      <c r="B23" s="113">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="120"/>
+      <c r="B24" s="113"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="120"/>
+      <c r="B25" s="113"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="120"/>
+      <c r="B26" s="113"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="120"/>
+      <c r="B27" s="113"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="124" t="s">
-        <v>244</v>
-      </c>
-      <c r="B28" s="124"/>
-      <c r="C28" s="124"/>
-      <c r="D28" s="124"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
+      <c r="A28" s="116" t="s">
+        <v>242</v>
+      </c>
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="116"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D29" s="76"/>
@@ -18332,7 +18362,7 @@
         <v>74</v>
       </c>
       <c r="B30" s="84">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="D30" s="76"/>
       <c r="G30" s="82"/>
@@ -18352,29 +18382,27 @@
         <v>170</v>
       </c>
       <c r="B32" s="84">
-        <v>25</v>
+        <v>5.6</v>
       </c>
       <c r="D32" s="76"/>
       <c r="G32" s="82"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="83" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="B33" s="84">
-        <v>0.5</v>
+        <v>14.3</v>
       </c>
       <c r="D33" s="76"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="92"/>
       <c r="G33" s="82"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="83" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B34" s="84">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D34" s="76"/>
       <c r="E34" s="80"/>
@@ -18383,22 +18411,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="83" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B35" s="84">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="79"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="82"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="83" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B36" s="84">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D36" s="76"/>
       <c r="E36" s="76"/>
@@ -18407,266 +18435,281 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="83" t="s">
-        <v>228</v>
-      </c>
-      <c r="B37" s="108">
-        <v>0.8</v>
+        <v>223</v>
+      </c>
+      <c r="B37" s="84">
+        <v>100</v>
       </c>
       <c r="D37" s="76"/>
-      <c r="E37" s="111"/>
+      <c r="E37" s="76"/>
       <c r="F37" s="79"/>
       <c r="G37" s="82"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="79"/>
-      <c r="B38" s="79"/>
-      <c r="C38" s="79"/>
+      <c r="A38" s="83" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="106">
+        <v>0.8</v>
+      </c>
       <c r="D38" s="76"/>
-      <c r="E38" s="79"/>
+      <c r="E38" s="107"/>
       <c r="F38" s="79"/>
       <c r="G38" s="82"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="83" t="s">
+      <c r="A39" s="79"/>
+      <c r="B39" s="79"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="82"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="126" t="s">
         <v>224</v>
       </c>
-      <c r="B39" s="87">
-        <f>B32/SQRT(B35)</f>
-        <v>2.7950849718747368</v>
-      </c>
-      <c r="G39" s="113" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="83" t="s">
+      <c r="B40" s="138">
+        <f>B32/SQRT(B36)</f>
+        <v>1.252198067399882</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="126" t="s">
         <v>226</v>
       </c>
-      <c r="B40" s="87">
-        <f>SQRT(B33*(1-B33)/B35)</f>
-        <v>5.5901699437494741E-2</v>
-      </c>
-      <c r="G40" s="82"/>
-    </row>
-    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="112" t="s">
+      <c r="B41" s="138">
+        <f>SQRT(B34*(1-B34)/B36)</f>
+        <v>0.11180339887498948</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="139" t="s">
         <v>227</v>
       </c>
-      <c r="B41" s="89" t="e">
-        <f>B40 *  SQRT((B36-B35)/(B36-1))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G41" s="82"/>
-    </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="112" t="s">
+      <c r="B42" s="140">
+        <f>B41 *  SQRT((B37-B36)/(B37-1))</f>
+        <v>0.1005037815259212</v>
+      </c>
+      <c r="G42" s="82"/>
+    </row>
+    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="139" t="s">
         <v>230</v>
       </c>
-      <c r="B42" s="89">
-        <f>(B31-B30)/(B32/SQRT(B35))</f>
-        <v>-35.419316763596676</v>
-      </c>
-      <c r="G42" s="82"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="83" t="s">
+      <c r="B43" s="140">
+        <f>(B31-B30)/(B32/SQRT(B36))</f>
+        <v>-9.5831484749991009</v>
+      </c>
+      <c r="G43" s="82"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="126" t="s">
         <v>220</v>
       </c>
-      <c r="B43" s="109">
-        <f>(1-B37)/2</f>
+      <c r="B44" s="141">
+        <f>(1-B38)/2</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="G43" s="82"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="83" t="s">
+      <c r="G44" s="82"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="126" t="s">
         <v>221</v>
       </c>
-      <c r="B44" s="110">
-        <f>B37+B43</f>
+      <c r="B45" s="142">
+        <f>B38+B44</f>
         <v>0.9</v>
       </c>
-      <c r="G44" s="82"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G45" s="82"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G46" s="82"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="77" t="s">
-        <v>187</v>
-      </c>
-      <c r="B47" s="77" t="s">
+      <c r="G47" s="82"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="123"/>
+      <c r="B48" s="123" t="s">
         <v>182</v>
       </c>
-      <c r="C47" s="77" t="s">
+      <c r="C48" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="D47" s="77" t="s">
+      <c r="D48" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="E47" s="77" t="s">
+      <c r="E48" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="F47" s="119"/>
-      <c r="G47" s="79"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="83" t="s">
+      <c r="F48" s="112"/>
+      <c r="G48" s="79"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="126" t="s">
         <v>184</v>
       </c>
-      <c r="B48" s="88">
+      <c r="B49" s="128">
         <v>1</v>
       </c>
-      <c r="C48" s="93">
-        <f>_xlfn.NORM.DIST(B48, $B$30, $B$39,FALSE)</f>
-        <v>5.4603584600867164E-274</v>
-      </c>
-      <c r="D48" s="93">
-        <f>_xlfn.NORM.DIST(B48, $B$33, $B$40, FALSE)</f>
-        <v>3.0318365123303672E-17</v>
-      </c>
-      <c r="E48" s="93" t="e">
-        <f>_xlfn.NORM.DIST(B48/$B$35, $B$33, $B$41,FALSE)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="84" t="s">
+      <c r="C49" s="129">
+        <f>_xlfn.NORM.DIST(B49, $B$30, $B$40,FALSE)</f>
+        <v>3.6403528427324646E-21</v>
+      </c>
+      <c r="D49" s="129">
+        <f>_xlfn.NORM.DIST(B49, $B$34, $B$41, FALSE)</f>
+        <v>1.6199821912178208E-4</v>
+      </c>
+      <c r="E49" s="129">
+        <f>_xlfn.NORM.DIST(B49/$B$36, $B$34, $B$42,FALSE)</f>
+        <v>1.7598204095915145E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="B49" s="88">
+      <c r="B50" s="128">
         <v>1</v>
       </c>
-      <c r="C49" s="93">
-        <f>_xlfn.NORM.DIST(B49, $B$30, $B$39,TRUE)</f>
-        <v>4.3055684240681732E-275</v>
-      </c>
-      <c r="D49" s="93">
-        <f>_xlfn.NORM.DIST(B49, $B$33, $B$40, TRUE)</f>
+      <c r="C50" s="129">
+        <f>_xlfn.NORM.DIST(B50, $B$30, $B$40,TRUE)</f>
+        <v>4.7065385071790097E-22</v>
+      </c>
+      <c r="D50" s="129">
+        <f>_xlfn.NORM.DIST(B50, $B$34, $B$41, TRUE)</f>
+        <v>0.99999612789178449</v>
+      </c>
+      <c r="E50" s="129">
+        <f>_xlfn.NORM.DIST(B50/$B$36, $B$34, $B$42,TRUE)</f>
+        <v>3.7771111457593937E-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="126" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="128">
         <v>1</v>
       </c>
-      <c r="E49" s="93" t="e">
-        <f>_xlfn.NORM.DIST(B49/$B$35, $B$33, $B$41,TRUE)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="B50" s="88">
+      <c r="C51" s="129">
+        <f>(1-_xlfn.NORM.DIST(B51, $B$30, $B$40,TRUE))</f>
         <v>1</v>
       </c>
-      <c r="C50" s="93">
-        <f>(1-_xlfn.NORM.DIST(B50, $B$30, $B$39,TRUE))</f>
+      <c r="D51" s="129">
+        <f>1 - _xlfn.NORM.DIST(B51, $B$34, $B$41, TRUE)</f>
+        <v>3.8721082155079856E-6</v>
+      </c>
+      <c r="E51" s="129">
+        <f>1 - _xlfn.NORM.DIST(B51/$B$36, $B$34, $B$42,TRUE)</f>
+        <v>0.99999622288885426</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="131" t="s">
+        <v>201</v>
+      </c>
+      <c r="B52" s="128">
         <v>1</v>
       </c>
-      <c r="D50" s="93">
-        <f>1 - _xlfn.NORM.DIST(B50, $B$33, $B$40, TRUE)</f>
+      <c r="C52" s="132">
+        <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E50" s="93" t="e">
-        <f>1 - _xlfn.NORM.DIST(B50/$B$35, $B$33, $B$41,TRUE)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="125" t="s">
-        <v>201</v>
-      </c>
-      <c r="B51" s="88">
+      <c r="D52" s="133">
+        <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="132">
+        <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="134"/>
+      <c r="B53" s="135">
         <v>1</v>
       </c>
-      <c r="C51" s="127">
-        <f>_xlfn.NORM.DIST(B52, $B$30, $B$39,TRUE) - _xlfn.NORM.DIST(B51, $B$30, $B$39,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="D51" s="129">
-        <f>_xlfn.NORM.DIST(B52, $B$33, $B$40, TRUE) - _xlfn.NORM.DIST(B51, $B$33, $B$40, TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="127" t="e">
-        <f>_xlfn.NORM.DIST(B52/$B$35, $B$33, $B$41,TRUE) - _xlfn.NORM.DIST(B51/$B$35, $B$33, $B$41,TRUE)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="126"/>
-      <c r="B52" s="107">
-        <v>1</v>
-      </c>
-      <c r="C52" s="128"/>
-      <c r="D52" s="130"/>
-      <c r="E52" s="128"/>
-      <c r="G52" s="79"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C53" s="136"/>
+      <c r="D53" s="137"/>
+      <c r="E53" s="136"/>
       <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="78"/>
-      <c r="B54" s="77" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="102" t="s">
-        <v>234</v>
-      </c>
       <c r="G54" s="79"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="83" t="s">
+      <c r="A55" s="122"/>
+      <c r="B55" s="123" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="123" t="s">
+        <v>244</v>
+      </c>
+      <c r="D55" s="143" t="s">
+        <v>222</v>
+      </c>
+      <c r="G55" s="79"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="126" t="s">
         <v>218</v>
       </c>
-      <c r="B55" s="93">
-        <f>_xlfn.NORM.INV(B43, $B$30, $B$39)</f>
-        <v>96.417954478463741</v>
-      </c>
-      <c r="C55" s="89">
-        <f>_xlfn.NORM.INV(B43, B33, B40)</f>
-        <v>0.42835908956927493</v>
-      </c>
-      <c r="G55" s="79"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="83" t="s">
+      <c r="B56" s="129">
+        <f>_xlfn.NORM.INV(B44, $B$30, $B$40)</f>
+        <v>11.395243606351759</v>
+      </c>
+      <c r="C56" s="138">
+        <f>B30-C58</f>
+        <v>8.7544865406300012</v>
+      </c>
+      <c r="D56" s="140">
+        <f>_xlfn.NORM.INV(B44, B34, B41)</f>
+        <v>0.35671817913854981</v>
+      </c>
+      <c r="G56" s="79"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="126" t="s">
         <v>219</v>
       </c>
-      <c r="B56" s="93">
-        <f>_xlfn.NORM.INV(B44, $B$30, $B$39)</f>
-        <v>103.58204552153626</v>
-      </c>
-      <c r="C56" s="87">
-        <f>_xlfn.NORM.INV(B44, B33, B40)</f>
-        <v>0.57164091043072507</v>
-      </c>
-      <c r="G56" s="79"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="85" t="s">
+      <c r="B57" s="129">
+        <f>_xlfn.NORM.INV(B45, $B$30, $B$40)</f>
+        <v>14.604756393648241</v>
+      </c>
+      <c r="C57" s="138">
+        <f>B30+C58</f>
+        <v>17.245513459369999</v>
+      </c>
+      <c r="D57" s="138">
+        <f>_xlfn.NORM.INV(B45, B34, B41)</f>
+        <v>0.64328182086145014</v>
+      </c>
+      <c r="G57" s="79"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="144" t="s">
         <v>229</v>
       </c>
-      <c r="B57" s="93">
-        <f>_xlfn.CONFIDENCE.NORM(1-B37, B32, B35)</f>
-        <v>3.582045521536255</v>
-      </c>
-      <c r="C57" s="87">
-        <f>_xlfn.CONFIDENCE.NORM(1-B37, B34, B35)</f>
-        <v>0.14328182086145019</v>
-      </c>
-      <c r="G57" s="79"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C58" s="100"/>
-      <c r="D58" s="76"/>
+      <c r="B58" s="129">
+        <f>_xlfn.CONFIDENCE.NORM(1-B38, B32, B36)</f>
+        <v>1.6047563936482421</v>
+      </c>
+      <c r="C58" s="138">
+        <f>_xlfn.CONFIDENCE.T(1-B38, B33, B36)</f>
+        <v>4.2455134593699979</v>
+      </c>
+      <c r="D58" s="138">
+        <f>_xlfn.CONFIDENCE.NORM(1-B38, B35, B36)</f>
+        <v>0.28656364172290039</v>
+      </c>
       <c r="G58" s="79"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C59" s="100"/>
       <c r="D59" s="76"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="79"/>
       <c r="G59" s="79"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -18674,6 +18717,12 @@
       <c r="E60" s="76"/>
       <c r="F60" s="79"/>
       <c r="G60" s="79"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="79"/>
+      <c r="G61" s="79"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B23">
@@ -18682,10 +18731,10 @@
   <mergeCells count="6">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D52:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added formulas of hyphotesis tests
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3A615C-B0CD-334E-95CB-093EC9309C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B25611-117E-0F42-B5EB-7089E14A1841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Probability Introduction" sheetId="4" r:id="rId3"/>
     <sheet name="Probability Distributions" sheetId="6" r:id="rId4"/>
     <sheet name="Sampling &amp; Confidence Intervals" sheetId="8" r:id="rId5"/>
+    <sheet name="Hypothesis Tests" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="262">
   <si>
     <t>E</t>
   </si>
@@ -833,6 +834,57 @@
   </si>
   <si>
     <t>population</t>
+  </si>
+  <si>
+    <t>Hypothesis Test Single Population</t>
+  </si>
+  <si>
+    <t>Hypothesis Test Comparing Two Population</t>
+  </si>
+  <si>
+    <t>probability left test</t>
+  </si>
+  <si>
+    <t>probability right test</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t># tail test</t>
+  </si>
+  <si>
+    <t>hypothesis</t>
+  </si>
+  <si>
+    <t>test statistic</t>
+  </si>
+  <si>
+    <t>statistic z-test</t>
+  </si>
+  <si>
+    <t>sample std deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> std deviation</t>
+  </si>
+  <si>
+    <t>Z Distribution</t>
+  </si>
+  <si>
+    <t>T Distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statistic test </t>
+  </si>
+  <si>
+    <t>statistics t-test</t>
+  </si>
+  <si>
+    <t>critical score (one tail)</t>
+  </si>
+  <si>
+    <t>critical score (two tail)</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1125,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1249,12 +1301,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1263,9 +1309,7 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1283,12 +1327,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1308,26 +1346,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1349,25 +1367,6 @@
     <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1384,6 +1383,85 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -12671,21 +12749,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="114">
+      <c r="C17" s="124">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="115"/>
+      <c r="D17" s="125"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="114">
+      <c r="C18" s="124">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="115"/>
+      <c r="D18" s="125"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -16753,7 +16831,7 @@
   <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16765,15 +16843,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="126" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
@@ -16782,13 +16860,13 @@
       <c r="B3" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="108" t="s">
         <v>168</v>
       </c>
       <c r="F3" s="79"/>
@@ -16802,15 +16880,15 @@
       <c r="B4" s="78">
         <v>75</v>
       </c>
-      <c r="C4" s="88">
+      <c r="C4" s="114">
         <f>B4/$B$9</f>
         <v>0.75</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="137">
         <f>A4*C4</f>
         <v>0.75</v>
       </c>
-      <c r="E4" s="90">
+      <c r="E4" s="137">
         <f>((A4-$D$9)^2)*C4</f>
         <v>3.2448000000000006</v>
       </c>
@@ -16825,15 +16903,15 @@
       <c r="B5" s="78">
         <v>13</v>
       </c>
-      <c r="C5" s="88">
+      <c r="C5" s="114">
         <f t="shared" ref="C5:C8" si="0">B5/$B$9</f>
         <v>0.13</v>
       </c>
-      <c r="D5" s="90">
+      <c r="D5" s="137">
         <f t="shared" ref="D5:D8" si="1">A5*C5</f>
         <v>0.26</v>
       </c>
-      <c r="E5" s="90">
+      <c r="E5" s="137">
         <f t="shared" ref="E5:E8" si="2">((A5-$D$9)^2)*C5</f>
         <v>0.15163200000000002</v>
       </c>
@@ -16848,15 +16926,15 @@
       <c r="B6" s="78">
         <v>18</v>
       </c>
-      <c r="C6" s="88">
+      <c r="C6" s="114">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="137">
         <f t="shared" si="1"/>
         <v>0.54</v>
       </c>
-      <c r="E6" s="90">
+      <c r="E6" s="137">
         <f t="shared" si="2"/>
         <v>1.152000000000002E-3</v>
       </c>
@@ -16871,15 +16949,15 @@
       <c r="B7" s="78">
         <v>17</v>
       </c>
-      <c r="C7" s="88">
+      <c r="C7" s="114">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="D7" s="90">
+      <c r="D7" s="137">
         <f t="shared" si="1"/>
         <v>0.68</v>
       </c>
-      <c r="E7" s="90">
+      <c r="E7" s="137">
         <f t="shared" si="2"/>
         <v>0.14388799999999999</v>
       </c>
@@ -16894,15 +16972,15 @@
       <c r="B8" s="78">
         <v>17</v>
       </c>
-      <c r="C8" s="88">
+      <c r="C8" s="114">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="D8" s="90">
+      <c r="D8" s="137">
         <f t="shared" si="1"/>
         <v>0.85000000000000009</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="137">
         <f t="shared" si="2"/>
         <v>0.62668800000000002</v>
       </c>
@@ -16914,15 +16992,15 @@
       <c r="B9" s="85">
         <v>100</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="123">
         <f t="shared" ref="C9" si="3">SUM(C4:C8)</f>
         <v>1.4</v>
       </c>
-      <c r="D9" s="90">
+      <c r="D9" s="137">
         <f>SUM(D4:D8)</f>
         <v>3.08</v>
       </c>
-      <c r="E9" s="90">
+      <c r="E9" s="137">
         <f>SQRT(SUM(E4:E8))</f>
         <v>2.0416072100186167</v>
       </c>
@@ -16931,58 +17009,58 @@
       <c r="H9" s="79"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
       <c r="F10" s="79"/>
       <c r="G10" s="82"/>
       <c r="H10" s="79"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
       <c r="F11" s="79"/>
       <c r="G11" s="82"/>
       <c r="H11" s="79"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
       <c r="F12" s="79"/>
       <c r="G12" s="82"/>
       <c r="H12" s="79"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
       <c r="F13" s="79"/>
       <c r="G13" s="82"/>
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="126" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="121"/>
-      <c r="C14" s="121"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="121"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="121"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
       <c r="F15" s="79"/>
       <c r="G15" s="82"/>
       <c r="H15" s="79"/>
@@ -16994,9 +17072,9 @@
       <c r="B16" s="83">
         <v>20</v>
       </c>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
       <c r="F16" s="79"/>
       <c r="G16" s="82"/>
       <c r="H16" s="79"/>
@@ -17005,12 +17083,12 @@
       <c r="A17" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="B17" s="99">
+      <c r="B17" s="95">
         <v>42</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="79"/>
       <c r="G17" s="82"/>
       <c r="H17" s="79"/>
@@ -17019,13 +17097,13 @@
       <c r="A18" s="83" t="s">
         <v>202</v>
       </c>
-      <c r="B18" s="90">
+      <c r="B18" s="88">
         <f>1/(B17-B16)</f>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
       <c r="F18" s="79"/>
       <c r="G18" s="82"/>
       <c r="H18" s="79"/>
@@ -17038,9 +17116,9 @@
         <f>(B17+B16)/2</f>
         <v>31</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
       <c r="F19" s="79"/>
       <c r="G19" s="82"/>
       <c r="H19" s="79"/>
@@ -17053,60 +17131,60 @@
         <f>(B17-B16)/SQRT(12)</f>
         <v>6.3508529610858835</v>
       </c>
-      <c r="C20" s="97"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
       <c r="F20" s="79"/>
       <c r="G20" s="82"/>
       <c r="H20" s="79"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="97"/>
-      <c r="C21" s="101" t="s">
+      <c r="B21" s="93"/>
+      <c r="C21" s="97" t="s">
         <v>205</v>
       </c>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
       <c r="F21" s="79"/>
       <c r="G21" s="82"/>
       <c r="H21" s="79"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="109" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="98"/>
-      <c r="E22" s="81" t="s">
+      <c r="D22" s="94"/>
+      <c r="E22" s="136" t="s">
         <v>200</v>
       </c>
-      <c r="F22" s="81" t="s">
+      <c r="F22" s="136" t="s">
         <v>203</v>
       </c>
       <c r="G22" s="82"/>
       <c r="H22" s="79"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="83">
+      <c r="B23" s="143">
         <v>24</v>
       </c>
-      <c r="C23" s="93">
+      <c r="C23" s="115">
         <f>$B$18*0</f>
         <v>0</v>
       </c>
-      <c r="D23" s="98"/>
-      <c r="E23" s="81">
+      <c r="D23" s="94"/>
+      <c r="E23" s="136">
         <v>70</v>
       </c>
-      <c r="F23" s="95">
+      <c r="F23" s="113">
         <f>((E23/100)/B18) + B16</f>
         <v>35.4</v>
       </c>
@@ -17114,13 +17192,13 @@
       <c r="H23" s="79"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="84" t="s">
+      <c r="A24" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B24" s="83">
+      <c r="B24" s="143">
         <v>31</v>
       </c>
-      <c r="C24" s="93">
+      <c r="C24" s="115">
         <f>$B$18*(B24-B16)</f>
         <v>0.5</v>
       </c>
@@ -17129,13 +17207,13 @@
       <c r="H24" s="79"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="83" t="s">
+      <c r="A25" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="83">
+      <c r="B25" s="143">
         <v>28</v>
       </c>
-      <c r="C25" s="93">
+      <c r="C25" s="115">
         <f>$B$18*($B$17-B25)</f>
         <v>0.63636363636363635</v>
       </c>
@@ -17144,13 +17222,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="117" t="s">
+      <c r="A26" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="83">
+      <c r="B26" s="143">
         <v>29</v>
       </c>
-      <c r="C26" s="119">
+      <c r="C26" s="130">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17159,11 +17237,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="118"/>
-      <c r="B27" s="81">
+      <c r="A27" s="129"/>
+      <c r="B27" s="142">
         <v>37</v>
       </c>
-      <c r="C27" s="120"/>
+      <c r="C27" s="131"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17179,15 +17257,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="127" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
+      <c r="B30" s="127"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="127"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17239,39 +17317,39 @@
       <c r="H35" s="79"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="77" t="s">
+      <c r="A36" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="77" t="s">
+      <c r="B36" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="77" t="s">
+      <c r="C36" s="109" t="s">
         <v>189</v>
       </c>
-      <c r="E36" s="81" t="s">
+      <c r="E36" s="136" t="s">
         <v>200</v>
       </c>
-      <c r="F36" s="81" t="s">
+      <c r="F36" s="136" t="s">
         <v>204</v>
       </c>
       <c r="G36" s="82"/>
       <c r="H36" s="79"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="83" t="s">
+      <c r="A37" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B37" s="83">
+      <c r="B37" s="143">
         <v>170</v>
       </c>
-      <c r="C37" s="93">
+      <c r="C37" s="115">
         <f>_xlfn.NORM.DIST(B37,$B$32,$B$33,FALSE)</f>
         <v>1.849993181041472E-27</v>
       </c>
-      <c r="E37" s="81">
+      <c r="E37" s="136">
         <v>35</v>
       </c>
-      <c r="F37" s="95">
+      <c r="F37" s="113">
         <f>_xlfn.NORM.INV(E37/100, B32, B33)</f>
         <v>673.11929714602923</v>
       </c>
@@ -17279,20 +17357,20 @@
       <c r="H37" s="79"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="84" t="s">
+      <c r="A38" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="83">
+      <c r="B38" s="143">
         <v>170</v>
       </c>
-      <c r="C38" s="93">
+      <c r="C38" s="115">
         <f>_xlfn.NORM.DIST(B38,$B$32,$B$33,TRUE)</f>
         <v>8.4361799794053529E-27</v>
       </c>
-      <c r="E38" s="85" t="s">
+      <c r="E38" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="F38" s="95">
+      <c r="F38" s="113">
         <f>B32 - (B34 * B33)</f>
         <v>643</v>
       </c>
@@ -17300,21 +17378,21 @@
       <c r="H38" s="79"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="83" t="s">
+      <c r="A39" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B39" s="83">
+      <c r="B39" s="143">
         <v>2300</v>
       </c>
-      <c r="C39" s="93">
+      <c r="C39" s="115">
         <f>(1-_xlfn.NORM.DIST(B39,$B$32,$B$33,TRUE))</f>
         <v>0</v>
       </c>
-      <c r="D39" s="94"/>
-      <c r="E39" s="89" t="s">
+      <c r="D39" s="91"/>
+      <c r="E39" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="F39" s="95">
+      <c r="F39" s="113">
         <f>B32 + (B34 * B33)</f>
         <v>741</v>
       </c>
@@ -17322,42 +17400,42 @@
       <c r="H39" s="79"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="117" t="s">
+      <c r="A40" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="B40" s="83">
+      <c r="B40" s="143">
         <v>3300</v>
       </c>
-      <c r="C40" s="119">
+      <c r="C40" s="130">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="94"/>
+      <c r="F40" s="91"/>
       <c r="G40" s="82"/>
       <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="118"/>
-      <c r="B41" s="81">
+      <c r="A41" s="129"/>
+      <c r="B41" s="142">
         <v>4200</v>
       </c>
-      <c r="C41" s="120"/>
+      <c r="C41" s="131"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
       <c r="H41" s="79"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="97"/>
+      <c r="A42" s="93"/>
       <c r="B42" s="79"/>
-      <c r="C42" s="100"/>
+      <c r="C42" s="96"/>
       <c r="F42" s="79"/>
       <c r="G42" s="79"/>
       <c r="H42" s="79"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="97"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="79"/>
-      <c r="C43" s="100"/>
+      <c r="C43" s="96"/>
       <c r="F43" s="79"/>
       <c r="G43" s="79"/>
       <c r="H43" s="79"/>
@@ -17368,15 +17446,15 @@
       <c r="H44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="116" t="s">
+      <c r="A46" s="127" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="116"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="116"/>
-      <c r="E46" s="116"/>
-      <c r="F46" s="116"/>
-      <c r="G46" s="116"/>
+      <c r="B46" s="127"/>
+      <c r="C46" s="127"/>
+      <c r="D46" s="127"/>
+      <c r="E46" s="127"/>
+      <c r="F46" s="127"/>
+      <c r="G46" s="127"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="83" t="s">
@@ -17422,96 +17500,96 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="77" t="s">
+      <c r="A54" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B54" s="77" t="s">
+      <c r="B54" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="C54" s="77" t="s">
+      <c r="C54" s="109" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="83" t="s">
+      <c r="A55" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="83">
+      <c r="B55" s="143">
         <v>6</v>
       </c>
-      <c r="C55" s="93">
+      <c r="C55" s="115">
         <f>_xlfn.BINOM.DIST(B55,$B$48,$B$49,FALSE)</f>
         <v>0.25728216171875024</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="84" t="s">
+      <c r="A56" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B56" s="83">
+      <c r="B56" s="143">
         <v>2</v>
       </c>
-      <c r="C56" s="93">
+      <c r="C56" s="115">
         <f>_xlfn.BINOM.DIST(B56,$B$48,$B$49,TRUE)</f>
         <v>6.0273437500000207E-6</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="83" t="s">
+      <c r="A57" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B57" s="83">
+      <c r="B57" s="143">
         <v>6</v>
       </c>
-      <c r="C57" s="93">
+      <c r="C57" s="115">
         <f>1 - _xlfn.BINOM.DIST(B57,$B$48,$B$49,TRUE)</f>
         <v>0.69833729609374973</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="117" t="s">
+      <c r="A58" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="B58" s="83">
+      <c r="B58" s="143">
         <v>2</v>
       </c>
-      <c r="C58" s="119">
+      <c r="C58" s="130">
         <f>_xlfn.BINOM.DIST(B59,$B$48,$B$49,TRUE) - _xlfn.BINOM.DIST(B58,$B$48,$B$49,TRUE)</f>
         <v>0.30165667656250023</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="118"/>
-      <c r="B59" s="81">
+      <c r="A59" s="129"/>
+      <c r="B59" s="142">
         <v>6</v>
       </c>
-      <c r="C59" s="120"/>
+      <c r="C59" s="131"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="97"/>
-      <c r="B60" s="79"/>
-      <c r="C60" s="100"/>
+      <c r="A60" s="144"/>
+      <c r="B60" s="145"/>
+      <c r="C60" s="146"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="97"/>
+      <c r="A61" s="93"/>
       <c r="B61" s="79"/>
-      <c r="C61" s="100"/>
+      <c r="C61" s="96"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="80"/>
       <c r="B62" s="80"/>
-      <c r="C62" s="94"/>
+      <c r="C62" s="91"/>
     </row>
     <row r="64" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A64" s="116" t="s">
+      <c r="A64" s="127" t="s">
         <v>198</v>
       </c>
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="116"/>
-      <c r="E64" s="116"/>
-      <c r="F64" s="116"/>
-      <c r="G64" s="116"/>
+      <c r="B64" s="127"/>
+      <c r="C64" s="127"/>
+      <c r="D64" s="127"/>
+      <c r="E64" s="127"/>
+      <c r="F64" s="127"/>
+      <c r="G64" s="127"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="83" t="s">
@@ -17531,105 +17609,105 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="77" t="s">
+      <c r="A69" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B69" s="77" t="s">
+      <c r="B69" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="C69" s="77" t="s">
+      <c r="C69" s="109" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="83" t="s">
+      <c r="A70" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B70" s="83">
+      <c r="B70" s="143">
         <v>5</v>
       </c>
-      <c r="C70" s="93">
+      <c r="C70" s="115">
         <f>_xlfn.POISSON.DIST(B70,$B$66,FALSE)</f>
         <v>2.6939453267530375E-3</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="84" t="s">
+      <c r="A71" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B71" s="83">
+      <c r="B71" s="143">
         <v>3</v>
       </c>
-      <c r="C71" s="93">
+      <c r="C71" s="115">
         <f>_xlfn.POISSON.DIST(B71,$B$66,TRUE)</f>
         <v>3.1709808559658942E-4</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="83" t="s">
+      <c r="A72" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B72" s="83">
+      <c r="B72" s="143">
         <v>6</v>
       </c>
-      <c r="C72" s="93">
+      <c r="C72" s="115">
         <f>(1 - _xlfn.POISSON.DIST(B72,$B$66,TRUE))</f>
         <v>0.9895496420502663</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="117" t="s">
+      <c r="A73" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="B73" s="83">
+      <c r="B73" s="143">
         <v>2</v>
       </c>
-      <c r="C73" s="119">
+      <c r="C73" s="130">
         <f>_xlfn.POISSON.DIST(B74,$B$66,TRUE) - _xlfn.POISSON.DIST(B73,$B$66,TRUE)</f>
         <v>3.8791531399499785E-3</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="118"/>
-      <c r="B74" s="81">
+      <c r="A74" s="129"/>
+      <c r="B74" s="142">
         <v>5</v>
       </c>
-      <c r="C74" s="120"/>
+      <c r="C74" s="131"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="97"/>
+      <c r="A75" s="93"/>
       <c r="B75" s="79"/>
-      <c r="C75" s="100"/>
+      <c r="C75" s="96"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="97"/>
+      <c r="A76" s="93"/>
       <c r="B76" s="79"/>
-      <c r="C76" s="100"/>
+      <c r="C76" s="96"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="80"/>
       <c r="B77" s="80"/>
-      <c r="C77" s="94"/>
+      <c r="C77" s="91"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="80"/>
       <c r="B78" s="80"/>
-      <c r="C78" s="94"/>
+      <c r="C78" s="91"/>
     </row>
     <row r="79" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A79" s="116" t="s">
+      <c r="A79" s="127" t="s">
         <v>199</v>
       </c>
-      <c r="B79" s="116"/>
-      <c r="C79" s="116"/>
-      <c r="D79" s="116"/>
-      <c r="E79" s="116"/>
-      <c r="F79" s="116"/>
-      <c r="G79" s="116"/>
+      <c r="B79" s="127"/>
+      <c r="C79" s="127"/>
+      <c r="D79" s="127"/>
+      <c r="E79" s="127"/>
+      <c r="F79" s="127"/>
+      <c r="G79" s="127"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B80" s="80"/>
-      <c r="C80" s="94"/>
+      <c r="C80" s="91"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="83" t="s">
@@ -17639,113 +17717,113 @@
         <f>6/5</f>
         <v>1.2</v>
       </c>
-      <c r="C81" s="94"/>
+      <c r="C81" s="91"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B82" s="80"/>
-      <c r="C82" s="94"/>
+      <c r="C82" s="91"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="77" t="s">
+      <c r="A83" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B83" s="77" t="s">
+      <c r="B83" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="C83" s="77" t="s">
+      <c r="C83" s="109" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="83" t="s">
+      <c r="A84" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B84" s="84">
+      <c r="B84" s="141">
         <v>1</v>
       </c>
-      <c r="C84" s="93">
+      <c r="C84" s="115">
         <f>_xlfn.EXPON.DIST(B84,$B$81,FALSE)</f>
         <v>0.36143305429464256</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="84" t="s">
+      <c r="A85" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B85" s="84">
+      <c r="B85" s="141">
         <f>2.2/6</f>
         <v>0.3666666666666667</v>
       </c>
-      <c r="C85" s="93">
+      <c r="C85" s="115">
         <f>_xlfn.EXPON.DIST(B85,$B$81,TRUE)</f>
         <v>0.35596357891685859</v>
       </c>
-      <c r="E85" s="96"/>
+      <c r="E85" s="92"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="83" t="s">
+      <c r="A86" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B86" s="84">
+      <c r="B86" s="141">
         <f>2.7/6</f>
         <v>0.45</v>
       </c>
-      <c r="C86" s="93">
+      <c r="C86" s="115">
         <f>1 - _xlfn.EXPON.DIST(B86,$B$81,TRUE)</f>
         <v>0.58274825237398964</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="117" t="s">
+      <c r="A87" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="B87" s="84">
+      <c r="B87" s="141">
         <f>2.1/6</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="C87" s="119">
+      <c r="C87" s="130">
         <f>_xlfn.EXPON.DIST(B88,$B$81,TRUE) - _xlfn.EXPON.DIST(B87,$B$81,TRUE)</f>
         <v>0.25047716007445753</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="118"/>
-      <c r="B88" s="81">
+      <c r="A88" s="129"/>
+      <c r="B88" s="142">
         <f>4.5/6</f>
         <v>0.75</v>
       </c>
-      <c r="C88" s="120"/>
+      <c r="C88" s="131"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="97"/>
+      <c r="A89" s="93"/>
       <c r="B89" s="79"/>
-      <c r="C89" s="100"/>
+      <c r="C89" s="96"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="97"/>
+      <c r="A90" s="93"/>
       <c r="B90" s="79"/>
-      <c r="C90" s="100"/>
+      <c r="C90" s="96"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="97"/>
+      <c r="A91" s="93"/>
       <c r="B91" s="79"/>
-      <c r="C91" s="100"/>
+      <c r="C91" s="96"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="80"/>
       <c r="B92" s="80"/>
-      <c r="C92" s="94"/>
+      <c r="C92" s="91"/>
     </row>
     <row r="93" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A93" s="116" t="s">
+      <c r="A93" s="127" t="s">
         <v>181</v>
       </c>
-      <c r="B93" s="116"/>
-      <c r="C93" s="116"/>
-      <c r="D93" s="116"/>
-      <c r="E93" s="116"/>
-      <c r="F93" s="116"/>
-      <c r="G93" s="116"/>
+      <c r="B93" s="127"/>
+      <c r="C93" s="127"/>
+      <c r="D93" s="127"/>
+      <c r="E93" s="127"/>
+      <c r="F93" s="127"/>
+      <c r="G93" s="127"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D94" s="75"/>
@@ -17762,8 +17840,8 @@
       </c>
       <c r="B96" s="79"/>
       <c r="C96" s="79"/>
-      <c r="D96" s="91"/>
-      <c r="E96" s="91"/>
+      <c r="D96" s="89"/>
+      <c r="E96" s="89"/>
       <c r="F96" s="79"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -17772,15 +17850,15 @@
       </c>
       <c r="B97" s="79"/>
       <c r="C97" s="79"/>
-      <c r="D97" s="91"/>
-      <c r="E97" s="91"/>
+      <c r="D97" s="89"/>
+      <c r="E97" s="89"/>
       <c r="F97" s="79"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B98" s="79"/>
       <c r="C98" s="79"/>
-      <c r="D98" s="91"/>
-      <c r="E98" s="91"/>
+      <c r="D98" s="89"/>
+      <c r="E98" s="89"/>
       <c r="F98" s="79"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -17790,13 +17868,13 @@
       <c r="B99" s="78" t="s">
         <v>176</v>
       </c>
-      <c r="C99" s="78" t="s">
+      <c r="C99" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="D99" s="78" t="s">
+      <c r="D99" s="108" t="s">
         <v>181</v>
       </c>
-      <c r="E99" s="91"/>
+      <c r="E99" s="89"/>
       <c r="F99" s="79"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -17806,10 +17884,10 @@
       <c r="B100" s="81">
         <v>7000</v>
       </c>
-      <c r="C100" s="95">
+      <c r="C100" s="113">
         <v>0.3</v>
       </c>
-      <c r="D100" s="78">
+      <c r="D100" s="108">
         <f>B100*C100</f>
         <v>2100</v>
       </c>
@@ -17821,14 +17899,14 @@
       <c r="B101" s="81">
         <v>19000</v>
       </c>
-      <c r="C101" s="95">
+      <c r="C101" s="113">
         <v>0.45</v>
       </c>
-      <c r="D101" s="78">
+      <c r="D101" s="108">
         <f t="shared" ref="D101:D102" si="4">B101*C101</f>
         <v>8550</v>
       </c>
-      <c r="E101" s="91"/>
+      <c r="E101" s="89"/>
       <c r="F101" s="79"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -17838,33 +17916,33 @@
       <c r="B102" s="81">
         <v>37000</v>
       </c>
-      <c r="C102" s="95">
+      <c r="C102" s="113">
         <v>0.25</v>
       </c>
-      <c r="D102" s="78">
+      <c r="D102" s="108">
         <f t="shared" si="4"/>
         <v>9250</v>
       </c>
-      <c r="E102" s="91"/>
+      <c r="E102" s="89"/>
       <c r="F102" s="79"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="79"/>
       <c r="B103" s="79"/>
       <c r="C103" s="79"/>
-      <c r="D103" s="78">
+      <c r="D103" s="108">
         <f>SUM(D100:D102)</f>
         <v>19900</v>
       </c>
-      <c r="E103" s="91"/>
+      <c r="E103" s="89"/>
       <c r="F103" s="79"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="79"/>
       <c r="B104" s="79"/>
       <c r="C104" s="79"/>
-      <c r="D104" s="91"/>
-      <c r="E104" s="91"/>
+      <c r="D104" s="89"/>
+      <c r="E104" s="89"/>
       <c r="F104" s="79"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -17901,7 +17979,7 @@
       <c r="G107" s="79"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="105"/>
+      <c r="A108" s="99"/>
       <c r="B108" s="79"/>
       <c r="C108" s="79"/>
       <c r="D108" s="79"/>
@@ -17913,7 +17991,7 @@
       <c r="A109" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="B109" s="102">
+      <c r="B109" s="98">
         <v>4</v>
       </c>
       <c r="C109" s="79"/>
@@ -17926,7 +18004,7 @@
       <c r="A110" s="83" t="s">
         <v>211</v>
       </c>
-      <c r="B110" s="102">
+      <c r="B110" s="98">
         <v>7</v>
       </c>
       <c r="C110" s="79"/>
@@ -17952,7 +18030,7 @@
       <c r="A112" s="83" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="102">
+      <c r="B112" s="98">
         <f>B111*B109</f>
         <v>300</v>
       </c>
@@ -17969,10 +18047,10 @@
       <c r="B114" s="78" t="s">
         <v>177</v>
       </c>
-      <c r="C114" s="78" t="s">
+      <c r="C114" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="D114" s="78" t="s">
+      <c r="D114" s="108" t="s">
         <v>181</v>
       </c>
     </row>
@@ -17983,10 +18061,10 @@
       <c r="B115" s="81">
         <v>25</v>
       </c>
-      <c r="C115" s="95">
+      <c r="C115" s="113">
         <v>0.35</v>
       </c>
-      <c r="D115" s="103">
+      <c r="D115" s="138">
         <f>C115*($B$110*MIN($B$111, B115) - $B$112)</f>
         <v>-43.75</v>
       </c>
@@ -17998,10 +18076,10 @@
       <c r="B116" s="81">
         <v>50</v>
       </c>
-      <c r="C116" s="95">
+      <c r="C116" s="113">
         <v>0.2</v>
       </c>
-      <c r="D116" s="103">
+      <c r="D116" s="138">
         <f t="shared" ref="D116:D117" si="5">C116*($B$110*MIN($B$111, B116) - $B$112)</f>
         <v>10</v>
       </c>
@@ -18013,10 +18091,10 @@
       <c r="B117" s="81">
         <v>75</v>
       </c>
-      <c r="C117" s="95">
+      <c r="C117" s="113">
         <v>0.45</v>
       </c>
-      <c r="D117" s="103">
+      <c r="D117" s="138">
         <f t="shared" si="5"/>
         <v>101.25</v>
       </c>
@@ -18025,20 +18103,13 @@
       <c r="A118" s="79"/>
       <c r="B118" s="79"/>
       <c r="C118" s="79"/>
-      <c r="D118" s="104">
+      <c r="D118" s="139">
         <f>SUM(D115:D117)</f>
         <v>67.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
     <mergeCell ref="A93:G93"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
@@ -18049,6 +18120,13 @@
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="C87:C88"/>
     <mergeCell ref="A79:G79"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18059,8 +18137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E279595A-CDC1-E441-A6DF-F172F4F13CC6}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18071,228 +18149,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="127" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="107" t="s">
         <v>238</v>
       </c>
       <c r="C3" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="108">
+      <c r="D3" s="102">
         <f>AVERAGE(A4:A23)</f>
         <v>34.6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="109">
+      <c r="A4" s="103">
         <v>25</v>
       </c>
-      <c r="B4" s="113" cm="1">
+      <c r="B4" s="107" cm="1">
         <f t="array" ref="B4:B23">_xlfn._xlws.SORT(A4:A23)</f>
         <v>5</v>
       </c>
-      <c r="C4" s="113"/>
+      <c r="C4" s="107"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="109">
+      <c r="A5" s="103">
         <v>20</v>
       </c>
-      <c r="B5" s="113">
+      <c r="B5" s="107">
         <v>10</v>
       </c>
-      <c r="C5" s="122" t="s">
+      <c r="C5" s="108" t="s">
         <v>217</v>
       </c>
-      <c r="D5" s="123" t="s">
+      <c r="D5" s="109" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="122" t="s">
+      <c r="E5" s="108" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="109">
+      <c r="A6" s="103">
         <v>5</v>
       </c>
-      <c r="B6" s="113">
+      <c r="B6" s="107">
         <v>15</v>
       </c>
-      <c r="C6" s="122">
+      <c r="C6" s="108">
         <v>5</v>
       </c>
-      <c r="D6" s="124">
+      <c r="D6" s="110">
         <f>AVERAGE(A4:A8)</f>
         <v>20</v>
       </c>
-      <c r="E6" s="125">
+      <c r="E6" s="111">
         <f>D6-$D$3</f>
         <v>-14.600000000000001</v>
       </c>
-      <c r="F6" s="110"/>
+      <c r="F6" s="104"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="109">
+      <c r="A7" s="103">
         <v>17</v>
       </c>
-      <c r="B7" s="113">
+      <c r="B7" s="107">
         <v>17</v>
       </c>
-      <c r="C7" s="123">
+      <c r="C7" s="109">
         <v>10</v>
       </c>
-      <c r="D7" s="124">
+      <c r="D7" s="110">
         <f>AVERAGE(A4:A13)</f>
         <v>28.8</v>
       </c>
-      <c r="E7" s="125">
+      <c r="E7" s="111">
         <f>D7-$D$3</f>
         <v>-5.8000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="109">
+      <c r="A8" s="103">
         <v>33</v>
       </c>
-      <c r="B8" s="113">
+      <c r="B8" s="107">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="109">
+      <c r="A9" s="103">
         <v>20</v>
       </c>
-      <c r="B9" s="113">
+      <c r="B9" s="107">
         <v>20</v>
       </c>
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="108" t="s">
         <v>217</v>
       </c>
-      <c r="D9" s="123" t="s">
+      <c r="D9" s="109" t="s">
         <v>233</v>
       </c>
-      <c r="E9" s="122" t="s">
+      <c r="E9" s="108" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="109">
+      <c r="A10" s="103">
         <v>41</v>
       </c>
-      <c r="B10" s="113">
+      <c r="B10" s="107">
         <v>20</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="108" t="s">
         <v>240</v>
       </c>
-      <c r="D10" s="124">
+      <c r="D10" s="110">
         <f>AVERAGE(B4:B8)</f>
         <v>13.4</v>
       </c>
-      <c r="E10" s="125">
+      <c r="E10" s="111">
         <f>D10-$D$3</f>
         <v>-21.200000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="109">
+      <c r="A11" s="103">
         <v>53</v>
       </c>
-      <c r="B11" s="113">
+      <c r="B11" s="107">
         <v>24</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="109" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="124">
+      <c r="D11" s="110">
         <f>AVERAGE(B19:B23)</f>
         <v>58.8</v>
       </c>
-      <c r="E11" s="125">
+      <c r="E11" s="111">
         <f>D11-$D$3</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="109">
+      <c r="A12" s="103">
         <v>50</v>
       </c>
-      <c r="B12" s="113">
+      <c r="B12" s="107">
         <v>25</v>
       </c>
-      <c r="D12" s="126" t="s">
+      <c r="D12" s="112" t="s">
         <v>239</v>
       </c>
-      <c r="E12" s="127">
+      <c r="E12" s="113">
         <f>MAX(ABS(E10), ABS(E11))</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="109">
+      <c r="A13" s="103">
         <v>24</v>
       </c>
-      <c r="B13" s="113">
+      <c r="B13" s="107">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="109">
+      <c r="A14" s="103">
         <v>41</v>
       </c>
-      <c r="B14" s="113">
+      <c r="B14" s="107">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="109">
+      <c r="A15" s="103">
         <v>52</v>
       </c>
-      <c r="B15" s="113">
+      <c r="B15" s="107">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="109">
+      <c r="A16" s="103">
         <v>47</v>
       </c>
-      <c r="B16" s="113">
+      <c r="B16" s="107">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="109">
+      <c r="A17" s="103">
         <v>15</v>
       </c>
-      <c r="B17" s="113">
+      <c r="B17" s="107">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="109">
+      <c r="A18" s="103">
         <v>44</v>
       </c>
-      <c r="B18" s="113">
+      <c r="B18" s="107">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="111">
+      <c r="A19" s="105">
         <v>10</v>
       </c>
-      <c r="B19" s="113">
+      <c r="B19" s="107">
         <v>50</v>
       </c>
     </row>
@@ -18300,7 +18378,7 @@
       <c r="A20" s="76">
         <v>36</v>
       </c>
-      <c r="B20" s="113">
+      <c r="B20" s="107">
         <v>52</v>
       </c>
     </row>
@@ -18308,7 +18386,7 @@
       <c r="A21" s="76">
         <v>60</v>
       </c>
-      <c r="B21" s="113">
+      <c r="B21" s="107">
         <v>53</v>
       </c>
     </row>
@@ -18316,7 +18394,7 @@
       <c r="A22" s="76">
         <v>20</v>
       </c>
-      <c r="B22" s="113">
+      <c r="B22" s="107">
         <v>60</v>
       </c>
     </row>
@@ -18324,32 +18402,32 @@
       <c r="A23" s="76">
         <v>79</v>
       </c>
-      <c r="B23" s="113">
+      <c r="B23" s="107">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="113"/>
+      <c r="B24" s="107"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="113"/>
+      <c r="B25" s="107"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="113"/>
+      <c r="B26" s="107"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="113"/>
+      <c r="B27" s="107"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="127" t="s">
         <v>242</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="116"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="116"/>
+      <c r="B28" s="127"/>
+      <c r="C28" s="127"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D29" s="76"/>
@@ -18406,7 +18484,7 @@
       </c>
       <c r="D34" s="76"/>
       <c r="E34" s="80"/>
-      <c r="F34" s="92"/>
+      <c r="F34" s="90"/>
       <c r="G34" s="82"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -18418,7 +18496,7 @@
       </c>
       <c r="D35" s="76"/>
       <c r="E35" s="80"/>
-      <c r="F35" s="92"/>
+      <c r="F35" s="90"/>
       <c r="G35" s="82"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -18449,11 +18527,11 @@
       <c r="A38" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="B38" s="106">
+      <c r="B38" s="100">
         <v>0.8</v>
       </c>
       <c r="D38" s="76"/>
-      <c r="E38" s="107"/>
+      <c r="E38" s="101"/>
       <c r="F38" s="79"/>
       <c r="G38" s="82"/>
     </row>
@@ -18467,58 +18545,58 @@
       <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="126" t="s">
+      <c r="A40" s="112" t="s">
         <v>224</v>
       </c>
-      <c r="B40" s="138">
+      <c r="B40" s="117">
         <f>B32/SQRT(B36)</f>
         <v>1.252198067399882</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="126" t="s">
+      <c r="A41" s="112" t="s">
         <v>226</v>
       </c>
-      <c r="B41" s="138">
+      <c r="B41" s="117">
         <f>SQRT(B34*(1-B34)/B36)</f>
         <v>0.11180339887498948</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="139" t="s">
+      <c r="A42" s="118" t="s">
         <v>227</v>
       </c>
-      <c r="B42" s="140">
+      <c r="B42" s="119">
         <f>B41 *  SQRT((B37-B36)/(B37-1))</f>
         <v>0.1005037815259212</v>
       </c>
       <c r="G42" s="82"/>
     </row>
     <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="139" t="s">
+      <c r="A43" s="118" t="s">
         <v>230</v>
       </c>
-      <c r="B43" s="140">
+      <c r="B43" s="119">
         <f>(B31-B30)/(B32/SQRT(B36))</f>
         <v>-9.5831484749991009</v>
       </c>
       <c r="G43" s="82"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="126" t="s">
+      <c r="A44" s="112" t="s">
         <v>220</v>
       </c>
-      <c r="B44" s="141">
+      <c r="B44" s="120">
         <f>(1-B38)/2</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="G44" s="82"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="126" t="s">
+      <c r="A45" s="112" t="s">
         <v>221</v>
       </c>
-      <c r="B45" s="142">
+      <c r="B45" s="121">
         <f>B38+B44</f>
         <v>0.9</v>
       </c>
@@ -18531,184 +18609,184 @@
       <c r="G47" s="82"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="123"/>
-      <c r="B48" s="123" t="s">
+      <c r="A48" s="109"/>
+      <c r="B48" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="C48" s="123" t="s">
+      <c r="C48" s="109" t="s">
         <v>231</v>
       </c>
-      <c r="D48" s="123" t="s">
+      <c r="D48" s="109" t="s">
         <v>225</v>
       </c>
-      <c r="E48" s="123" t="s">
+      <c r="E48" s="109" t="s">
         <v>232</v>
       </c>
-      <c r="F48" s="112"/>
+      <c r="F48" s="106"/>
       <c r="G48" s="79"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="126" t="s">
+      <c r="A49" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B49" s="128">
+      <c r="B49" s="147">
         <v>1</v>
       </c>
-      <c r="C49" s="129">
+      <c r="C49" s="115">
         <f>_xlfn.NORM.DIST(B49, $B$30, $B$40,FALSE)</f>
         <v>3.6403528427324646E-21</v>
       </c>
-      <c r="D49" s="129">
+      <c r="D49" s="115">
         <f>_xlfn.NORM.DIST(B49, $B$34, $B$41, FALSE)</f>
         <v>1.6199821912178208E-4</v>
       </c>
-      <c r="E49" s="129">
+      <c r="E49" s="115">
         <f>_xlfn.NORM.DIST(B49/$B$36, $B$34, $B$42,FALSE)</f>
         <v>1.7598204095915145E-4</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="130" t="s">
+      <c r="A50" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="128">
+      <c r="B50" s="147">
         <v>1</v>
       </c>
-      <c r="C50" s="129">
+      <c r="C50" s="115">
         <f>_xlfn.NORM.DIST(B50, $B$30, $B$40,TRUE)</f>
         <v>4.7065385071790097E-22</v>
       </c>
-      <c r="D50" s="129">
+      <c r="D50" s="115">
         <f>_xlfn.NORM.DIST(B50, $B$34, $B$41, TRUE)</f>
         <v>0.99999612789178449</v>
       </c>
-      <c r="E50" s="129">
+      <c r="E50" s="115">
         <f>_xlfn.NORM.DIST(B50/$B$36, $B$34, $B$42,TRUE)</f>
         <v>3.7771111457593937E-6</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="126" t="s">
+      <c r="A51" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B51" s="128">
+      <c r="B51" s="147">
         <v>1</v>
       </c>
-      <c r="C51" s="129">
+      <c r="C51" s="115">
         <f>(1-_xlfn.NORM.DIST(B51, $B$30, $B$40,TRUE))</f>
         <v>1</v>
       </c>
-      <c r="D51" s="129">
+      <c r="D51" s="115">
         <f>1 - _xlfn.NORM.DIST(B51, $B$34, $B$41, TRUE)</f>
         <v>3.8721082155079856E-6</v>
       </c>
-      <c r="E51" s="129">
+      <c r="E51" s="115">
         <f>1 - _xlfn.NORM.DIST(B51/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0.99999622288885426</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="131" t="s">
+      <c r="A52" s="128" t="s">
         <v>201</v>
       </c>
-      <c r="B52" s="128">
+      <c r="B52" s="147">
         <v>1</v>
       </c>
-      <c r="C52" s="132">
+      <c r="C52" s="130">
         <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="133">
+      <c r="D52" s="132">
         <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="132">
+      <c r="E52" s="130">
         <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="134"/>
-      <c r="B53" s="135">
+      <c r="A53" s="129"/>
+      <c r="B53" s="148">
         <v>1</v>
       </c>
-      <c r="C53" s="136"/>
-      <c r="D53" s="137"/>
-      <c r="E53" s="136"/>
+      <c r="C53" s="131"/>
+      <c r="D53" s="133"/>
+      <c r="E53" s="131"/>
       <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G54" s="79"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="122"/>
-      <c r="B55" s="123" t="s">
+      <c r="A55" s="108"/>
+      <c r="B55" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="123" t="s">
+      <c r="C55" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="D55" s="143" t="s">
+      <c r="D55" s="122" t="s">
         <v>222</v>
       </c>
       <c r="G55" s="79"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="126" t="s">
+      <c r="A56" s="112" t="s">
         <v>218</v>
       </c>
-      <c r="B56" s="129">
+      <c r="B56" s="115">
         <f>_xlfn.NORM.INV(B44, $B$30, $B$40)</f>
         <v>11.395243606351759</v>
       </c>
-      <c r="C56" s="138">
+      <c r="C56" s="117">
         <f>B30-C58</f>
         <v>8.7544865406300012</v>
       </c>
-      <c r="D56" s="140">
+      <c r="D56" s="119">
         <f>_xlfn.NORM.INV(B44, B34, B41)</f>
         <v>0.35671817913854981</v>
       </c>
       <c r="G56" s="79"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="126" t="s">
+      <c r="A57" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="B57" s="129">
+      <c r="B57" s="115">
         <f>_xlfn.NORM.INV(B45, $B$30, $B$40)</f>
         <v>14.604756393648241</v>
       </c>
-      <c r="C57" s="138">
+      <c r="C57" s="117">
         <f>B30+C58</f>
         <v>17.245513459369999</v>
       </c>
-      <c r="D57" s="138">
+      <c r="D57" s="117">
         <f>_xlfn.NORM.INV(B45, B34, B41)</f>
         <v>0.64328182086145014</v>
       </c>
       <c r="G57" s="79"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="144" t="s">
+      <c r="A58" s="123" t="s">
         <v>229</v>
       </c>
-      <c r="B58" s="129">
+      <c r="B58" s="115">
         <f>_xlfn.CONFIDENCE.NORM(1-B38, B32, B36)</f>
         <v>1.6047563936482421</v>
       </c>
-      <c r="C58" s="138">
+      <c r="C58" s="117">
         <f>_xlfn.CONFIDENCE.T(1-B38, B33, B36)</f>
         <v>4.2455134593699979</v>
       </c>
-      <c r="D58" s="138">
+      <c r="D58" s="117">
         <f>_xlfn.CONFIDENCE.NORM(1-B38, B35, B36)</f>
         <v>0.28656364172290039</v>
       </c>
       <c r="G58" s="79"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C59" s="100"/>
+      <c r="C59" s="96"/>
       <c r="D59" s="76"/>
       <c r="G59" s="79"/>
     </row>
@@ -18739,4 +18817,324 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="7" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A1" s="127" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="76"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="134" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="84">
+        <v>75</v>
+      </c>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="134" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="135">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="134" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" s="135">
+        <v>14.4</v>
+      </c>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="134" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="135">
+        <v>14.4</v>
+      </c>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="134" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="84">
+        <v>30</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="134" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8" s="84">
+        <v>1</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="134" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="134" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" s="84">
+        <v>2.1038836780136476</v>
+      </c>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="134" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="84">
+        <v>-2.5103950552320091</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="27"/>
+      <c r="B13" s="152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="108" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" s="79"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="123" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" s="130">
+        <f>_xlfn.NORM.S.INV(1-B9)</f>
+        <v>1.2815515655446006</v>
+      </c>
+      <c r="C14" s="115">
+        <f>_xlfn.T.INV(1-B9, B7)</f>
+        <v>1.3104150253913947</v>
+      </c>
+      <c r="D14" s="79"/>
+      <c r="F14" s="75"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="131"/>
+      <c r="C15" s="115">
+        <f>_xlfn.T.INV((B9/B8), B7)</f>
+        <v>-1.3104150253913947</v>
+      </c>
+      <c r="D15" s="151">
+        <f>_xlfn.T.INV(1-(B9/B8),B7)</f>
+        <v>1.3104150253913947</v>
+      </c>
+      <c r="F15" s="75"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="149" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="153">
+        <f>(B4-B3)/(B5/SQRT(B7))</f>
+        <v>-2.5103950552320091</v>
+      </c>
+      <c r="C16" s="154"/>
+      <c r="D16" s="79"/>
+      <c r="F16" s="75"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="150" t="s">
+        <v>247</v>
+      </c>
+      <c r="B17" s="115">
+        <f>_xlfn.NORM.S.DIST(B10, TRUE)</f>
+        <v>0.98230570245217108</v>
+      </c>
+      <c r="C17" s="115">
+        <f>_xlfn.T.DIST(B11, B7, TRUE)</f>
+        <v>8.8413521905273355E-3</v>
+      </c>
+      <c r="D17" s="79"/>
+      <c r="F17" s="75"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="150" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" s="115">
+        <f>1-B17</f>
+        <v>1.7694297547828919E-2</v>
+      </c>
+      <c r="C18" s="115">
+        <f>1-C17</f>
+        <v>0.99115864780947271</v>
+      </c>
+      <c r="D18" s="79"/>
+      <c r="F18" s="75"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" s="115">
+        <f>B8 * IF(B10&gt;0, B18, B17)</f>
+        <v>1.7694297547828919E-2</v>
+      </c>
+      <c r="C19" s="115">
+        <f>B8 * IF(B11&gt;0, C18, C17)</f>
+        <v>8.8413521905273355E-3</v>
+      </c>
+      <c r="D19" s="79"/>
+      <c r="F19" s="75"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="149" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="117" t="str">
+        <f>IF(B19&lt;B9, "Reject", "Do not reject")</f>
+        <v>Reject</v>
+      </c>
+      <c r="C20" s="117" t="str">
+        <f>IF(C19&lt;C9, "Reject", "Do not reject")</f>
+        <v>Do not reject</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="F20" s="75"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="75"/>
+      <c r="F21" s="75"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="76"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="76"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="76"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+    </row>
+    <row r="25" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A25" s="127" t="s">
+        <v>246</v>
+      </c>
+      <c r="B25" s="126"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="126"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:C16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added formulas to calculate hypothesis on proportion values
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B25611-117E-0F42-B5EB-7089E14A1841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464DB1F-5C88-2848-94A2-4813BD293F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="267">
   <si>
     <t>E</t>
   </si>
@@ -875,9 +875,6 @@
     <t>T Distribution</t>
   </si>
   <si>
-    <t xml:space="preserve">statistic test </t>
-  </si>
-  <si>
     <t>statistics t-test</t>
   </si>
   <si>
@@ -885,19 +882,38 @@
   </si>
   <si>
     <t>critical score (two tail)</t>
+  </si>
+  <si>
+    <t>statistic test  proportion</t>
+  </si>
+  <si>
+    <t>sample proportion</t>
+  </si>
+  <si>
+    <t>statistic test mean</t>
+  </si>
+  <si>
+    <t>p-value proportion</t>
+  </si>
+  <si>
+    <t>Type error 2</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1002,7 +1018,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1027,8 +1043,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1119,13 +1140,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1384,6 +1502,60 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1410,58 +1582,32 @@
     <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -12749,21 +12895,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="124">
+      <c r="C17" s="144">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="125"/>
+      <c r="D17" s="145"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="124">
+      <c r="C18" s="144">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="125"/>
+      <c r="D18" s="145"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -16843,15 +16989,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="146" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
@@ -16884,11 +17030,11 @@
         <f>B4/$B$9</f>
         <v>0.75</v>
       </c>
-      <c r="D4" s="137">
+      <c r="D4" s="125">
         <f>A4*C4</f>
         <v>0.75</v>
       </c>
-      <c r="E4" s="137">
+      <c r="E4" s="125">
         <f>((A4-$D$9)^2)*C4</f>
         <v>3.2448000000000006</v>
       </c>
@@ -16907,11 +17053,11 @@
         <f t="shared" ref="C5:C8" si="0">B5/$B$9</f>
         <v>0.13</v>
       </c>
-      <c r="D5" s="137">
+      <c r="D5" s="125">
         <f t="shared" ref="D5:D8" si="1">A5*C5</f>
         <v>0.26</v>
       </c>
-      <c r="E5" s="137">
+      <c r="E5" s="125">
         <f t="shared" ref="E5:E8" si="2">((A5-$D$9)^2)*C5</f>
         <v>0.15163200000000002</v>
       </c>
@@ -16930,11 +17076,11 @@
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="D6" s="137">
+      <c r="D6" s="125">
         <f t="shared" si="1"/>
         <v>0.54</v>
       </c>
-      <c r="E6" s="137">
+      <c r="E6" s="125">
         <f t="shared" si="2"/>
         <v>1.152000000000002E-3</v>
       </c>
@@ -16953,11 +17099,11 @@
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="D7" s="137">
+      <c r="D7" s="125">
         <f t="shared" si="1"/>
         <v>0.68</v>
       </c>
-      <c r="E7" s="137">
+      <c r="E7" s="125">
         <f t="shared" si="2"/>
         <v>0.14388799999999999</v>
       </c>
@@ -16976,11 +17122,11 @@
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="D8" s="137">
+      <c r="D8" s="125">
         <f t="shared" si="1"/>
         <v>0.85000000000000009</v>
       </c>
-      <c r="E8" s="137">
+      <c r="E8" s="125">
         <f t="shared" si="2"/>
         <v>0.62668800000000002</v>
       </c>
@@ -16996,11 +17142,11 @@
         <f t="shared" ref="C9" si="3">SUM(C4:C8)</f>
         <v>1.4</v>
       </c>
-      <c r="D9" s="137">
+      <c r="D9" s="125">
         <f>SUM(D4:D8)</f>
         <v>3.08</v>
       </c>
-      <c r="E9" s="137">
+      <c r="E9" s="125">
         <f>SQRT(SUM(E4:E8))</f>
         <v>2.0416072100186167</v>
       </c>
@@ -17045,15 +17191,15 @@
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="146" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="126"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="146"/>
+      <c r="F14" s="146"/>
+      <c r="G14" s="146"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -17153,17 +17299,17 @@
       <c r="A22" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="140" t="s">
+      <c r="B22" s="77" t="s">
         <v>182</v>
       </c>
       <c r="C22" s="109" t="s">
         <v>189</v>
       </c>
       <c r="D22" s="94"/>
-      <c r="E22" s="136" t="s">
+      <c r="E22" s="124" t="s">
         <v>200</v>
       </c>
-      <c r="F22" s="136" t="s">
+      <c r="F22" s="124" t="s">
         <v>203</v>
       </c>
       <c r="G22" s="82"/>
@@ -17173,7 +17319,7 @@
       <c r="A23" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="143">
+      <c r="B23" s="83">
         <v>24</v>
       </c>
       <c r="C23" s="115">
@@ -17181,7 +17327,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="94"/>
-      <c r="E23" s="136">
+      <c r="E23" s="124">
         <v>70</v>
       </c>
       <c r="F23" s="113">
@@ -17195,7 +17341,7 @@
       <c r="A24" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B24" s="143">
+      <c r="B24" s="83">
         <v>31</v>
       </c>
       <c r="C24" s="115">
@@ -17210,7 +17356,7 @@
       <c r="A25" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="143">
+      <c r="B25" s="83">
         <v>28</v>
       </c>
       <c r="C25" s="115">
@@ -17222,13 +17368,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="128" t="s">
+      <c r="A26" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="143">
+      <c r="B26" s="83">
         <v>29</v>
       </c>
-      <c r="C26" s="130">
+      <c r="C26" s="150">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17237,11 +17383,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="129"/>
-      <c r="B27" s="142">
+      <c r="A27" s="149"/>
+      <c r="B27" s="81">
         <v>37</v>
       </c>
-      <c r="C27" s="131"/>
+      <c r="C27" s="151"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17257,15 +17403,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="127" t="s">
+      <c r="A30" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="127"/>
-      <c r="C30" s="127"/>
-      <c r="D30" s="127"/>
-      <c r="E30" s="127"/>
-      <c r="F30" s="127"/>
-      <c r="G30" s="127"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="147"/>
+      <c r="E30" s="147"/>
+      <c r="F30" s="147"/>
+      <c r="G30" s="147"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17320,16 +17466,16 @@
       <c r="A36" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="140" t="s">
+      <c r="B36" s="77" t="s">
         <v>182</v>
       </c>
       <c r="C36" s="109" t="s">
         <v>189</v>
       </c>
-      <c r="E36" s="136" t="s">
+      <c r="E36" s="124" t="s">
         <v>200</v>
       </c>
-      <c r="F36" s="136" t="s">
+      <c r="F36" s="124" t="s">
         <v>204</v>
       </c>
       <c r="G36" s="82"/>
@@ -17339,14 +17485,14 @@
       <c r="A37" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B37" s="143">
+      <c r="B37" s="83">
         <v>170</v>
       </c>
       <c r="C37" s="115">
         <f>_xlfn.NORM.DIST(B37,$B$32,$B$33,FALSE)</f>
         <v>1.849993181041472E-27</v>
       </c>
-      <c r="E37" s="136">
+      <c r="E37" s="124">
         <v>35</v>
       </c>
       <c r="F37" s="113">
@@ -17360,7 +17506,7 @@
       <c r="A38" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="143">
+      <c r="B38" s="83">
         <v>170</v>
       </c>
       <c r="C38" s="115">
@@ -17381,7 +17527,7 @@
       <c r="A39" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B39" s="143">
+      <c r="B39" s="83">
         <v>2300</v>
       </c>
       <c r="C39" s="115">
@@ -17400,13 +17546,13 @@
       <c r="H39" s="79"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="128" t="s">
+      <c r="A40" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="B40" s="143">
+      <c r="B40" s="83">
         <v>3300</v>
       </c>
-      <c r="C40" s="130">
+      <c r="C40" s="150">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
         <v>0</v>
       </c>
@@ -17415,11 +17561,11 @@
       <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="129"/>
-      <c r="B41" s="142">
+      <c r="A41" s="149"/>
+      <c r="B41" s="81">
         <v>4200</v>
       </c>
-      <c r="C41" s="131"/>
+      <c r="C41" s="151"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
       <c r="H41" s="79"/>
@@ -17446,15 +17592,15 @@
       <c r="H44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="127" t="s">
+      <c r="A46" s="147" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="127"/>
-      <c r="C46" s="127"/>
-      <c r="D46" s="127"/>
-      <c r="E46" s="127"/>
-      <c r="F46" s="127"/>
-      <c r="G46" s="127"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="147"/>
+      <c r="D46" s="147"/>
+      <c r="E46" s="147"/>
+      <c r="F46" s="147"/>
+      <c r="G46" s="147"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="83" t="s">
@@ -17503,7 +17649,7 @@
       <c r="A54" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B54" s="140" t="s">
+      <c r="B54" s="77" t="s">
         <v>182</v>
       </c>
       <c r="C54" s="109" t="s">
@@ -17514,7 +17660,7 @@
       <c r="A55" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="143">
+      <c r="B55" s="83">
         <v>6</v>
       </c>
       <c r="C55" s="115">
@@ -17526,7 +17672,7 @@
       <c r="A56" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B56" s="143">
+      <c r="B56" s="83">
         <v>2</v>
       </c>
       <c r="C56" s="115">
@@ -17538,7 +17684,7 @@
       <c r="A57" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B57" s="143">
+      <c r="B57" s="83">
         <v>6</v>
       </c>
       <c r="C57" s="115">
@@ -17547,28 +17693,28 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="128" t="s">
+      <c r="A58" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="B58" s="143">
+      <c r="B58" s="83">
         <v>2</v>
       </c>
-      <c r="C58" s="130">
+      <c r="C58" s="150">
         <f>_xlfn.BINOM.DIST(B59,$B$48,$B$49,TRUE) - _xlfn.BINOM.DIST(B58,$B$48,$B$49,TRUE)</f>
         <v>0.30165667656250023</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="129"/>
-      <c r="B59" s="142">
+      <c r="A59" s="149"/>
+      <c r="B59" s="81">
         <v>6</v>
       </c>
-      <c r="C59" s="131"/>
+      <c r="C59" s="151"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="144"/>
-      <c r="B60" s="145"/>
-      <c r="C60" s="146"/>
+      <c r="A60" s="93"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="96"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="93"/>
@@ -17581,15 +17727,15 @@
       <c r="C62" s="91"/>
     </row>
     <row r="64" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A64" s="127" t="s">
+      <c r="A64" s="147" t="s">
         <v>198</v>
       </c>
-      <c r="B64" s="127"/>
-      <c r="C64" s="127"/>
-      <c r="D64" s="127"/>
-      <c r="E64" s="127"/>
-      <c r="F64" s="127"/>
-      <c r="G64" s="127"/>
+      <c r="B64" s="147"/>
+      <c r="C64" s="147"/>
+      <c r="D64" s="147"/>
+      <c r="E64" s="147"/>
+      <c r="F64" s="147"/>
+      <c r="G64" s="147"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="83" t="s">
@@ -17612,7 +17758,7 @@
       <c r="A69" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B69" s="140" t="s">
+      <c r="B69" s="77" t="s">
         <v>182</v>
       </c>
       <c r="C69" s="109" t="s">
@@ -17623,7 +17769,7 @@
       <c r="A70" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B70" s="143">
+      <c r="B70" s="83">
         <v>5</v>
       </c>
       <c r="C70" s="115">
@@ -17635,7 +17781,7 @@
       <c r="A71" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B71" s="143">
+      <c r="B71" s="83">
         <v>3</v>
       </c>
       <c r="C71" s="115">
@@ -17647,7 +17793,7 @@
       <c r="A72" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B72" s="143">
+      <c r="B72" s="83">
         <v>6</v>
       </c>
       <c r="C72" s="115">
@@ -17656,23 +17802,23 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="128" t="s">
+      <c r="A73" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="B73" s="143">
+      <c r="B73" s="83">
         <v>2</v>
       </c>
-      <c r="C73" s="130">
+      <c r="C73" s="150">
         <f>_xlfn.POISSON.DIST(B74,$B$66,TRUE) - _xlfn.POISSON.DIST(B73,$B$66,TRUE)</f>
         <v>3.8791531399499785E-3</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="129"/>
-      <c r="B74" s="142">
+      <c r="A74" s="149"/>
+      <c r="B74" s="81">
         <v>5</v>
       </c>
-      <c r="C74" s="131"/>
+      <c r="C74" s="151"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="93"/>
@@ -17695,15 +17841,15 @@
       <c r="C78" s="91"/>
     </row>
     <row r="79" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A79" s="127" t="s">
+      <c r="A79" s="147" t="s">
         <v>199</v>
       </c>
-      <c r="B79" s="127"/>
-      <c r="C79" s="127"/>
-      <c r="D79" s="127"/>
-      <c r="E79" s="127"/>
-      <c r="F79" s="127"/>
-      <c r="G79" s="127"/>
+      <c r="B79" s="147"/>
+      <c r="C79" s="147"/>
+      <c r="D79" s="147"/>
+      <c r="E79" s="147"/>
+      <c r="F79" s="147"/>
+      <c r="G79" s="147"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B80" s="80"/>
@@ -17727,7 +17873,7 @@
       <c r="A83" s="109" t="s">
         <v>187</v>
       </c>
-      <c r="B83" s="140" t="s">
+      <c r="B83" s="77" t="s">
         <v>182</v>
       </c>
       <c r="C83" s="109" t="s">
@@ -17738,7 +17884,7 @@
       <c r="A84" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B84" s="141">
+      <c r="B84" s="84">
         <v>1</v>
       </c>
       <c r="C84" s="115">
@@ -17750,7 +17896,7 @@
       <c r="A85" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B85" s="141">
+      <c r="B85" s="84">
         <f>2.2/6</f>
         <v>0.3666666666666667</v>
       </c>
@@ -17764,7 +17910,7 @@
       <c r="A86" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B86" s="141">
+      <c r="B86" s="84">
         <f>2.7/6</f>
         <v>0.45</v>
       </c>
@@ -17774,25 +17920,25 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="128" t="s">
+      <c r="A87" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="B87" s="141">
+      <c r="B87" s="84">
         <f>2.1/6</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="C87" s="130">
+      <c r="C87" s="150">
         <f>_xlfn.EXPON.DIST(B88,$B$81,TRUE) - _xlfn.EXPON.DIST(B87,$B$81,TRUE)</f>
         <v>0.25047716007445753</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="129"/>
-      <c r="B88" s="142">
+      <c r="A88" s="149"/>
+      <c r="B88" s="81">
         <f>4.5/6</f>
         <v>0.75</v>
       </c>
-      <c r="C88" s="131"/>
+      <c r="C88" s="151"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="93"/>
@@ -17815,15 +17961,15 @@
       <c r="C92" s="91"/>
     </row>
     <row r="93" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A93" s="127" t="s">
+      <c r="A93" s="147" t="s">
         <v>181</v>
       </c>
-      <c r="B93" s="127"/>
-      <c r="C93" s="127"/>
-      <c r="D93" s="127"/>
-      <c r="E93" s="127"/>
-      <c r="F93" s="127"/>
-      <c r="G93" s="127"/>
+      <c r="B93" s="147"/>
+      <c r="C93" s="147"/>
+      <c r="D93" s="147"/>
+      <c r="E93" s="147"/>
+      <c r="F93" s="147"/>
+      <c r="G93" s="147"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D94" s="75"/>
@@ -18064,7 +18210,7 @@
       <c r="C115" s="113">
         <v>0.35</v>
       </c>
-      <c r="D115" s="138">
+      <c r="D115" s="126">
         <f>C115*($B$110*MIN($B$111, B115) - $B$112)</f>
         <v>-43.75</v>
       </c>
@@ -18079,7 +18225,7 @@
       <c r="C116" s="113">
         <v>0.2</v>
       </c>
-      <c r="D116" s="138">
+      <c r="D116" s="126">
         <f t="shared" ref="D116:D117" si="5">C116*($B$110*MIN($B$111, B116) - $B$112)</f>
         <v>10</v>
       </c>
@@ -18094,7 +18240,7 @@
       <c r="C117" s="113">
         <v>0.45</v>
       </c>
-      <c r="D117" s="138">
+      <c r="D117" s="126">
         <f t="shared" si="5"/>
         <v>101.25</v>
       </c>
@@ -18103,7 +18249,7 @@
       <c r="A118" s="79"/>
       <c r="B118" s="79"/>
       <c r="C118" s="79"/>
-      <c r="D118" s="139">
+      <c r="D118" s="127">
         <f>SUM(D115:D117)</f>
         <v>67.5</v>
       </c>
@@ -18138,7 +18284,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18149,15 +18295,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="147" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
@@ -18419,15 +18565,15 @@
       <c r="B27" s="107"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="127" t="s">
+      <c r="A28" s="147" t="s">
         <v>242</v>
       </c>
-      <c r="B28" s="127"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="127"/>
-      <c r="E28" s="127"/>
-      <c r="F28" s="127"/>
-      <c r="G28" s="127"/>
+      <c r="B28" s="147"/>
+      <c r="C28" s="147"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="147"/>
+      <c r="F28" s="147"/>
+      <c r="G28" s="147"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D29" s="76"/>
@@ -18610,7 +18756,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="109"/>
-      <c r="B48" s="140" t="s">
+      <c r="B48" s="77" t="s">
         <v>182</v>
       </c>
       <c r="C48" s="109" t="s">
@@ -18629,7 +18775,7 @@
       <c r="A49" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B49" s="147">
+      <c r="B49" s="128">
         <v>1</v>
       </c>
       <c r="C49" s="115">
@@ -18649,7 +18795,7 @@
       <c r="A50" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="147">
+      <c r="B50" s="128">
         <v>1</v>
       </c>
       <c r="C50" s="115">
@@ -18669,7 +18815,7 @@
       <c r="A51" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B51" s="147">
+      <c r="B51" s="128">
         <v>1</v>
       </c>
       <c r="C51" s="115">
@@ -18686,33 +18832,33 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="128" t="s">
+      <c r="A52" s="148" t="s">
         <v>201</v>
       </c>
-      <c r="B52" s="147">
+      <c r="B52" s="128">
         <v>1</v>
       </c>
-      <c r="C52" s="130">
+      <c r="C52" s="150">
         <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="132">
+      <c r="D52" s="152">
         <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="130">
+      <c r="E52" s="150">
         <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="129"/>
-      <c r="B53" s="148">
+      <c r="A53" s="149"/>
+      <c r="B53" s="129">
         <v>1</v>
       </c>
-      <c r="C53" s="131"/>
-      <c r="D53" s="133"/>
-      <c r="E53" s="131"/>
+      <c r="C53" s="151"/>
+      <c r="D53" s="153"/>
+      <c r="E53" s="151"/>
       <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -18821,318 +18967,403 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22.6640625" style="141" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="22.6640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="75"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="154" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="76"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="A2" s="130"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="134" t="s">
+      <c r="A3" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="84">
-        <v>75</v>
-      </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="B3" s="134">
+        <v>30</v>
+      </c>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="134" t="s">
+      <c r="A4" s="133" t="s">
         <v>233</v>
       </c>
-      <c r="B4" s="135">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="B4" s="134">
+        <v>31</v>
+      </c>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="133" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="134">
+        <v>0.18</v>
+      </c>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="133" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="134">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="133" t="s">
         <v>255</v>
       </c>
-      <c r="B5" s="135">
-        <v>14.4</v>
-      </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="134" t="s">
+      <c r="B7" s="134">
+        <v>6</v>
+      </c>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="133" t="s">
         <v>254</v>
       </c>
-      <c r="B6" s="135">
-        <v>14.4</v>
-      </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="134" t="s">
+      <c r="B8" s="134">
+        <v>2.6997942308422096</v>
+      </c>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="133" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="84">
-        <v>30</v>
-      </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="134" t="s">
+      <c r="B9" s="134">
+        <v>40</v>
+      </c>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="133" t="s">
         <v>250</v>
       </c>
-      <c r="B8" s="84">
-        <v>1</v>
-      </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="134" t="s">
+      <c r="B10" s="134">
+        <v>2</v>
+      </c>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="133" t="s">
         <v>252</v>
       </c>
-      <c r="B9" s="84">
-        <v>0.1</v>
-      </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="134" t="s">
+      <c r="B11" s="134">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="132"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="133" t="s">
         <v>253</v>
       </c>
-      <c r="B10" s="84">
-        <v>2.1038836780136476</v>
-      </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="134" t="s">
+      <c r="B12" s="134">
+        <v>0.61595762357319761</v>
+      </c>
+      <c r="C12" s="131"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="132"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="133" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="134">
+        <v>0.61595762357319761</v>
+      </c>
+      <c r="C13" s="131"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="132"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="80"/>
+      <c r="B14" s="157"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="161" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="137">
+        <f>(B4-B3)/(B8/SQRT(B9))</f>
+        <v>2.3426064283290926</v>
+      </c>
+      <c r="C15" s="131"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="161" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="162">
+        <f>(B6-B5)/SQRT(B5*(1-B5)/B9)</f>
+        <v>0.32924319888319686</v>
+      </c>
+      <c r="C16" s="131"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="132"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="142"/>
+      <c r="B18" s="159" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="159" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="131"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="136" t="s">
         <v>259</v>
       </c>
-      <c r="B11" s="84">
-        <v>-2.5103950552320091</v>
-      </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="152" t="s">
-        <v>256</v>
-      </c>
-      <c r="C13" s="108" t="s">
-        <v>257</v>
-      </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="123" t="s">
+      <c r="B19" s="160">
+        <f>_xlfn.NORM.S.INV(1-B11)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="C19" s="137">
+        <f>_xlfn.T.INV(B11, (B9-1))</f>
+        <v>-1.6848751217112248</v>
+      </c>
+      <c r="D19" s="158">
+        <f>_xlfn.T.INV(1-B11, B9)</f>
+        <v>1.6838510133356521</v>
+      </c>
+      <c r="F19" s="132"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="136" t="s">
         <v>260</v>
       </c>
-      <c r="B14" s="130">
-        <f>_xlfn.NORM.S.INV(1-B9)</f>
-        <v>1.2815515655446006</v>
-      </c>
-      <c r="C14" s="115">
-        <f>_xlfn.T.INV(1-B9, B7)</f>
-        <v>1.3104150253913947</v>
-      </c>
-      <c r="D14" s="79"/>
-      <c r="F14" s="75"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="115">
-        <f>_xlfn.T.INV((B9/B8), B7)</f>
-        <v>-1.3104150253913947</v>
-      </c>
-      <c r="D15" s="151">
-        <f>_xlfn.T.INV(1-(B9/B8),B7)</f>
-        <v>1.3104150253913947</v>
-      </c>
-      <c r="F15" s="75"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="149" t="s">
-        <v>258</v>
-      </c>
-      <c r="B16" s="153">
-        <f>(B4-B3)/(B5/SQRT(B7))</f>
-        <v>-2.5103950552320091</v>
-      </c>
-      <c r="C16" s="154"/>
-      <c r="D16" s="79"/>
-      <c r="F16" s="75"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="150" t="s">
+      <c r="B20" s="160"/>
+      <c r="C20" s="137">
+        <f>_xlfn.T.INV((B11/B10), B9)</f>
+        <v>-2.0210753903062737</v>
+      </c>
+      <c r="D20" s="158">
+        <f>_xlfn.T.INV(1-(B11/B10),B9)</f>
+        <v>2.0210753903062715</v>
+      </c>
+      <c r="F20" s="132" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="136" t="s">
         <v>247</v>
       </c>
-      <c r="B17" s="115">
-        <f>_xlfn.NORM.S.DIST(B10, TRUE)</f>
-        <v>0.98230570245217108</v>
-      </c>
-      <c r="C17" s="115">
-        <f>_xlfn.T.DIST(B11, B7, TRUE)</f>
-        <v>8.8413521905273355E-3</v>
-      </c>
-      <c r="D17" s="79"/>
-      <c r="F17" s="75"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="150" t="s">
+      <c r="B21" s="137">
+        <f>_xlfn.NORM.S.DIST(B12, TRUE)</f>
+        <v>0.73103875575403099</v>
+      </c>
+      <c r="C21" s="137">
+        <f>_xlfn.T.DIST(B13, (B9-1), TRUE)</f>
+        <v>0.72924949230545577</v>
+      </c>
+      <c r="D21" s="131"/>
+      <c r="F21" s="75" t="s">
+        <v>266</v>
+      </c>
+      <c r="G21" s="75">
+        <f>B3 + B19 * (B7/SQRT(B9))</f>
+        <v>31.560445163626671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="138" t="s">
         <v>248</v>
       </c>
-      <c r="B18" s="115">
-        <f>1-B17</f>
-        <v>1.7694297547828919E-2</v>
-      </c>
-      <c r="C18" s="115">
-        <f>1-C17</f>
-        <v>0.99115864780947271</v>
-      </c>
-      <c r="D18" s="79"/>
-      <c r="F18" s="75"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="149" t="s">
+      <c r="B22" s="139">
+        <f>1-B21</f>
+        <v>0.26896124424596901</v>
+      </c>
+      <c r="C22" s="139">
+        <f>1-C21</f>
+        <v>0.27075050769454423</v>
+      </c>
+      <c r="D22" s="131"/>
+      <c r="F22" s="132" t="s">
+        <v>265</v>
+      </c>
+      <c r="G22" s="75">
+        <f>_xlfn.NORM.DIST(G21, G20, B7/SQRT(B9), TRUE)</f>
+        <v>0.72265973985512544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="139">
+        <f>IF(B11&gt;0, B22, B21)</f>
+        <v>0.26896124424596901</v>
+      </c>
+      <c r="C23" s="139"/>
+      <c r="D23" s="131"/>
+      <c r="F23" s="132"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="138" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="115">
-        <f>B8 * IF(B10&gt;0, B18, B17)</f>
-        <v>1.7694297547828919E-2</v>
-      </c>
-      <c r="C19" s="115">
-        <f>B8 * IF(B11&gt;0, C18, C17)</f>
-        <v>8.8413521905273355E-3</v>
-      </c>
-      <c r="D19" s="79"/>
-      <c r="F19" s="75"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="149" t="s">
+      <c r="B24" s="135">
+        <f>B10 * IF(B12&gt;0, B22, B21)</f>
+        <v>0.53792248849193802</v>
+      </c>
+      <c r="C24" s="135">
+        <f>B10 * IF(B13&gt;0, C22, C21)</f>
+        <v>0.54150101538908846</v>
+      </c>
+      <c r="D24" s="131"/>
+      <c r="E24" s="141"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="138" t="s">
         <v>251</v>
       </c>
-      <c r="B20" s="117" t="str">
-        <f>IF(B19&lt;B9, "Reject", "Do not reject")</f>
-        <v>Reject</v>
-      </c>
-      <c r="C20" s="117" t="str">
-        <f>IF(C19&lt;C9, "Reject", "Do not reject")</f>
+      <c r="B25" s="135" t="str">
+        <f>IF(B24&lt;B11, "Reject", "Do not reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="F20" s="75"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="75"/>
-      <c r="F21" s="75"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="76"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="76"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="76"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-    </row>
-    <row r="25" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A25" s="127" t="s">
+      <c r="C25" s="135" t="str">
+        <f>IF(C24&lt;B11, "Reject", "Do not reject")</f>
+        <v>Do not reject</v>
+      </c>
+      <c r="D25" s="143"/>
+      <c r="F25" s="132"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C26" s="131"/>
+      <c r="F26" s="132"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="130"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="131"/>
+      <c r="F27" s="132"/>
+      <c r="G27" s="132"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="130"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="131"/>
+      <c r="F28" s="132"/>
+      <c r="G28" s="132"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="130"/>
+      <c r="B29" s="140"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="132"/>
+    </row>
+    <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A30" s="154" t="s">
         <v>246</v>
       </c>
-      <c r="B25" s="126"/>
-      <c r="C25" s="126"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="126"/>
-      <c r="F25" s="126"/>
-      <c r="G25" s="126"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added formula type b 2 error for hypothesis
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464DB1F-5C88-2848-94A2-4813BD293F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E694990-FF5E-3A4D-B2F8-7E47512ED539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="267">
   <si>
     <t>E</t>
   </si>
@@ -893,13 +893,13 @@
     <t>statistic test mean</t>
   </si>
   <si>
-    <t>p-value proportion</t>
-  </si>
-  <si>
-    <t>Type error 2</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>tail test</t>
+  </si>
+  <si>
+    <t>Type II error Bx</t>
+  </si>
+  <si>
+    <t>Type II error BPx</t>
   </si>
 </sst>
 </file>
@@ -18284,7 +18284,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18967,10 +18967,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I26" sqref="F17:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19097,7 +19097,7 @@
         <v>250</v>
       </c>
       <c r="B10" s="134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="131"/>
       <c r="D10" s="131"/>
@@ -19182,188 +19182,201 @@
       <c r="G16" s="132"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="161" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17" s="162">
+        <f>B3 + B21 * (B7/SQRT(B9))</f>
+        <v>31.560445163626671</v>
+      </c>
       <c r="C17" s="131"/>
       <c r="D17" s="131"/>
       <c r="E17" s="132"/>
       <c r="F17" s="132"/>
+      <c r="G17" s="132"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="142"/>
-      <c r="B18" s="159" t="s">
-        <v>256</v>
-      </c>
-      <c r="C18" s="159" t="s">
-        <v>257</v>
-      </c>
+      <c r="A18" s="161" t="s">
+        <v>266</v>
+      </c>
+      <c r="B18" s="162">
+        <f>_xlfn.NORM.DIST(G23, G22, B7/SQRT(B9), TRUE)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="131"/>
       <c r="D18" s="131"/>
       <c r="E18" s="132"/>
       <c r="F18" s="132"/>
+      <c r="G18" s="132"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="136" t="s">
+      <c r="C19" s="131"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="142"/>
+      <c r="B20" s="159" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="159" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="131"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="132"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="136" t="s">
         <v>259</v>
       </c>
-      <c r="B19" s="160">
+      <c r="B21" s="160">
         <f>_xlfn.NORM.S.INV(1-B11)</f>
         <v>1.6448536269514715</v>
       </c>
-      <c r="C19" s="137">
+      <c r="C21" s="137">
         <f>_xlfn.T.INV(B11, (B9-1))</f>
         <v>-1.6848751217112248</v>
       </c>
-      <c r="D19" s="158">
+      <c r="D21" s="158">
         <f>_xlfn.T.INV(1-B11, B9)</f>
         <v>1.6838510133356521</v>
       </c>
-      <c r="F19" s="132"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="136" t="s">
+      <c r="F21" s="132"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="136" t="s">
         <v>260</v>
       </c>
-      <c r="B20" s="160"/>
-      <c r="C20" s="137">
+      <c r="B22" s="160"/>
+      <c r="C22" s="137">
         <f>_xlfn.T.INV((B11/B10), B9)</f>
-        <v>-2.0210753903062737</v>
-      </c>
-      <c r="D20" s="158">
+        <v>-1.6838510133356521</v>
+      </c>
+      <c r="D22" s="158">
         <f>_xlfn.T.INV(1-(B11/B10),B9)</f>
-        <v>2.0210753903062715</v>
-      </c>
-      <c r="F20" s="132" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="75">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="136" t="s">
+        <v>1.6838510133356521</v>
+      </c>
+      <c r="F22" s="132"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="136" t="s">
         <v>247</v>
       </c>
-      <c r="B21" s="137">
+      <c r="B23" s="137">
         <f>_xlfn.NORM.S.DIST(B12, TRUE)</f>
         <v>0.73103875575403099</v>
       </c>
-      <c r="C21" s="137">
+      <c r="C23" s="137">
         <f>_xlfn.T.DIST(B13, (B9-1), TRUE)</f>
         <v>0.72924949230545577</v>
       </c>
-      <c r="D21" s="131"/>
-      <c r="F21" s="75" t="s">
-        <v>266</v>
-      </c>
-      <c r="G21" s="75">
-        <f>B3 + B19 * (B7/SQRT(B9))</f>
-        <v>31.560445163626671</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="138" t="s">
-        <v>248</v>
-      </c>
-      <c r="B22" s="139">
-        <f>1-B21</f>
-        <v>0.26896124424596901</v>
-      </c>
-      <c r="C22" s="139">
-        <f>1-C21</f>
-        <v>0.27075050769454423</v>
-      </c>
-      <c r="D22" s="131"/>
-      <c r="F22" s="132" t="s">
-        <v>265</v>
-      </c>
-      <c r="G22" s="75">
-        <f>_xlfn.NORM.DIST(G21, G20, B7/SQRT(B9), TRUE)</f>
-        <v>0.72265973985512544</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="138" t="s">
-        <v>264</v>
-      </c>
-      <c r="B23" s="139">
-        <f>IF(B11&gt;0, B22, B21)</f>
-        <v>0.26896124424596901</v>
-      </c>
-      <c r="C23" s="139"/>
       <c r="D23" s="131"/>
-      <c r="F23" s="132"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="138" t="s">
-        <v>249</v>
-      </c>
-      <c r="B24" s="135">
-        <f>B10 * IF(B12&gt;0, B22, B21)</f>
-        <v>0.53792248849193802</v>
-      </c>
-      <c r="C24" s="135">
-        <f>B10 * IF(B13&gt;0, C22, C21)</f>
-        <v>0.54150101538908846</v>
+        <v>248</v>
+      </c>
+      <c r="B24" s="139">
+        <f>1-B23</f>
+        <v>0.26896124424596901</v>
+      </c>
+      <c r="C24" s="139">
+        <f>1-C23</f>
+        <v>0.27075050769454423</v>
       </c>
       <c r="D24" s="131"/>
-      <c r="E24" s="141"/>
+      <c r="F24" s="132"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="138" t="s">
+        <v>264</v>
+      </c>
+      <c r="B25" s="139" t="str">
+        <f>IF(B12&gt;0, "Right", "Left")</f>
+        <v>Right</v>
+      </c>
+      <c r="C25" s="139" t="str">
+        <f>IF(B13&gt;0, "Right", "Left")</f>
+        <v>Right</v>
+      </c>
+      <c r="D25" s="131"/>
+      <c r="F25" s="132"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="138" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="135">
+        <f>B10*IF(B25="Right",B24,B23)</f>
+        <v>0.26896124424596901</v>
+      </c>
+      <c r="C26" s="135">
+        <f>B10 * IF(C25="Right", C24, C23)</f>
+        <v>0.27075050769454423</v>
+      </c>
+      <c r="D26" s="131"/>
+      <c r="E26" s="141"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="138" t="s">
         <v>251</v>
       </c>
-      <c r="B25" s="135" t="str">
-        <f>IF(B24&lt;B11, "Reject", "Do not reject")</f>
+      <c r="B27" s="135" t="str">
+        <f>IF(B26&lt;B11, "Reject", "Do not reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="C25" s="135" t="str">
-        <f>IF(C24&lt;B11, "Reject", "Do not reject")</f>
+      <c r="C27" s="135" t="str">
+        <f>IF(C26&lt;B11, "Reject", "Do not reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="D25" s="143"/>
-      <c r="F25" s="132"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="131"/>
-      <c r="F26" s="132"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="130"/>
-      <c r="B27" s="140"/>
-      <c r="C27" s="131"/>
+      <c r="D27" s="143"/>
       <c r="F27" s="132"/>
-      <c r="G27" s="132"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="130"/>
-      <c r="B28" s="140"/>
       <c r="C28" s="131"/>
       <c r="F28" s="132"/>
-      <c r="G28" s="132"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="130"/>
       <c r="B29" s="140"/>
       <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
       <c r="F29" s="132"/>
       <c r="G29" s="132"/>
     </row>
-    <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="154" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="130"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="131"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="130"/>
+      <c r="B31" s="140"/>
+      <c r="C31" s="131"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="132"/>
+    </row>
+    <row r="32" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A32" s="154" t="s">
         <v>246</v>
       </c>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="156"/>
-      <c r="F30" s="156"/>
-      <c r="G30" s="156"/>
+      <c r="B32" s="155"/>
+      <c r="C32" s="155"/>
+      <c r="D32" s="155"/>
+      <c r="E32" s="156"/>
+      <c r="F32" s="156"/>
+      <c r="G32" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Refactored formulas for T distributions and Type 2 error in sample hypotheses
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E694990-FF5E-3A4D-B2F8-7E47512ED539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BA84B5-4533-404A-9CCC-A03114B94EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="264">
   <si>
     <t>E</t>
   </si>
@@ -851,18 +851,9 @@
     <t>p-value</t>
   </si>
   <si>
-    <t># tail test</t>
-  </si>
-  <si>
     <t>hypothesis</t>
   </si>
   <si>
-    <t>test statistic</t>
-  </si>
-  <si>
-    <t>statistic z-test</t>
-  </si>
-  <si>
     <t>sample std deviation</t>
   </si>
   <si>
@@ -875,38 +866,38 @@
     <t>T Distribution</t>
   </si>
   <si>
-    <t>statistics t-test</t>
-  </si>
-  <si>
-    <t>critical score (one tail)</t>
-  </si>
-  <si>
-    <t>critical score (two tail)</t>
-  </si>
-  <si>
-    <t>statistic test  proportion</t>
-  </si>
-  <si>
     <t>sample proportion</t>
   </si>
   <si>
-    <t>statistic test mean</t>
-  </si>
-  <si>
-    <t>tail test</t>
-  </si>
-  <si>
     <t>Type II error Bx</t>
   </si>
   <si>
     <t>Type II error BPx</t>
+  </si>
+  <si>
+    <t>critical score value</t>
+  </si>
+  <si>
+    <t>Use T distribution when you have sample standard deviation (s)</t>
+  </si>
+  <si>
+    <t># tail tests</t>
+  </si>
+  <si>
+    <t>significance level</t>
+  </si>
+  <si>
+    <t>ZT test statistic mean</t>
+  </si>
+  <si>
+    <t>ZT test statistic proportion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -914,8 +905,9 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1017,8 +1009,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1048,8 +1047,14 @@
         <fgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1170,80 +1175,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1531,30 +1469,40 @@
     <xf numFmtId="4" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1562,7 +1510,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1576,6 +1523,7 @@
     <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1591,31 +1539,65 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -12895,21 +12877,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="144">
+      <c r="C17" s="148">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="145"/>
+      <c r="D17" s="149"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="144">
+      <c r="C18" s="148">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="145"/>
+      <c r="D18" s="149"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -16989,15 +16971,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="155" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
@@ -17191,15 +17173,15 @@
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="146" t="s">
+      <c r="A14" s="155" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="146"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="146"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
+      <c r="B14" s="155"/>
+      <c r="C14" s="155"/>
+      <c r="D14" s="155"/>
+      <c r="E14" s="155"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="155"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -17368,13 +17350,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="148" t="s">
+      <c r="A26" s="151" t="s">
         <v>201</v>
       </c>
       <c r="B26" s="83">
         <v>29</v>
       </c>
-      <c r="C26" s="150">
+      <c r="C26" s="153">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17383,11 +17365,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="149"/>
+      <c r="A27" s="152"/>
       <c r="B27" s="81">
         <v>37</v>
       </c>
-      <c r="C27" s="151"/>
+      <c r="C27" s="154"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17403,15 +17385,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="147" t="s">
+      <c r="A30" s="150" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="147"/>
-      <c r="C30" s="147"/>
-      <c r="D30" s="147"/>
-      <c r="E30" s="147"/>
-      <c r="F30" s="147"/>
-      <c r="G30" s="147"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="150"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17546,13 +17528,13 @@
       <c r="H39" s="79"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="148" t="s">
+      <c r="A40" s="151" t="s">
         <v>201</v>
       </c>
       <c r="B40" s="83">
         <v>3300</v>
       </c>
-      <c r="C40" s="150">
+      <c r="C40" s="153">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
         <v>0</v>
       </c>
@@ -17561,11 +17543,11 @@
       <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="149"/>
+      <c r="A41" s="152"/>
       <c r="B41" s="81">
         <v>4200</v>
       </c>
-      <c r="C41" s="151"/>
+      <c r="C41" s="154"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
       <c r="H41" s="79"/>
@@ -17592,15 +17574,15 @@
       <c r="H44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="147" t="s">
+      <c r="A46" s="150" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="147"/>
-      <c r="C46" s="147"/>
-      <c r="D46" s="147"/>
-      <c r="E46" s="147"/>
-      <c r="F46" s="147"/>
-      <c r="G46" s="147"/>
+      <c r="B46" s="150"/>
+      <c r="C46" s="150"/>
+      <c r="D46" s="150"/>
+      <c r="E46" s="150"/>
+      <c r="F46" s="150"/>
+      <c r="G46" s="150"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="83" t="s">
@@ -17693,23 +17675,23 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="148" t="s">
+      <c r="A58" s="151" t="s">
         <v>201</v>
       </c>
       <c r="B58" s="83">
         <v>2</v>
       </c>
-      <c r="C58" s="150">
+      <c r="C58" s="153">
         <f>_xlfn.BINOM.DIST(B59,$B$48,$B$49,TRUE) - _xlfn.BINOM.DIST(B58,$B$48,$B$49,TRUE)</f>
         <v>0.30165667656250023</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="149"/>
+      <c r="A59" s="152"/>
       <c r="B59" s="81">
         <v>6</v>
       </c>
-      <c r="C59" s="151"/>
+      <c r="C59" s="154"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="93"/>
@@ -17727,15 +17709,15 @@
       <c r="C62" s="91"/>
     </row>
     <row r="64" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A64" s="147" t="s">
+      <c r="A64" s="150" t="s">
         <v>198</v>
       </c>
-      <c r="B64" s="147"/>
-      <c r="C64" s="147"/>
-      <c r="D64" s="147"/>
-      <c r="E64" s="147"/>
-      <c r="F64" s="147"/>
-      <c r="G64" s="147"/>
+      <c r="B64" s="150"/>
+      <c r="C64" s="150"/>
+      <c r="D64" s="150"/>
+      <c r="E64" s="150"/>
+      <c r="F64" s="150"/>
+      <c r="G64" s="150"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="83" t="s">
@@ -17802,23 +17784,23 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="148" t="s">
+      <c r="A73" s="151" t="s">
         <v>201</v>
       </c>
       <c r="B73" s="83">
         <v>2</v>
       </c>
-      <c r="C73" s="150">
+      <c r="C73" s="153">
         <f>_xlfn.POISSON.DIST(B74,$B$66,TRUE) - _xlfn.POISSON.DIST(B73,$B$66,TRUE)</f>
         <v>3.8791531399499785E-3</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="149"/>
+      <c r="A74" s="152"/>
       <c r="B74" s="81">
         <v>5</v>
       </c>
-      <c r="C74" s="151"/>
+      <c r="C74" s="154"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="93"/>
@@ -17841,15 +17823,15 @@
       <c r="C78" s="91"/>
     </row>
     <row r="79" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A79" s="147" t="s">
+      <c r="A79" s="150" t="s">
         <v>199</v>
       </c>
-      <c r="B79" s="147"/>
-      <c r="C79" s="147"/>
-      <c r="D79" s="147"/>
-      <c r="E79" s="147"/>
-      <c r="F79" s="147"/>
-      <c r="G79" s="147"/>
+      <c r="B79" s="150"/>
+      <c r="C79" s="150"/>
+      <c r="D79" s="150"/>
+      <c r="E79" s="150"/>
+      <c r="F79" s="150"/>
+      <c r="G79" s="150"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B80" s="80"/>
@@ -17920,25 +17902,25 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="148" t="s">
+      <c r="A87" s="151" t="s">
         <v>201</v>
       </c>
       <c r="B87" s="84">
         <f>2.1/6</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="C87" s="150">
+      <c r="C87" s="153">
         <f>_xlfn.EXPON.DIST(B88,$B$81,TRUE) - _xlfn.EXPON.DIST(B87,$B$81,TRUE)</f>
         <v>0.25047716007445753</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="149"/>
+      <c r="A88" s="152"/>
       <c r="B88" s="81">
         <f>4.5/6</f>
         <v>0.75</v>
       </c>
-      <c r="C88" s="151"/>
+      <c r="C88" s="154"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="93"/>
@@ -17961,15 +17943,15 @@
       <c r="C92" s="91"/>
     </row>
     <row r="93" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A93" s="147" t="s">
+      <c r="A93" s="150" t="s">
         <v>181</v>
       </c>
-      <c r="B93" s="147"/>
-      <c r="C93" s="147"/>
-      <c r="D93" s="147"/>
-      <c r="E93" s="147"/>
-      <c r="F93" s="147"/>
-      <c r="G93" s="147"/>
+      <c r="B93" s="150"/>
+      <c r="C93" s="150"/>
+      <c r="D93" s="150"/>
+      <c r="E93" s="150"/>
+      <c r="F93" s="150"/>
+      <c r="G93" s="150"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D94" s="75"/>
@@ -18256,6 +18238,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="A93:G93"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
@@ -18266,13 +18255,6 @@
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="C87:C88"/>
     <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18295,15 +18277,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="150" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
@@ -18565,15 +18547,15 @@
       <c r="B27" s="107"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="147" t="s">
+      <c r="A28" s="150" t="s">
         <v>242</v>
       </c>
-      <c r="B28" s="147"/>
-      <c r="C28" s="147"/>
-      <c r="D28" s="147"/>
-      <c r="E28" s="147"/>
-      <c r="F28" s="147"/>
-      <c r="G28" s="147"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D29" s="76"/>
@@ -18832,33 +18814,33 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="148" t="s">
+      <c r="A52" s="151" t="s">
         <v>201</v>
       </c>
       <c r="B52" s="128">
         <v>1</v>
       </c>
-      <c r="C52" s="150">
+      <c r="C52" s="153">
         <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="152">
+      <c r="D52" s="156">
         <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="150">
+      <c r="E52" s="153">
         <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="149"/>
+      <c r="A53" s="152"/>
       <c r="B53" s="129">
         <v>1</v>
       </c>
-      <c r="C53" s="151"/>
-      <c r="D53" s="153"/>
-      <c r="E53" s="151"/>
+      <c r="C53" s="154"/>
+      <c r="D53" s="157"/>
+      <c r="E53" s="154"/>
       <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -18967,30 +18949,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="F17:I26"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="22.6640625" style="141" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="75" customWidth="1"/>
+    <col min="2" max="4" width="22.6640625" style="137" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="22.6640625" style="75" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="75"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="158" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="130"/>
@@ -19032,7 +19014,7 @@
         <v>222</v>
       </c>
       <c r="B5" s="134">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="C5" s="131"/>
       <c r="D5" s="131"/>
@@ -19042,10 +19024,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="133" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B6" s="134">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="131"/>
       <c r="D6" s="131"/>
@@ -19055,7 +19037,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="133" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B7" s="134">
         <v>6</v>
@@ -19067,11 +19049,11 @@
       <c r="G7" s="132"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="133" t="s">
-        <v>254</v>
+      <c r="A8" s="142" t="s">
+        <v>251</v>
       </c>
       <c r="B8" s="134">
-        <v>2.6997942308422096</v>
+        <v>0</v>
       </c>
       <c r="C8" s="131"/>
       <c r="D8" s="131"/>
@@ -19094,10 +19076,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="B10" s="134">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C10" s="131"/>
       <c r="D10" s="131"/>
@@ -19107,10 +19089,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="133" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B11" s="134">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="C11" s="131"/>
       <c r="D11" s="131"/>
@@ -19119,12 +19101,8 @@
       <c r="G11" s="132"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="133" t="s">
-        <v>253</v>
-      </c>
-      <c r="B12" s="134">
-        <v>0.61595762357319761</v>
-      </c>
+      <c r="A12" s="80"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="131"/>
       <c r="D12" s="131"/>
       <c r="E12" s="132"/>
@@ -19132,11 +19110,12 @@
       <c r="G12" s="132"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="133" t="s">
-        <v>258</v>
-      </c>
-      <c r="B13" s="134">
-        <v>0.61595762357319761</v>
+      <c r="A13" s="83" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="143">
+        <f>B14</f>
+        <v>1.0540925533894598</v>
       </c>
       <c r="C13" s="131"/>
       <c r="D13" s="131"/>
@@ -19145,8 +19124,13 @@
       <c r="G13" s="132"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="80"/>
-      <c r="B14" s="157"/>
+      <c r="A14" s="140" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" s="135">
+        <f>(B4-B3)/(IF(B8&gt;0, B8, B7)/SQRT(B9))</f>
+        <v>1.0540925533894598</v>
+      </c>
       <c r="C14" s="131"/>
       <c r="D14" s="131"/>
       <c r="E14" s="132"/>
@@ -19154,12 +19138,12 @@
       <c r="G14" s="132"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="161" t="s">
+      <c r="A15" s="140" t="s">
         <v>263</v>
       </c>
-      <c r="B15" s="137">
-        <f>(B4-B3)/(B8/SQRT(B9))</f>
-        <v>2.3426064283290926</v>
+      <c r="B15" s="141">
+        <f>IF(B5 &gt; 0, (B6-B5)/SQRT(B5*(1-B5)/B9), 0)</f>
+        <v>0</v>
       </c>
       <c r="C15" s="131"/>
       <c r="D15" s="131"/>
@@ -19168,12 +19152,12 @@
       <c r="G15" s="132"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="161" t="s">
-        <v>261</v>
-      </c>
-      <c r="B16" s="162">
-        <f>(B6-B5)/SQRT(B5*(1-B5)/B9)</f>
-        <v>0.32924319888319686</v>
+      <c r="A16" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="141">
+        <f>B3 + B21 * (B7/SQRT(B9))</f>
+        <v>31.560445163626671</v>
       </c>
       <c r="C16" s="131"/>
       <c r="D16" s="131"/>
@@ -19182,12 +19166,12 @@
       <c r="G16" s="132"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="161" t="s">
-        <v>265</v>
-      </c>
-      <c r="B17" s="162">
-        <f>B3 + B21 * (B7/SQRT(B9))</f>
-        <v>31.560445163626671</v>
+      <c r="A17" s="140" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="141">
+        <f>_xlfn.NORM.DIST(B16,B4, B7/SQRT(B9), TRUE)</f>
+        <v>0.72265973985512544</v>
       </c>
       <c r="C17" s="131"/>
       <c r="D17" s="131"/>
@@ -19195,189 +19179,171 @@
       <c r="F17" s="132"/>
       <c r="G17" s="132"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="161" t="s">
-        <v>266</v>
-      </c>
-      <c r="B18" s="162">
-        <f>_xlfn.NORM.DIST(G23, G22, B7/SQRT(B9), TRUE)</f>
-        <v>0.5</v>
-      </c>
-      <c r="C18" s="131"/>
-      <c r="D18" s="131"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="132"/>
-    </row>
+    <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="131"/>
+      <c r="A19" s="161" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="161"/>
+      <c r="C19" s="161"/>
       <c r="D19" s="131"/>
       <c r="E19" s="132"/>
       <c r="F19" s="132"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="142"/>
-      <c r="B20" s="159" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" s="159" t="s">
-        <v>257</v>
+      <c r="A20" s="145"/>
+      <c r="B20" s="146" t="s">
+        <v>253</v>
+      </c>
+      <c r="C20" s="146" t="s">
+        <v>254</v>
       </c>
       <c r="D20" s="131"/>
-      <c r="E20" s="132"/>
+      <c r="E20" s="131"/>
       <c r="F20" s="132"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="136" t="s">
-        <v>259</v>
-      </c>
-      <c r="B21" s="160">
-        <f>_xlfn.NORM.S.INV(1-B11)</f>
+      <c r="A21" s="140" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" s="147">
+        <f>_xlfn.NORM.S.INV(1-B10)</f>
         <v>1.6448536269514715</v>
       </c>
-      <c r="C21" s="137">
-        <f>_xlfn.T.INV(B11, (B9-1))</f>
-        <v>-1.6848751217112248</v>
-      </c>
-      <c r="D21" s="158">
-        <f>_xlfn.T.INV(1-B11, B9)</f>
-        <v>1.6838510133356521</v>
-      </c>
-      <c r="F21" s="132"/>
+      <c r="C21" s="135">
+        <f>_xlfn.T.INV(IF(B11=1, 1-B10, B10/B11), B9 -1)</f>
+        <v>1.6848751217112248</v>
+      </c>
+      <c r="D21" s="75"/>
+      <c r="E21" s="132"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="136" t="s">
-        <v>260</v>
-      </c>
-      <c r="B22" s="160"/>
-      <c r="C22" s="137">
-        <f>_xlfn.T.INV((B11/B10), B9)</f>
-        <v>-1.6838510133356521</v>
-      </c>
-      <c r="D22" s="158">
-        <f>_xlfn.T.INV(1-(B11/B10),B9)</f>
-        <v>1.6838510133356521</v>
-      </c>
-      <c r="F22" s="132"/>
+      <c r="A22" s="140" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="135">
+        <f>_xlfn.NORM.S.DIST(IF(B15 &gt; 0, B15, B13), TRUE)</f>
+        <v>0.85407972742810578</v>
+      </c>
+      <c r="C22" s="135">
+        <f>_xlfn.T.DIST(IF(B15 &gt; B15, B15, B13), (B9-1), TRUE)</f>
+        <v>0.8508362851697302</v>
+      </c>
+      <c r="D22" s="131"/>
+      <c r="E22" s="144"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="136" t="s">
-        <v>247</v>
-      </c>
-      <c r="B23" s="137">
-        <f>_xlfn.NORM.S.DIST(B12, TRUE)</f>
-        <v>0.73103875575403099</v>
-      </c>
-      <c r="C23" s="137">
-        <f>_xlfn.T.DIST(B13, (B9-1), TRUE)</f>
-        <v>0.72924949230545577</v>
+      <c r="A23" s="140" t="s">
+        <v>248</v>
+      </c>
+      <c r="B23" s="135">
+        <f>1-B22</f>
+        <v>0.14592027257189422</v>
+      </c>
+      <c r="C23" s="135">
+        <f>1-C22</f>
+        <v>0.1491637148302698</v>
       </c>
       <c r="D23" s="131"/>
+      <c r="F23" s="132"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="138" t="s">
-        <v>248</v>
-      </c>
-      <c r="B24" s="139">
-        <f>1-B23</f>
-        <v>0.26896124424596901</v>
-      </c>
-      <c r="C24" s="139">
-        <f>1-C23</f>
-        <v>0.27075050769454423</v>
+      <c r="A24" s="140" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" s="135">
+        <f>B11 * IF(B13 &gt; 0,  B23,  B22)</f>
+        <v>0.14592027257189422</v>
+      </c>
+      <c r="C24" s="135">
+        <f>B11 * IF(B13 &gt; 0, C23, C22)</f>
+        <v>0.1491637148302698</v>
       </c>
       <c r="D24" s="131"/>
-      <c r="F24" s="132"/>
+      <c r="E24" s="137"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="138" t="s">
-        <v>264</v>
-      </c>
-      <c r="B25" s="139" t="str">
-        <f>IF(B12&gt;0, "Right", "Left")</f>
-        <v>Right</v>
-      </c>
-      <c r="C25" s="139" t="str">
-        <f>IF(B13&gt;0, "Right", "Left")</f>
-        <v>Right</v>
-      </c>
-      <c r="D25" s="131"/>
+      <c r="A25" s="140" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="135" t="str">
+        <f>IF(B24 &gt; B10,  "Do not reject", "Reject")</f>
+        <v>Do not reject</v>
+      </c>
+      <c r="C25" s="135" t="str">
+        <f>IF(C24 &gt; B10, "Do not reject",  "Reject")</f>
+        <v>Do not reject</v>
+      </c>
+      <c r="D25" s="138"/>
       <c r="F25" s="132"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="138" t="s">
-        <v>249</v>
-      </c>
-      <c r="B26" s="135">
-        <f>B10*IF(B25="Right",B24,B23)</f>
-        <v>0.26896124424596901</v>
-      </c>
-      <c r="C26" s="135">
-        <f>B10 * IF(C25="Right", C24, C23)</f>
-        <v>0.27075050769454423</v>
-      </c>
-      <c r="D26" s="131"/>
-      <c r="E26" s="141"/>
+      <c r="C26" s="131"/>
+      <c r="F26" s="132"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="138" t="s">
-        <v>251</v>
-      </c>
-      <c r="B27" s="135" t="str">
-        <f>IF(B26&lt;B11, "Reject", "Do not reject")</f>
-        <v>Do not reject</v>
-      </c>
-      <c r="C27" s="135" t="str">
-        <f>IF(C26&lt;B11, "Reject", "Do not reject")</f>
-        <v>Do not reject</v>
-      </c>
-      <c r="D27" s="143"/>
+      <c r="A27" s="130"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="131"/>
       <c r="F27" s="132"/>
+      <c r="G27" s="132"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="130"/>
+      <c r="B28" s="136"/>
       <c r="C28" s="131"/>
       <c r="F28" s="132"/>
+      <c r="G28" s="132"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="130"/>
-      <c r="B29" s="140"/>
+      <c r="B29" s="136"/>
       <c r="C29" s="131"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="132"/>
       <c r="F29" s="132"/>
       <c r="G29" s="132"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="130"/>
-      <c r="B30" s="140"/>
-      <c r="C30" s="131"/>
-      <c r="F30" s="132"/>
-      <c r="G30" s="132"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="130"/>
-      <c r="B31" s="140"/>
-      <c r="C31" s="131"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
-      <c r="G31" s="132"/>
-    </row>
-    <row r="32" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A32" s="154" t="s">
+    <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A30" s="158" t="s">
         <v>246</v>
       </c>
-      <c r="B32" s="155"/>
-      <c r="C32" s="155"/>
-      <c r="D32" s="155"/>
-      <c r="E32" s="156"/>
-      <c r="F32" s="156"/>
-      <c r="G32" s="156"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
+  <conditionalFormatting sqref="B5:B6">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>$B$14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve probability values in probability distributions
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BA84B5-4533-404A-9CCC-A03114B94EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE458E01-464A-3A41-875E-89701A191F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
     <sheet name="Descriptive Statistics-2" sheetId="3" r:id="rId2"/>
     <sheet name="Probability Introduction" sheetId="4" r:id="rId3"/>
     <sheet name="Probability Distributions" sheetId="6" r:id="rId4"/>
-    <sheet name="Sampling &amp; Confidence Intervals" sheetId="8" r:id="rId5"/>
+    <sheet name="Confidence Intervals &amp; Sampling" sheetId="8" r:id="rId5"/>
     <sheet name="Hypothesis Tests" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="265">
   <si>
     <t>E</t>
   </si>
@@ -566,9 +566,6 @@
     <t>A176</t>
   </si>
   <si>
-    <t>Outcome</t>
-  </si>
-  <si>
     <t>Std Dev</t>
   </si>
   <si>
@@ -579,9 +576,6 @@
   </si>
   <si>
     <t>variance</t>
-  </si>
-  <si>
-    <t>Datatset</t>
   </si>
   <si>
     <t>Determine the expected monetary value​ (EMV) for the new product.</t>
@@ -827,9 +821,6 @@
     <t>5 largest</t>
   </si>
   <si>
-    <t>Normal Distribution Sampling</t>
-  </si>
-  <si>
     <t>sample std dev</t>
   </si>
   <si>
@@ -891,6 +882,18 @@
   </si>
   <si>
     <t>ZT test statistic proportion</t>
+  </si>
+  <si>
+    <t>Confidence Intervals &amp; Sampling Distributions</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1184,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1347,18 +1350,6 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1389,13 +1380,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1510,6 +1495,7 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1523,7 +1509,6 @@
     <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1540,6 +1525,32 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -12877,21 +12888,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="148">
+      <c r="C17" s="142">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="149"/>
+      <c r="D17" s="143"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="148">
+      <c r="C18" s="142">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="149"/>
+      <c r="D18" s="143"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -14796,7 +14807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O996"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -16956,10 +16967,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AD4EF6-892A-F84F-8FD1-A47C9BD9CBDB}">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16971,31 +16982,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
+      <c r="A1" s="144" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="79"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="79"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="103" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="103" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="102" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="102" t="s">
         <v>167</v>
-      </c>
-      <c r="B3" s="77" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="109" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="108" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="108" t="s">
-        <v>168</v>
       </c>
       <c r="F3" s="79"/>
       <c r="G3" s="80"/>
@@ -17005,20 +17020,20 @@
       <c r="A4" s="81">
         <v>1</v>
       </c>
-      <c r="B4" s="78">
-        <v>75</v>
-      </c>
-      <c r="C4" s="114">
+      <c r="B4" s="81">
+        <v>15</v>
+      </c>
+      <c r="C4" s="108">
         <f>B4/$B$9</f>
-        <v>0.75</v>
-      </c>
-      <c r="D4" s="125">
+        <v>0.1875</v>
+      </c>
+      <c r="D4" s="119">
         <f>A4*C4</f>
-        <v>0.75</v>
-      </c>
-      <c r="E4" s="125">
+        <v>0.1875</v>
+      </c>
+      <c r="E4" s="119">
         <f>((A4-$D$9)^2)*C4</f>
-        <v>3.2448000000000006</v>
+        <v>0.82687500000000003</v>
       </c>
       <c r="F4" s="79"/>
       <c r="G4" s="80"/>
@@ -17028,20 +17043,20 @@
       <c r="A5" s="81">
         <v>2</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="81">
         <v>13</v>
       </c>
-      <c r="C5" s="114">
+      <c r="C5" s="108">
         <f t="shared" ref="C5:C8" si="0">B5/$B$9</f>
-        <v>0.13</v>
-      </c>
-      <c r="D5" s="125">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="D5" s="119">
         <f t="shared" ref="D5:D8" si="1">A5*C5</f>
-        <v>0.26</v>
-      </c>
-      <c r="E5" s="125">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E5" s="119">
         <f t="shared" ref="E5:E8" si="2">((A5-$D$9)^2)*C5</f>
-        <v>0.15163200000000002</v>
+        <v>0.19662500000000005</v>
       </c>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
@@ -17051,20 +17066,20 @@
       <c r="A6" s="81">
         <v>3</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="81">
         <v>18</v>
       </c>
-      <c r="C6" s="114">
+      <c r="C6" s="108">
         <f t="shared" si="0"/>
-        <v>0.18</v>
-      </c>
-      <c r="D6" s="125">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="D6" s="119">
         <f t="shared" si="1"/>
-        <v>0.54</v>
-      </c>
-      <c r="E6" s="125">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E6" s="119">
         <f t="shared" si="2"/>
-        <v>1.152000000000002E-3</v>
+        <v>2.2500000000000042E-3</v>
       </c>
       <c r="F6" s="79"/>
       <c r="G6" s="79"/>
@@ -17074,20 +17089,20 @@
       <c r="A7" s="81">
         <v>4</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="81">
         <v>17</v>
       </c>
-      <c r="C7" s="114">
+      <c r="C7" s="108">
         <f t="shared" si="0"/>
-        <v>0.17</v>
-      </c>
-      <c r="D7" s="125">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="D7" s="119">
         <f t="shared" si="1"/>
-        <v>0.68</v>
-      </c>
-      <c r="E7" s="125">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="119">
         <f t="shared" si="2"/>
-        <v>0.14388799999999999</v>
+        <v>0.17212499999999997</v>
       </c>
       <c r="F7" s="79"/>
       <c r="G7" s="82"/>
@@ -17097,222 +17112,224 @@
       <c r="A8" s="81">
         <v>5</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="81">
         <v>17</v>
       </c>
-      <c r="C8" s="114">
+      <c r="C8" s="108">
         <f t="shared" si="0"/>
-        <v>0.17</v>
-      </c>
-      <c r="D8" s="125">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="D8" s="119">
         <f t="shared" si="1"/>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="E8" s="125">
+        <v>1.0625</v>
+      </c>
+      <c r="E8" s="119">
         <f t="shared" si="2"/>
-        <v>0.62668800000000002</v>
+        <v>0.76712499999999995</v>
       </c>
       <c r="F8" s="79"/>
       <c r="G8" s="82"/>
       <c r="H8" s="79"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="85">
-        <v>100</v>
-      </c>
-      <c r="C9" s="123">
+      <c r="A9" s="79"/>
+      <c r="B9" s="117">
+        <f>SUM(B4:B8)</f>
+        <v>80</v>
+      </c>
+      <c r="C9" s="117">
         <f t="shared" ref="C9" si="3">SUM(C4:C8)</f>
-        <v>1.4</v>
-      </c>
-      <c r="D9" s="125">
+        <v>1</v>
+      </c>
+      <c r="D9" s="119">
         <f>SUM(D4:D8)</f>
-        <v>3.08</v>
-      </c>
-      <c r="E9" s="125">
+        <v>3.1</v>
+      </c>
+      <c r="E9" s="119">
         <f>SQRT(SUM(E4:E8))</f>
-        <v>2.0416072100186167</v>
+        <v>1.4017845768876187</v>
       </c>
       <c r="F9" s="79"/>
       <c r="G9" s="82"/>
       <c r="H9" s="79"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
       <c r="F10" s="79"/>
       <c r="G10" s="82"/>
       <c r="H10" s="79"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
       <c r="F11" s="79"/>
       <c r="G11" s="82"/>
       <c r="H11" s="79"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
       <c r="F12" s="79"/>
       <c r="G12" s="82"/>
       <c r="H12" s="79"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
       <c r="F13" s="79"/>
       <c r="G13" s="82"/>
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="155" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" s="155"/>
-      <c r="C14" s="155"/>
-      <c r="D14" s="155"/>
-      <c r="E14" s="155"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="155"/>
+      <c r="A14" s="144" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="144"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="144"/>
+      <c r="F14" s="144"/>
+      <c r="G14" s="144"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="79"/>
       <c r="G15" s="82"/>
       <c r="H15" s="79"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="83" t="s">
-        <v>191</v>
+      <c r="A16" s="106" t="s">
+        <v>189</v>
       </c>
       <c r="B16" s="83">
         <v>20</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
       <c r="F16" s="79"/>
       <c r="G16" s="82"/>
       <c r="H16" s="79"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="83" t="s">
-        <v>192</v>
-      </c>
-      <c r="B17" s="95">
+      <c r="A17" s="106" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" s="91">
         <v>42</v>
       </c>
-      <c r="C17" s="93"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="79"/>
       <c r="G17" s="82"/>
       <c r="H17" s="79"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="83" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="88">
+      <c r="A18" s="106" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="119">
         <f>1/(B17-B16)</f>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="94"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
       <c r="F18" s="79"/>
       <c r="G18" s="82"/>
       <c r="H18" s="79"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="83" t="s">
+      <c r="A19" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="86">
+      <c r="B19" s="164">
         <f>(B17+B16)/2</f>
         <v>31</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
       <c r="F19" s="79"/>
       <c r="G19" s="82"/>
       <c r="H19" s="79"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="83" t="s">
-        <v>170</v>
-      </c>
-      <c r="B20" s="86">
+      <c r="A20" s="106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="164">
         <f>(B17-B16)/SQRT(12)</f>
         <v>6.3508529610858835</v>
       </c>
-      <c r="C20" s="93"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
       <c r="F20" s="79"/>
       <c r="G20" s="82"/>
       <c r="H20" s="79"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="93"/>
-      <c r="C21" s="97" t="s">
-        <v>205</v>
-      </c>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="93" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
       <c r="F21" s="79"/>
       <c r="G21" s="82"/>
       <c r="H21" s="79"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="103" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="103" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="77" t="s">
-        <v>182</v>
-      </c>
-      <c r="C22" s="109" t="s">
-        <v>189</v>
-      </c>
-      <c r="D22" s="94"/>
-      <c r="E22" s="124" t="s">
-        <v>200</v>
-      </c>
-      <c r="F22" s="124" t="s">
-        <v>203</v>
+      <c r="D22" s="90"/>
+      <c r="E22" s="118" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" s="118" t="s">
+        <v>201</v>
       </c>
       <c r="G22" s="82"/>
       <c r="H22" s="79"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="112" t="s">
-        <v>184</v>
+      <c r="A23" s="106" t="s">
+        <v>182</v>
       </c>
       <c r="B23" s="83">
         <v>24</v>
       </c>
-      <c r="C23" s="115">
+      <c r="C23" s="109">
         <f>$B$18*0</f>
         <v>0</v>
       </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="124">
+      <c r="D23" s="90"/>
+      <c r="E23" s="156">
         <v>70</v>
       </c>
-      <c r="F23" s="113">
+      <c r="F23" s="107">
         <f>((E23/100)/B18) + B16</f>
         <v>35.4</v>
       </c>
@@ -17320,13 +17337,13 @@
       <c r="H23" s="79"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="116" t="s">
-        <v>185</v>
+      <c r="A24" s="110" t="s">
+        <v>263</v>
       </c>
       <c r="B24" s="83">
         <v>31</v>
       </c>
-      <c r="C24" s="115">
+      <c r="C24" s="109">
         <f>$B$18*(B24-B16)</f>
         <v>0.5</v>
       </c>
@@ -17335,13 +17352,13 @@
       <c r="H24" s="79"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="112" t="s">
-        <v>186</v>
+      <c r="A25" s="106" t="s">
+        <v>264</v>
       </c>
       <c r="B25" s="83">
         <v>28</v>
       </c>
-      <c r="C25" s="115">
+      <c r="C25" s="109">
         <f>$B$18*($B$17-B25)</f>
         <v>0.63636363636363635</v>
       </c>
@@ -17350,13 +17367,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="151" t="s">
-        <v>201</v>
+      <c r="A26" s="146" t="s">
+        <v>199</v>
       </c>
       <c r="B26" s="83">
         <v>29</v>
       </c>
-      <c r="C26" s="153">
+      <c r="C26" s="148">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17365,11 +17382,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="152"/>
+      <c r="A27" s="147"/>
       <c r="B27" s="81">
         <v>37</v>
       </c>
-      <c r="C27" s="154"/>
+      <c r="C27" s="149"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17385,15 +17402,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="150" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" s="150"/>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
+      <c r="A30" s="145" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" s="145"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17402,22 +17419,22 @@
       <c r="H31" s="79"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="83" t="s">
+      <c r="A32" s="106" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="84">
-        <v>692</v>
+        <v>16.3</v>
       </c>
       <c r="F32" s="79"/>
       <c r="G32" s="82"/>
       <c r="H32" s="79"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="83" t="s">
-        <v>170</v>
+      <c r="A33" s="106" t="s">
+        <v>169</v>
       </c>
       <c r="B33" s="84">
-        <v>49</v>
+        <v>4.2</v>
       </c>
       <c r="C33" s="79"/>
       <c r="F33" s="79"/>
@@ -17425,8 +17442,8 @@
       <c r="H33" s="79"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="83" t="s">
-        <v>237</v>
+      <c r="A34" s="106" t="s">
+        <v>235</v>
       </c>
       <c r="B34" s="84">
         <v>1</v>
@@ -17445,648 +17462,632 @@
       <c r="H35" s="79"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="103" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="103" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="77" t="s">
+      <c r="E36" s="118" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="118" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36" s="82"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="106" t="s">
         <v>182</v>
-      </c>
-      <c r="C36" s="109" t="s">
-        <v>189</v>
-      </c>
-      <c r="E36" s="124" t="s">
-        <v>200</v>
-      </c>
-      <c r="F36" s="124" t="s">
-        <v>204</v>
-      </c>
-      <c r="G36" s="82"/>
-      <c r="H36" s="79"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="112" t="s">
-        <v>184</v>
       </c>
       <c r="B37" s="83">
         <v>170</v>
       </c>
-      <c r="C37" s="115">
+      <c r="C37" s="109">
         <f>_xlfn.NORM.DIST(B37,$B$32,$B$33,FALSE)</f>
-        <v>1.849993181041472E-27</v>
-      </c>
-      <c r="E37" s="124">
-        <v>35</v>
-      </c>
-      <c r="F37" s="113">
+        <v>1.4845303686723813E-292</v>
+      </c>
+      <c r="E37" s="156">
+        <v>99.7</v>
+      </c>
+      <c r="F37" s="107">
         <f>_xlfn.NORM.INV(E37/100, B32, B33)</f>
-        <v>673.11929714602923</v>
+        <v>27.840681818868966</v>
       </c>
       <c r="G37" s="82"/>
-      <c r="H37" s="79"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="116" t="s">
-        <v>185</v>
+      <c r="A38" s="110" t="s">
+        <v>263</v>
       </c>
       <c r="B38" s="83">
         <v>170</v>
       </c>
-      <c r="C38" s="115">
+      <c r="C38" s="109">
         <f>_xlfn.NORM.DIST(B38,$B$32,$B$33,TRUE)</f>
-        <v>8.4361799794053529E-27</v>
-      </c>
-      <c r="E38" s="123" t="s">
-        <v>235</v>
-      </c>
-      <c r="F38" s="113">
+        <v>1</v>
+      </c>
+      <c r="E38" s="117" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" s="107">
         <f>B32 - (B34 * B33)</f>
-        <v>643</v>
+        <v>12.100000000000001</v>
       </c>
       <c r="G38" s="82"/>
-      <c r="H38" s="79"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="112" t="s">
-        <v>186</v>
+      <c r="A39" s="106" t="s">
+        <v>264</v>
       </c>
       <c r="B39" s="83">
-        <v>2300</v>
-      </c>
-      <c r="C39" s="115">
+        <v>3</v>
+      </c>
+      <c r="C39" s="109">
         <f>(1-_xlfn.NORM.DIST(B39,$B$32,$B$33,TRUE))</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="91"/>
-      <c r="E39" s="119" t="s">
-        <v>236</v>
-      </c>
-      <c r="F39" s="113">
+        <v>0.99922901521552998</v>
+      </c>
+      <c r="D39" s="87"/>
+      <c r="E39" s="113" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="107">
         <f>B32 + (B34 * B33)</f>
-        <v>741</v>
+        <v>20.5</v>
       </c>
       <c r="G39" s="82"/>
-      <c r="H39" s="79"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="151" t="s">
-        <v>201</v>
+      <c r="A40" s="146" t="s">
+        <v>199</v>
       </c>
       <c r="B40" s="83">
-        <v>3300</v>
-      </c>
-      <c r="C40" s="153">
+        <v>14</v>
+      </c>
+      <c r="C40" s="148">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="91"/>
+        <v>0.44786484587392167</v>
+      </c>
+      <c r="F40" s="87"/>
       <c r="G40" s="82"/>
-      <c r="H40" s="79"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="152"/>
+      <c r="A41" s="147"/>
       <c r="B41" s="81">
-        <v>4200</v>
-      </c>
-      <c r="C41" s="154"/>
+        <v>19</v>
+      </c>
+      <c r="C41" s="149"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="93"/>
+      <c r="A42" s="89"/>
       <c r="B42" s="79"/>
-      <c r="C42" s="96"/>
+      <c r="C42" s="92"/>
       <c r="F42" s="79"/>
       <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="93"/>
+      <c r="A43" s="89"/>
       <c r="B43" s="79"/>
-      <c r="C43" s="96"/>
+      <c r="C43" s="92"/>
       <c r="F43" s="79"/>
       <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F44" s="79"/>
       <c r="G44" s="79"/>
-      <c r="H44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="150" t="s">
-        <v>196</v>
-      </c>
-      <c r="B46" s="150"/>
-      <c r="C46" s="150"/>
-      <c r="D46" s="150"/>
-      <c r="E46" s="150"/>
-      <c r="F46" s="150"/>
-      <c r="G46" s="150"/>
+      <c r="A46" s="145" t="s">
+        <v>194</v>
+      </c>
+      <c r="B46" s="145"/>
+      <c r="C46" s="145"/>
+      <c r="D46" s="145"/>
+      <c r="E46" s="145"/>
+      <c r="F46" s="145"/>
+      <c r="G46" s="145"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="83" t="s">
+      <c r="A48" s="106" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="83">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="83">
+      <c r="B49" s="83">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="83" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="106">
+        <f>B49*B48</f>
+        <v>6.6499999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="B51" s="106">
+        <f>B49*(1-B48)*B48</f>
+        <v>0.3325000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="B49" s="83">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="83" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="83">
-        <f>B48*B49</f>
-        <v>6.6499999999999995</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="B51" s="83">
-        <f>B48*(1-B49)*B49</f>
-        <v>0.3325000000000003</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="83" t="s">
-        <v>170</v>
-      </c>
-      <c r="B52" s="84">
+      <c r="B52" s="110">
         <f>SQRT(B51)</f>
         <v>0.57662812973354005</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="109" t="s">
-        <v>187</v>
-      </c>
-      <c r="B54" s="77" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="163"/>
+      <c r="B53" s="86"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="103" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="103" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="C54" s="109" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="112" t="s">
-        <v>184</v>
-      </c>
-      <c r="B55" s="83">
+      <c r="B56" s="83">
         <v>6</v>
       </c>
-      <c r="C55" s="115">
-        <f>_xlfn.BINOM.DIST(B55,$B$48,$B$49,FALSE)</f>
+      <c r="C56" s="109">
+        <f>_xlfn.BINOM.DIST(B56,$B$49,$B$48,FALSE)</f>
         <v>0.25728216171875024</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="116" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="B57" s="83">
+        <v>2</v>
+      </c>
+      <c r="C57" s="109">
+        <f>_xlfn.BINOM.DIST(B57, $B$49, $B$48, TRUE)</f>
+        <v>6.0273437500000207E-6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="106" t="s">
+        <v>264</v>
+      </c>
+      <c r="B58" s="83">
+        <v>6</v>
+      </c>
+      <c r="C58" s="109">
+        <f>1 - _xlfn.BINOM.DIST(B58,$B$49,$B$48,TRUE)</f>
+        <v>0.69833729609374973</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="146" t="s">
+        <v>199</v>
+      </c>
+      <c r="B59" s="83">
+        <v>2</v>
+      </c>
+      <c r="C59" s="148">
+        <f>_xlfn.BINOM.DIST(B60,$B$49,$B$48,TRUE) - _xlfn.BINOM.DIST(B59,$B$49,$B$48,TRUE)</f>
+        <v>0.30165667656250023</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="147"/>
+      <c r="B60" s="81">
+        <v>6</v>
+      </c>
+      <c r="C60" s="149"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="89"/>
+      <c r="B61" s="79"/>
+      <c r="C61" s="92"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="89"/>
+      <c r="B62" s="79"/>
+      <c r="C62" s="92"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="80"/>
+      <c r="B63" s="80"/>
+      <c r="C63" s="87"/>
+    </row>
+    <row r="65" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A65" s="145" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="145"/>
+      <c r="C65" s="145"/>
+      <c r="D65" s="145"/>
+      <c r="E65" s="145"/>
+      <c r="F65" s="145"/>
+      <c r="G65" s="145"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="106" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="84">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" s="108">
+        <f>SQRT(B67)</f>
+        <v>1.8439088914585775</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="B56" s="83">
+      <c r="B70" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="103" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="83">
+        <v>5</v>
+      </c>
+      <c r="C71" s="109">
+        <f>_xlfn.POISSON.DIST(B71,$B$67,FALSE)</f>
+        <v>0.12636072257615658</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="B72" s="83">
+        <v>3</v>
+      </c>
+      <c r="C72" s="109">
+        <f>_xlfn.POISSON.DIST(B72,$B$67,TRUE)</f>
+        <v>0.55835705528289536</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="106" t="s">
+        <v>264</v>
+      </c>
+      <c r="B73" s="83">
+        <v>6</v>
+      </c>
+      <c r="C73" s="109">
+        <f>(1 - _xlfn.POISSON.DIST(B73,$B$67,TRUE))</f>
+        <v>5.78532206573662E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="146" t="s">
+        <v>199</v>
+      </c>
+      <c r="B74" s="83">
         <v>2</v>
       </c>
-      <c r="C56" s="115">
-        <f>_xlfn.BINOM.DIST(B56,$B$48,$B$49,TRUE)</f>
-        <v>6.0273437500000207E-6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="112" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" s="83">
-        <v>6</v>
-      </c>
-      <c r="C57" s="115">
-        <f>1 - _xlfn.BINOM.DIST(B57,$B$48,$B$49,TRUE)</f>
-        <v>0.69833729609374973</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="151" t="s">
-        <v>201</v>
-      </c>
-      <c r="B58" s="83">
-        <v>2</v>
-      </c>
-      <c r="C58" s="153">
-        <f>_xlfn.BINOM.DIST(B59,$B$48,$B$49,TRUE) - _xlfn.BINOM.DIST(B58,$B$48,$B$49,TRUE)</f>
-        <v>0.30165667656250023</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="152"/>
-      <c r="B59" s="81">
-        <v>6</v>
-      </c>
-      <c r="C59" s="154"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="93"/>
-      <c r="B60" s="79"/>
-      <c r="C60" s="96"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="93"/>
-      <c r="B61" s="79"/>
-      <c r="C61" s="96"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="80"/>
-      <c r="B62" s="80"/>
-      <c r="C62" s="91"/>
-    </row>
-    <row r="64" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A64" s="150" t="s">
-        <v>198</v>
-      </c>
-      <c r="B64" s="150"/>
-      <c r="C64" s="150"/>
-      <c r="D64" s="150"/>
-      <c r="E64" s="150"/>
-      <c r="F64" s="150"/>
-      <c r="G64" s="150"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="83" t="s">
-        <v>193</v>
-      </c>
-      <c r="B66" s="83">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="83" t="s">
-        <v>170</v>
-      </c>
-      <c r="B67" s="87">
-        <f>SQRT(B66)</f>
-        <v>3.8078865529319543</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="109" t="s">
-        <v>187</v>
-      </c>
-      <c r="B69" s="77" t="s">
-        <v>182</v>
-      </c>
-      <c r="C69" s="109" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="112" t="s">
-        <v>184</v>
-      </c>
-      <c r="B70" s="83">
+      <c r="C74" s="148">
+        <f>_xlfn.POISSON.DIST(B75,$B$67,TRUE) - _xlfn.POISSON.DIST(B74,$B$67,TRUE)</f>
+        <v>0.53080248168669208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="147"/>
+      <c r="B75" s="81">
         <v>5</v>
       </c>
-      <c r="C70" s="115">
-        <f>_xlfn.POISSON.DIST(B70,$B$66,FALSE)</f>
-        <v>2.6939453267530375E-3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="116" t="s">
-        <v>185</v>
-      </c>
-      <c r="B71" s="83">
-        <v>3</v>
-      </c>
-      <c r="C71" s="115">
-        <f>_xlfn.POISSON.DIST(B71,$B$66,TRUE)</f>
-        <v>3.1709808559658942E-4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="112" t="s">
-        <v>186</v>
-      </c>
-      <c r="B72" s="83">
-        <v>6</v>
-      </c>
-      <c r="C72" s="115">
-        <f>(1 - _xlfn.POISSON.DIST(B72,$B$66,TRUE))</f>
-        <v>0.9895496420502663</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="151" t="s">
-        <v>201</v>
-      </c>
-      <c r="B73" s="83">
-        <v>2</v>
-      </c>
-      <c r="C73" s="153">
-        <f>_xlfn.POISSON.DIST(B74,$B$66,TRUE) - _xlfn.POISSON.DIST(B73,$B$66,TRUE)</f>
-        <v>3.8791531399499785E-3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="152"/>
-      <c r="B74" s="81">
-        <v>5</v>
-      </c>
-      <c r="C74" s="154"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="93"/>
-      <c r="B75" s="79"/>
-      <c r="C75" s="96"/>
+      <c r="C75" s="149"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="93"/>
+      <c r="A76" s="89"/>
       <c r="B76" s="79"/>
-      <c r="C76" s="96"/>
+      <c r="C76" s="92"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="80"/>
-      <c r="B77" s="80"/>
-      <c r="C77" s="91"/>
+      <c r="A77" s="89"/>
+      <c r="B77" s="79"/>
+      <c r="C77" s="92"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="80"/>
       <c r="B78" s="80"/>
-      <c r="C78" s="91"/>
-    </row>
-    <row r="79" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A79" s="150" t="s">
-        <v>199</v>
-      </c>
-      <c r="B79" s="150"/>
-      <c r="C79" s="150"/>
-      <c r="D79" s="150"/>
-      <c r="E79" s="150"/>
-      <c r="F79" s="150"/>
-      <c r="G79" s="150"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B80" s="80"/>
-      <c r="C80" s="91"/>
+      <c r="C78" s="87"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="80"/>
+      <c r="B79" s="80"/>
+      <c r="C79" s="87"/>
+    </row>
+    <row r="80" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A80" s="145" t="s">
+        <v>197</v>
+      </c>
+      <c r="B80" s="145"/>
+      <c r="C80" s="145"/>
+      <c r="D80" s="145"/>
+      <c r="E80" s="145"/>
+      <c r="F80" s="145"/>
+      <c r="G80" s="145"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="83" t="s">
+      <c r="B81" s="80"/>
+      <c r="C81" s="87"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="B81" s="84">
+      <c r="B82" s="84">
         <f>6/5</f>
         <v>1.2</v>
       </c>
-      <c r="C81" s="91"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B82" s="80"/>
-      <c r="C82" s="91"/>
+      <c r="C82" s="87"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="109" t="s">
-        <v>187</v>
-      </c>
-      <c r="B83" s="77" t="s">
+      <c r="B83" s="80"/>
+      <c r="C83" s="87"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="103" t="s">
+        <v>185</v>
+      </c>
+      <c r="B84" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" s="103" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="C83" s="109" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="112" t="s">
-        <v>184</v>
-      </c>
-      <c r="B84" s="84">
+      <c r="B85" s="84">
         <v>1</v>
       </c>
-      <c r="C84" s="115">
-        <f>_xlfn.EXPON.DIST(B84,$B$81,FALSE)</f>
+      <c r="C85" s="109">
+        <f>_xlfn.EXPON.DIST(B85,$B$82,FALSE)</f>
         <v>0.36143305429464256</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="116" t="s">
-        <v>185</v>
-      </c>
-      <c r="B85" s="84">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="B86" s="84">
         <f>2.2/6</f>
         <v>0.3666666666666667</v>
       </c>
-      <c r="C85" s="115">
-        <f>_xlfn.EXPON.DIST(B85,$B$81,TRUE)</f>
+      <c r="C86" s="109">
+        <f>_xlfn.EXPON.DIST(B86,$B$82,TRUE)</f>
         <v>0.35596357891685859</v>
       </c>
-      <c r="E85" s="92"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="112" t="s">
-        <v>186</v>
-      </c>
-      <c r="B86" s="84">
+      <c r="E86" s="88"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="106" t="s">
+        <v>264</v>
+      </c>
+      <c r="B87" s="84">
         <f>2.7/6</f>
         <v>0.45</v>
       </c>
-      <c r="C86" s="115">
-        <f>1 - _xlfn.EXPON.DIST(B86,$B$81,TRUE)</f>
+      <c r="C87" s="109">
+        <f>1 - _xlfn.EXPON.DIST(B87,$B$82,TRUE)</f>
         <v>0.58274825237398964</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="151" t="s">
-        <v>201</v>
-      </c>
-      <c r="B87" s="84">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="146" t="s">
+        <v>199</v>
+      </c>
+      <c r="B88" s="84">
         <f>2.1/6</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="C87" s="153">
-        <f>_xlfn.EXPON.DIST(B88,$B$81,TRUE) - _xlfn.EXPON.DIST(B87,$B$81,TRUE)</f>
+      <c r="C88" s="148">
+        <f>_xlfn.EXPON.DIST(B89,$B$82,TRUE) - _xlfn.EXPON.DIST(B88,$B$82,TRUE)</f>
         <v>0.25047716007445753</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="152"/>
-      <c r="B88" s="81">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="147"/>
+      <c r="B89" s="81">
         <f>4.5/6</f>
         <v>0.75</v>
       </c>
-      <c r="C88" s="154"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="93"/>
-      <c r="B89" s="79"/>
-      <c r="C89" s="96"/>
+      <c r="C89" s="149"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="93"/>
+      <c r="A90" s="89"/>
       <c r="B90" s="79"/>
-      <c r="C90" s="96"/>
+      <c r="C90" s="92"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="93"/>
+      <c r="A91" s="89"/>
       <c r="B91" s="79"/>
-      <c r="C91" s="96"/>
+      <c r="C91" s="92"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="80"/>
-      <c r="B92" s="80"/>
-      <c r="C92" s="91"/>
-    </row>
-    <row r="93" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A93" s="150" t="s">
-        <v>181</v>
-      </c>
-      <c r="B93" s="150"/>
-      <c r="C93" s="150"/>
-      <c r="D93" s="150"/>
-      <c r="E93" s="150"/>
-      <c r="F93" s="150"/>
-      <c r="G93" s="150"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D94" s="75"/>
-      <c r="E94" s="75"/>
+      <c r="A92" s="89"/>
+      <c r="B92" s="79"/>
+      <c r="C92" s="92"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="80"/>
+      <c r="B93" s="80"/>
+      <c r="C93" s="87"/>
+    </row>
+    <row r="94" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A94" s="145" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" s="145"/>
+      <c r="C94" s="145"/>
+      <c r="D94" s="145"/>
+      <c r="E94" s="145"/>
+      <c r="F94" s="145"/>
+      <c r="G94" s="145"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="75" t="s">
-        <v>175</v>
-      </c>
+      <c r="D95" s="75"/>
+      <c r="E95" s="75"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="79" t="s">
-        <v>174</v>
-      </c>
-      <c r="B96" s="79"/>
-      <c r="C96" s="79"/>
-      <c r="D96" s="89"/>
-      <c r="E96" s="89"/>
-      <c r="F96" s="79"/>
+      <c r="A96" s="75" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="75" t="s">
-        <v>173</v>
+      <c r="A97" s="79" t="s">
+        <v>172</v>
       </c>
       <c r="B97" s="79"/>
       <c r="C97" s="79"/>
-      <c r="D97" s="89"/>
-      <c r="E97" s="89"/>
+      <c r="D97" s="85"/>
+      <c r="E97" s="85"/>
       <c r="F97" s="79"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="75" t="s">
+        <v>171</v>
+      </c>
       <c r="B98" s="79"/>
       <c r="C98" s="79"/>
-      <c r="D98" s="89"/>
-      <c r="E98" s="89"/>
+      <c r="D98" s="85"/>
+      <c r="E98" s="85"/>
       <c r="F98" s="79"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="78" t="s">
-        <v>206</v>
-      </c>
-      <c r="B99" s="78" t="s">
-        <v>176</v>
-      </c>
-      <c r="C99" s="108" t="s">
+      <c r="B99" s="79"/>
+      <c r="C99" s="79"/>
+      <c r="D99" s="85"/>
+      <c r="E99" s="85"/>
+      <c r="F99" s="79"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" s="102" t="s">
+        <v>174</v>
+      </c>
+      <c r="C100" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="D99" s="108" t="s">
-        <v>181</v>
-      </c>
-      <c r="E99" s="89"/>
-      <c r="F99" s="79"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="83" t="s">
-        <v>178</v>
-      </c>
-      <c r="B100" s="81">
-        <v>7000</v>
-      </c>
-      <c r="C100" s="113">
-        <v>0.3</v>
-      </c>
-      <c r="D100" s="108">
-        <f>B100*C100</f>
-        <v>2100</v>
-      </c>
+      <c r="D100" s="102" t="s">
+        <v>179</v>
+      </c>
+      <c r="E100" s="85"/>
+      <c r="F100" s="79"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="83" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B101" s="81">
-        <v>19000</v>
-      </c>
-      <c r="C101" s="113">
-        <v>0.45</v>
-      </c>
-      <c r="D101" s="108">
-        <f t="shared" ref="D101:D102" si="4">B101*C101</f>
-        <v>8550</v>
-      </c>
-      <c r="E101" s="89"/>
-      <c r="F101" s="79"/>
+        <v>7000</v>
+      </c>
+      <c r="C101" s="165">
+        <v>0.3</v>
+      </c>
+      <c r="D101" s="102">
+        <f>B101*C101</f>
+        <v>2100</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="83" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B102" s="81">
+        <v>19000</v>
+      </c>
+      <c r="C102" s="165">
+        <v>0.45</v>
+      </c>
+      <c r="D102" s="102">
+        <f t="shared" ref="D102:D103" si="4">B102*C102</f>
+        <v>8550</v>
+      </c>
+      <c r="E102" s="85"/>
+      <c r="F102" s="79"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="83" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="81">
         <v>37000</v>
       </c>
-      <c r="C102" s="113">
+      <c r="C103" s="165">
         <v>0.25</v>
       </c>
-      <c r="D102" s="108">
+      <c r="D103" s="102">
         <f t="shared" si="4"/>
         <v>9250</v>
       </c>
-      <c r="E102" s="89"/>
-      <c r="F102" s="79"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="79"/>
-      <c r="B103" s="79"/>
-      <c r="C103" s="79"/>
-      <c r="D103" s="108">
-        <f>SUM(D100:D102)</f>
-        <v>19900</v>
-      </c>
-      <c r="E103" s="89"/>
+      <c r="E103" s="85"/>
       <c r="F103" s="79"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="79"/>
       <c r="B104" s="79"/>
       <c r="C104" s="79"/>
-      <c r="D104" s="89"/>
-      <c r="E104" s="89"/>
+      <c r="D104" s="102">
+        <f>SUM(D101:D103)</f>
+        <v>19900</v>
+      </c>
+      <c r="E104" s="85"/>
       <c r="F104" s="79"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="79" t="s">
-        <v>207</v>
-      </c>
+      <c r="A105" s="79"/>
       <c r="B105" s="79"/>
       <c r="C105" s="79"/>
-      <c r="D105" s="79"/>
-      <c r="E105" s="79"/>
+      <c r="D105" s="85"/>
+      <c r="E105" s="85"/>
       <c r="F105" s="79"/>
-      <c r="G105" s="79"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="79" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B106" s="79"/>
       <c r="C106" s="79"/>
@@ -18097,7 +18098,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="79" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B107" s="79"/>
       <c r="C107" s="79"/>
@@ -18107,7 +18108,9 @@
       <c r="G107" s="79"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="99"/>
+      <c r="A108" s="79" t="s">
+        <v>207</v>
+      </c>
       <c r="B108" s="79"/>
       <c r="C108" s="79"/>
       <c r="D108" s="79"/>
@@ -18116,12 +18119,8 @@
       <c r="G108" s="79"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="83" t="s">
-        <v>210</v>
-      </c>
-      <c r="B109" s="98">
-        <v>4</v>
-      </c>
+      <c r="A109" s="95"/>
+      <c r="B109" s="79"/>
       <c r="C109" s="79"/>
       <c r="D109" s="79"/>
       <c r="E109" s="79"/>
@@ -18129,11 +18128,11 @@
       <c r="G109" s="79"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="83" t="s">
-        <v>211</v>
-      </c>
-      <c r="B110" s="98">
-        <v>7</v>
+      <c r="A110" s="106" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="94">
+        <v>4</v>
       </c>
       <c r="C110" s="79"/>
       <c r="D110" s="79"/>
@@ -18142,11 +18141,11 @@
       <c r="G110" s="79"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="B111" s="81">
-        <v>75</v>
+      <c r="A111" s="106" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" s="94">
+        <v>7</v>
       </c>
       <c r="C111" s="79"/>
       <c r="D111" s="79"/>
@@ -18155,12 +18154,11 @@
       <c r="G111" s="79"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="83" t="s">
-        <v>212</v>
-      </c>
-      <c r="B112" s="98">
-        <f>B111*B109</f>
-        <v>300</v>
+      <c r="A112" s="106" t="s">
+        <v>211</v>
+      </c>
+      <c r="B112" s="81">
+        <v>75</v>
       </c>
       <c r="C112" s="79"/>
       <c r="D112" s="79"/>
@@ -18168,93 +18166,119 @@
       <c r="F112" s="79"/>
       <c r="G112" s="79"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="78" t="s">
-        <v>206</v>
-      </c>
-      <c r="B114" s="78" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B113" s="94">
+        <f>B112*B110</f>
+        <v>300</v>
+      </c>
+      <c r="C113" s="79"/>
+      <c r="D113" s="79"/>
+      <c r="E113" s="79"/>
+      <c r="F113" s="79"/>
+      <c r="G113" s="79"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B115" s="102" t="s">
+        <v>175</v>
+      </c>
+      <c r="C115" s="102" t="s">
+        <v>109</v>
+      </c>
+      <c r="D115" s="102" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="B116" s="81">
+        <v>25</v>
+      </c>
+      <c r="C116" s="107">
+        <v>0.35</v>
+      </c>
+      <c r="D116" s="120">
+        <f>C116*($B$111*MIN($B$112, B116) - $B$113)</f>
+        <v>-43.75</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="C114" s="108" t="s">
-        <v>109</v>
-      </c>
-      <c r="D114" s="108" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="83" t="s">
+      <c r="B117" s="81">
+        <v>50</v>
+      </c>
+      <c r="C117" s="107">
+        <v>0.2</v>
+      </c>
+      <c r="D117" s="120">
+        <f t="shared" ref="D117:D118" si="5">C117*($B$111*MIN($B$112, B117) - $B$113)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="83" t="s">
         <v>178</v>
       </c>
-      <c r="B115" s="81">
-        <v>25</v>
-      </c>
-      <c r="C115" s="113">
-        <v>0.35</v>
-      </c>
-      <c r="D115" s="126">
-        <f>C115*($B$110*MIN($B$111, B115) - $B$112)</f>
-        <v>-43.75</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="83" t="s">
-        <v>179</v>
-      </c>
-      <c r="B116" s="81">
-        <v>50</v>
-      </c>
-      <c r="C116" s="113">
-        <v>0.2</v>
-      </c>
-      <c r="D116" s="126">
-        <f t="shared" ref="D116:D117" si="5">C116*($B$110*MIN($B$111, B116) - $B$112)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="83" t="s">
-        <v>180</v>
-      </c>
-      <c r="B117" s="81">
+      <c r="B118" s="81">
         <v>75</v>
       </c>
-      <c r="C117" s="113">
+      <c r="C118" s="107">
         <v>0.45</v>
       </c>
-      <c r="D117" s="126">
+      <c r="D118" s="120">
         <f t="shared" si="5"/>
         <v>101.25</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="79"/>
-      <c r="B118" s="79"/>
-      <c r="C118" s="79"/>
-      <c r="D118" s="127">
-        <f>SUM(D115:D117)</f>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="79"/>
+      <c r="B119" s="79"/>
+      <c r="C119" s="79"/>
+      <c r="D119" s="121">
+        <f>SUM(D116:D118)</f>
         <v>67.5</v>
       </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="79"/>
+      <c r="B120" s="79"/>
+      <c r="C120" s="79"/>
+      <c r="F120" s="76"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" s="79"/>
+      <c r="B121" s="79"/>
+      <c r="C121" s="79"/>
+      <c r="F121" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A80:G80"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A65:G65"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="A79:G79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18266,7 +18290,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18277,285 +18301,298 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
+      <c r="A1" s="145" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="107" t="s">
-        <v>238</v>
-      </c>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="160" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="102">
+      <c r="D3" s="98">
         <f>AVERAGE(A4:A23)</f>
         <v>34.6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="103">
+      <c r="A4" s="158">
         <v>25</v>
       </c>
-      <c r="B4" s="107" cm="1">
+      <c r="B4" s="77" cm="1">
         <f t="array" ref="B4:B23">_xlfn._xlws.SORT(A4:A23)</f>
         <v>5</v>
       </c>
-      <c r="C4" s="107"/>
+      <c r="C4" s="124"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="103">
+      <c r="A5" s="158">
         <v>20</v>
       </c>
-      <c r="B5" s="107">
+      <c r="B5" s="77">
         <v>10</v>
       </c>
-      <c r="C5" s="108" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" s="109" t="s">
-        <v>233</v>
-      </c>
-      <c r="E5" s="108" t="s">
-        <v>216</v>
+      <c r="C5" s="157" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>231</v>
+      </c>
+      <c r="E5" s="102" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="103">
+      <c r="A6" s="158">
         <v>5</v>
       </c>
-      <c r="B6" s="107">
+      <c r="B6" s="77">
         <v>15</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="161">
         <v>5</v>
       </c>
-      <c r="D6" s="110">
+      <c r="D6" s="104">
         <f>AVERAGE(A4:A8)</f>
         <v>20</v>
       </c>
-      <c r="E6" s="111">
+      <c r="E6" s="105">
         <f>D6-$D$3</f>
         <v>-14.600000000000001</v>
       </c>
-      <c r="F6" s="104"/>
+      <c r="F6" s="99"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="103">
+      <c r="A7" s="158">
         <v>17</v>
       </c>
-      <c r="B7" s="107">
+      <c r="B7" s="77">
         <v>17</v>
       </c>
-      <c r="C7" s="109">
+      <c r="C7" s="162">
         <v>10</v>
       </c>
-      <c r="D7" s="110">
+      <c r="D7" s="104">
         <f>AVERAGE(A4:A13)</f>
         <v>28.8</v>
       </c>
-      <c r="E7" s="111">
+      <c r="E7" s="105">
         <f>D7-$D$3</f>
         <v>-5.8000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="103">
+      <c r="A8" s="158">
         <v>33</v>
       </c>
-      <c r="B8" s="107">
+      <c r="B8" s="77">
         <v>20</v>
       </c>
+      <c r="C8" s="79"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="103">
+      <c r="A9" s="158">
         <v>20</v>
       </c>
-      <c r="B9" s="107">
+      <c r="B9" s="77">
         <v>20</v>
       </c>
-      <c r="C9" s="108" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="109" t="s">
-        <v>233</v>
-      </c>
-      <c r="E9" s="108" t="s">
-        <v>216</v>
+      <c r="C9" s="157" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" s="102" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="103">
+      <c r="A10" s="158">
         <v>41</v>
       </c>
-      <c r="B10" s="107">
+      <c r="B10" s="77">
         <v>20</v>
       </c>
-      <c r="C10" s="108" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="110">
+      <c r="C10" s="161" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="104">
         <f>AVERAGE(B4:B8)</f>
         <v>13.4</v>
       </c>
-      <c r="E10" s="111">
+      <c r="E10" s="105">
         <f>D10-$D$3</f>
         <v>-21.200000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="103">
+      <c r="A11" s="158">
         <v>53</v>
       </c>
-      <c r="B11" s="107">
+      <c r="B11" s="77">
         <v>24</v>
       </c>
-      <c r="C11" s="109" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" s="110">
+      <c r="C11" s="162" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="104">
         <f>AVERAGE(B19:B23)</f>
         <v>58.8</v>
       </c>
-      <c r="E11" s="111">
+      <c r="E11" s="105">
         <f>D11-$D$3</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="103">
+      <c r="A12" s="158">
         <v>50</v>
       </c>
-      <c r="B12" s="107">
+      <c r="B12" s="77">
         <v>25</v>
       </c>
-      <c r="D12" s="112" t="s">
-        <v>239</v>
-      </c>
-      <c r="E12" s="113">
+      <c r="C12" s="79"/>
+      <c r="D12" s="106" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" s="107">
         <f>MAX(ABS(E10), ABS(E11))</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="103">
+      <c r="A13" s="158">
         <v>24</v>
       </c>
-      <c r="B13" s="107">
+      <c r="B13" s="77">
         <v>33</v>
       </c>
+      <c r="C13" s="79"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="103">
+      <c r="A14" s="158">
         <v>41</v>
       </c>
-      <c r="B14" s="107">
+      <c r="B14" s="77">
         <v>36</v>
       </c>
+      <c r="C14" s="79"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="103">
+      <c r="A15" s="158">
         <v>52</v>
       </c>
-      <c r="B15" s="107">
+      <c r="B15" s="77">
         <v>41</v>
       </c>
+      <c r="C15" s="79"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="103">
+      <c r="A16" s="158">
         <v>47</v>
       </c>
-      <c r="B16" s="107">
+      <c r="B16" s="77">
         <v>41</v>
       </c>
+      <c r="C16" s="79"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="103">
+      <c r="A17" s="158">
         <v>15</v>
       </c>
-      <c r="B17" s="107">
+      <c r="B17" s="77">
         <v>44</v>
       </c>
+      <c r="C17" s="79"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="103">
+      <c r="A18" s="158">
         <v>44</v>
       </c>
-      <c r="B18" s="107">
+      <c r="B18" s="77">
         <v>47</v>
       </c>
+      <c r="C18" s="79"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="105">
+      <c r="A19" s="159">
         <v>10</v>
       </c>
-      <c r="B19" s="107">
+      <c r="B19" s="77">
         <v>50</v>
       </c>
+      <c r="C19" s="79"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="76">
+      <c r="A20" s="78">
         <v>36</v>
       </c>
-      <c r="B20" s="107">
+      <c r="B20" s="77">
         <v>52</v>
       </c>
+      <c r="C20" s="79"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="76">
+      <c r="A21" s="78">
         <v>60</v>
       </c>
-      <c r="B21" s="107">
+      <c r="B21" s="77">
         <v>53</v>
       </c>
+      <c r="C21" s="79"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="76">
+      <c r="A22" s="78">
         <v>20</v>
       </c>
-      <c r="B22" s="107">
+      <c r="B22" s="77">
         <v>60</v>
       </c>
+      <c r="C22" s="79"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="76">
+      <c r="A23" s="78">
         <v>79</v>
       </c>
-      <c r="B23" s="107">
+      <c r="B23" s="77">
         <v>79</v>
       </c>
+      <c r="C23" s="79"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="107"/>
+      <c r="B24" s="101"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="107"/>
+      <c r="B25" s="101"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="107"/>
+      <c r="B26" s="101"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="107"/>
+      <c r="B27" s="101"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="150" t="s">
-        <v>242</v>
-      </c>
-      <c r="B28" s="150"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="150"/>
-      <c r="G28" s="150"/>
+      <c r="A28" s="145" t="s">
+        <v>261</v>
+      </c>
+      <c r="B28" s="145"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D29" s="76"/>
@@ -18564,18 +18601,18 @@
       <c r="G29" s="82"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="83" t="s">
+      <c r="A30" s="106" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="84">
-        <v>13</v>
+        <v>393.5</v>
       </c>
       <c r="D30" s="76"/>
       <c r="G30" s="82"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="83" t="s">
-        <v>233</v>
+      <c r="A31" s="106" t="s">
+        <v>231</v>
       </c>
       <c r="B31" s="84">
         <v>1</v>
@@ -18584,8 +18621,8 @@
       <c r="G31" s="82"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="83" t="s">
-        <v>170</v>
+      <c r="A32" s="106" t="s">
+        <v>169</v>
       </c>
       <c r="B32" s="84">
         <v>5.6</v>
@@ -18594,45 +18631,45 @@
       <c r="G32" s="82"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="83" t="s">
-        <v>243</v>
+      <c r="A33" s="106" t="s">
+        <v>240</v>
       </c>
       <c r="B33" s="84">
-        <v>14.3</v>
+        <v>50.3</v>
       </c>
       <c r="D33" s="76"/>
       <c r="G33" s="82"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="83" t="s">
-        <v>222</v>
+      <c r="A34" s="106" t="s">
+        <v>220</v>
       </c>
       <c r="B34" s="84">
         <v>0.5</v>
       </c>
       <c r="D34" s="76"/>
       <c r="E34" s="80"/>
-      <c r="F34" s="90"/>
+      <c r="F34" s="86"/>
       <c r="G34" s="82"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="83" t="s">
-        <v>234</v>
+      <c r="A35" s="106" t="s">
+        <v>232</v>
       </c>
       <c r="B35" s="84">
         <v>1</v>
       </c>
       <c r="D35" s="76"/>
       <c r="E35" s="80"/>
-      <c r="F35" s="90"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="82"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="83" t="s">
-        <v>215</v>
+      <c r="A36" s="106" t="s">
+        <v>213</v>
       </c>
       <c r="B36" s="84">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D36" s="76"/>
       <c r="E36" s="76"/>
@@ -18640,8 +18677,8 @@
       <c r="G36" s="82"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="83" t="s">
-        <v>223</v>
+      <c r="A37" s="106" t="s">
+        <v>221</v>
       </c>
       <c r="B37" s="84">
         <v>100</v>
@@ -18652,14 +18689,14 @@
       <c r="G37" s="82"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="83" t="s">
-        <v>228</v>
-      </c>
-      <c r="B38" s="100">
+      <c r="A38" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="B38" s="96">
         <v>0.8</v>
       </c>
       <c r="D38" s="76"/>
-      <c r="E38" s="101"/>
+      <c r="E38" s="97"/>
       <c r="F38" s="79"/>
       <c r="G38" s="82"/>
     </row>
@@ -18673,58 +18710,58 @@
       <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="112" t="s">
+      <c r="A40" s="106" t="s">
+        <v>222</v>
+      </c>
+      <c r="B40" s="111">
+        <f>B32/SQRT(B36)</f>
+        <v>1.1199999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="106" t="s">
         <v>224</v>
       </c>
-      <c r="B40" s="117">
-        <f>B32/SQRT(B36)</f>
-        <v>1.252198067399882</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="112" t="s">
-        <v>226</v>
-      </c>
-      <c r="B41" s="117">
+      <c r="B41" s="111">
         <f>SQRT(B34*(1-B34)/B36)</f>
-        <v>0.11180339887498948</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="118" t="s">
-        <v>227</v>
-      </c>
-      <c r="B42" s="119">
+      <c r="A42" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="B42" s="113">
         <f>B41 *  SQRT((B37-B36)/(B37-1))</f>
-        <v>0.1005037815259212</v>
+        <v>8.7038827977848926E-2</v>
       </c>
       <c r="G42" s="82"/>
     </row>
     <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="118" t="s">
-        <v>230</v>
-      </c>
-      <c r="B43" s="119">
+      <c r="A43" s="112" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="113">
         <f>(B31-B30)/(B32/SQRT(B36))</f>
-        <v>-9.5831484749991009</v>
+        <v>-350.44642857142861</v>
       </c>
       <c r="G43" s="82"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="112" t="s">
-        <v>220</v>
-      </c>
-      <c r="B44" s="120">
+      <c r="A44" s="106" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" s="114">
         <f>(1-B38)/2</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="G44" s="82"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="112" t="s">
-        <v>221</v>
-      </c>
-      <c r="B45" s="121">
+      <c r="A45" s="106" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" s="115">
         <f>B38+B44</f>
         <v>0.9</v>
       </c>
@@ -18737,184 +18774,184 @@
       <c r="G47" s="82"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="109"/>
-      <c r="B48" s="77" t="s">
+      <c r="A48" s="103"/>
+      <c r="B48" s="103" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="103" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="103" t="s">
+        <v>223</v>
+      </c>
+      <c r="E48" s="103" t="s">
+        <v>230</v>
+      </c>
+      <c r="F48" s="100"/>
+      <c r="G48" s="79"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="C48" s="109" t="s">
-        <v>231</v>
-      </c>
-      <c r="D48" s="109" t="s">
-        <v>225</v>
-      </c>
-      <c r="E48" s="109" t="s">
-        <v>232</v>
-      </c>
-      <c r="F48" s="106"/>
-      <c r="G48" s="79"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="112" t="s">
+      <c r="B49" s="122">
+        <v>1</v>
+      </c>
+      <c r="C49" s="109">
+        <f>_xlfn.NORM.DIST(B49, $B$30, $B$40,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="109">
+        <f>_xlfn.NORM.DIST(B49, $B$34, $B$41, FALSE)</f>
+        <v>1.4867195147342977E-5</v>
+      </c>
+      <c r="E49" s="109">
+        <f>_xlfn.NORM.DIST(B49/$B$36, $B$34, $B$42,FALSE)</f>
+        <v>3.9447003166566339E-6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="110" t="s">
+        <v>183</v>
+      </c>
+      <c r="B50" s="122">
+        <v>1</v>
+      </c>
+      <c r="C50" s="109">
+        <f>_xlfn.NORM.DIST(B50, $B$30, $B$40,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="109">
+        <f>_xlfn.NORM.DIST(B50, $B$34, $B$41, TRUE)</f>
+        <v>0.99999971334842808</v>
+      </c>
+      <c r="E50" s="109">
+        <f>_xlfn.NORM.DIST(B50/$B$36, $B$34, $B$42,TRUE)</f>
+        <v>6.2853190747001746E-8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="106" t="s">
         <v>184</v>
       </c>
-      <c r="B49" s="128">
+      <c r="B51" s="122">
         <v>1</v>
       </c>
-      <c r="C49" s="115">
-        <f>_xlfn.NORM.DIST(B49, $B$30, $B$40,FALSE)</f>
-        <v>3.6403528427324646E-21</v>
-      </c>
-      <c r="D49" s="115">
-        <f>_xlfn.NORM.DIST(B49, $B$34, $B$41, FALSE)</f>
-        <v>1.6199821912178208E-4</v>
-      </c>
-      <c r="E49" s="115">
-        <f>_xlfn.NORM.DIST(B49/$B$36, $B$34, $B$42,FALSE)</f>
-        <v>1.7598204095915145E-4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="116" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" s="128">
-        <v>1</v>
-      </c>
-      <c r="C50" s="115">
-        <f>_xlfn.NORM.DIST(B50, $B$30, $B$40,TRUE)</f>
-        <v>4.7065385071790097E-22</v>
-      </c>
-      <c r="D50" s="115">
-        <f>_xlfn.NORM.DIST(B50, $B$34, $B$41, TRUE)</f>
-        <v>0.99999612789178449</v>
-      </c>
-      <c r="E50" s="115">
-        <f>_xlfn.NORM.DIST(B50/$B$36, $B$34, $B$42,TRUE)</f>
-        <v>3.7771111457593937E-6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="112" t="s">
-        <v>186</v>
-      </c>
-      <c r="B51" s="128">
-        <v>1</v>
-      </c>
-      <c r="C51" s="115">
+      <c r="C51" s="109">
         <f>(1-_xlfn.NORM.DIST(B51, $B$30, $B$40,TRUE))</f>
         <v>1</v>
       </c>
-      <c r="D51" s="115">
+      <c r="D51" s="109">
         <f>1 - _xlfn.NORM.DIST(B51, $B$34, $B$41, TRUE)</f>
-        <v>3.8721082155079856E-6</v>
-      </c>
-      <c r="E51" s="115">
+        <v>2.8665157192353519E-7</v>
+      </c>
+      <c r="E51" s="109">
         <f>1 - _xlfn.NORM.DIST(B51/$B$36, $B$34, $B$42,TRUE)</f>
-        <v>0.99999622288885426</v>
+        <v>0.99999993714680924</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="151" t="s">
-        <v>201</v>
-      </c>
-      <c r="B52" s="128">
+      <c r="A52" s="146" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="122">
         <v>1</v>
       </c>
-      <c r="C52" s="153">
+      <c r="C52" s="148">
         <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="156">
+      <c r="D52" s="150">
         <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="153">
+      <c r="E52" s="148">
         <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="152"/>
-      <c r="B53" s="129">
+      <c r="A53" s="147"/>
+      <c r="B53" s="123">
         <v>1</v>
       </c>
-      <c r="C53" s="154"/>
-      <c r="D53" s="157"/>
-      <c r="E53" s="154"/>
+      <c r="C53" s="149"/>
+      <c r="D53" s="151"/>
+      <c r="E53" s="149"/>
       <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G54" s="79"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="108"/>
-      <c r="B55" s="109" t="s">
+      <c r="A55" s="102"/>
+      <c r="B55" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="109" t="s">
-        <v>244</v>
-      </c>
-      <c r="D55" s="122" t="s">
-        <v>222</v>
+      <c r="C55" s="103" t="s">
+        <v>241</v>
+      </c>
+      <c r="D55" s="116" t="s">
+        <v>220</v>
       </c>
       <c r="G55" s="79"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="112" t="s">
-        <v>218</v>
-      </c>
-      <c r="B56" s="115">
+      <c r="A56" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="B56" s="109">
         <f>_xlfn.NORM.INV(B44, $B$30, $B$40)</f>
-        <v>11.395243606351759</v>
-      </c>
-      <c r="C56" s="117">
+        <v>392.06466224659005</v>
+      </c>
+      <c r="C56" s="111">
         <f>B30-C58</f>
-        <v>8.7544865406300012</v>
-      </c>
-      <c r="D56" s="119">
+        <v>380.2425705072481</v>
+      </c>
+      <c r="D56" s="113">
         <f>_xlfn.NORM.INV(B44, B34, B41)</f>
-        <v>0.35671817913854981</v>
+        <v>0.37184484344553992</v>
       </c>
       <c r="G56" s="79"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="112" t="s">
-        <v>219</v>
-      </c>
-      <c r="B57" s="115">
+      <c r="A57" s="106" t="s">
+        <v>217</v>
+      </c>
+      <c r="B57" s="109">
         <f>_xlfn.NORM.INV(B45, $B$30, $B$40)</f>
-        <v>14.604756393648241</v>
-      </c>
-      <c r="C57" s="117">
+        <v>394.93533775340995</v>
+      </c>
+      <c r="C57" s="111">
         <f>B30+C58</f>
-        <v>17.245513459369999</v>
-      </c>
-      <c r="D57" s="117">
+        <v>406.7574294927519</v>
+      </c>
+      <c r="D57" s="111">
         <f>_xlfn.NORM.INV(B45, B34, B41)</f>
-        <v>0.64328182086145014</v>
+        <v>0.62815515655446008</v>
       </c>
       <c r="G57" s="79"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="123" t="s">
-        <v>229</v>
-      </c>
-      <c r="B58" s="115">
+      <c r="A58" s="117" t="s">
+        <v>227</v>
+      </c>
+      <c r="B58" s="109">
         <f>_xlfn.CONFIDENCE.NORM(1-B38, B32, B36)</f>
-        <v>1.6047563936482421</v>
-      </c>
-      <c r="C58" s="117">
+        <v>1.4353377534099525</v>
+      </c>
+      <c r="C58" s="111">
         <f>_xlfn.CONFIDENCE.T(1-B38, B33, B36)</f>
-        <v>4.2455134593699979</v>
-      </c>
-      <c r="D58" s="117">
+        <v>13.257429492751886</v>
+      </c>
+      <c r="D58" s="111">
         <f>_xlfn.CONFIDENCE.NORM(1-B38, B35, B36)</f>
-        <v>0.28656364172290039</v>
+        <v>0.25631031310892011</v>
       </c>
       <c r="G58" s="79"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C59" s="96"/>
+      <c r="C59" s="92"/>
       <c r="D59" s="76"/>
       <c r="G59" s="79"/>
     </row>
@@ -18951,369 +18988,369 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="75" customWidth="1"/>
-    <col min="2" max="4" width="22.6640625" style="137" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22.6640625" style="131" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="22.6640625" style="75" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="75"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="158" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
+      <c r="A1" s="152" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="130"/>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
+      <c r="A2" s="124"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="127" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="134">
+      <c r="B3" s="128">
         <v>30</v>
       </c>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="133" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" s="134">
+      <c r="A4" s="127" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="128">
         <v>31</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="133" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5" s="134">
+      <c r="A5" s="127" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="128">
         <v>0</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="133" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6" s="134">
+      <c r="A6" s="127" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="128">
         <v>0</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="133" t="s">
-        <v>252</v>
-      </c>
-      <c r="B7" s="134">
+      <c r="A7" s="127" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7" s="128">
         <v>6</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="142" t="s">
-        <v>251</v>
-      </c>
-      <c r="B8" s="134">
+      <c r="A8" s="136" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="128">
         <v>0</v>
       </c>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="133" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="134">
+      <c r="A9" s="127" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="128">
         <v>40</v>
       </c>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="132"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="133" t="s">
-        <v>261</v>
-      </c>
-      <c r="B10" s="134">
+      <c r="A10" s="127" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="128">
         <v>0.05</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="133" t="s">
-        <v>260</v>
-      </c>
-      <c r="B11" s="134">
+      <c r="A11" s="127" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" s="128">
         <v>1</v>
       </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="80"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="132"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="83" t="s">
-        <v>262</v>
-      </c>
-      <c r="B13" s="143">
+        <v>259</v>
+      </c>
+      <c r="B13" s="137">
         <f>B14</f>
         <v>1.0540925533894598</v>
       </c>
-      <c r="C13" s="131"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="132"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="140" t="s">
-        <v>262</v>
-      </c>
-      <c r="B14" s="135">
+      <c r="A14" s="134" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="129">
         <f>(B4-B3)/(IF(B8&gt;0, B8, B7)/SQRT(B9))</f>
         <v>1.0540925533894598</v>
       </c>
-      <c r="C14" s="131"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="140" t="s">
-        <v>263</v>
-      </c>
-      <c r="B15" s="141">
+      <c r="A15" s="134" t="s">
+        <v>260</v>
+      </c>
+      <c r="B15" s="135">
         <f>IF(B5 &gt; 0, (B6-B5)/SQRT(B5*(1-B5)/B9), 0)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="132"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="132"/>
+      <c r="C15" s="125"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="140" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="141">
+      <c r="A16" s="134" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="135">
         <f>B3 + B21 * (B7/SQRT(B9))</f>
         <v>31.560445163626671</v>
       </c>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="140" t="s">
-        <v>257</v>
-      </c>
-      <c r="B17" s="141">
+      <c r="A17" s="134" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="135">
         <f>_xlfn.NORM.DIST(B16,B4, B7/SQRT(B9), TRUE)</f>
         <v>0.72265973985512544</v>
       </c>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="132"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
     </row>
     <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="161" t="s">
-        <v>259</v>
-      </c>
-      <c r="B19" s="161"/>
-      <c r="C19" s="161"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
+      <c r="A19" s="155" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" s="155"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="145"/>
-      <c r="B20" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="C20" s="146" t="s">
-        <v>254</v>
-      </c>
-      <c r="D20" s="131"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="132"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="140" t="s">
+        <v>250</v>
+      </c>
+      <c r="C20" s="140" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="126"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="140" t="s">
-        <v>258</v>
-      </c>
-      <c r="B21" s="147">
+      <c r="A21" s="134" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="141">
         <f>_xlfn.NORM.S.INV(1-B10)</f>
         <v>1.6448536269514715</v>
       </c>
-      <c r="C21" s="135">
+      <c r="C21" s="129">
         <f>_xlfn.T.INV(IF(B11=1, 1-B10, B10/B11), B9 -1)</f>
         <v>1.6848751217112248</v>
       </c>
       <c r="D21" s="75"/>
-      <c r="E21" s="132"/>
+      <c r="E21" s="126"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="140" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="135">
+      <c r="A22" s="134" t="s">
+        <v>244</v>
+      </c>
+      <c r="B22" s="129">
         <f>_xlfn.NORM.S.DIST(IF(B15 &gt; 0, B15, B13), TRUE)</f>
         <v>0.85407972742810578</v>
       </c>
-      <c r="C22" s="135">
+      <c r="C22" s="129">
         <f>_xlfn.T.DIST(IF(B15 &gt; B15, B15, B13), (B9-1), TRUE)</f>
         <v>0.8508362851697302</v>
       </c>
-      <c r="D22" s="131"/>
-      <c r="E22" s="144"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="138"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="140" t="s">
-        <v>248</v>
-      </c>
-      <c r="B23" s="135">
+      <c r="A23" s="134" t="s">
+        <v>245</v>
+      </c>
+      <c r="B23" s="129">
         <f>1-B22</f>
         <v>0.14592027257189422</v>
       </c>
-      <c r="C23" s="135">
+      <c r="C23" s="129">
         <f>1-C22</f>
         <v>0.1491637148302698</v>
       </c>
-      <c r="D23" s="131"/>
-      <c r="F23" s="132"/>
+      <c r="D23" s="125"/>
+      <c r="F23" s="126"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="140" t="s">
-        <v>249</v>
-      </c>
-      <c r="B24" s="135">
+      <c r="A24" s="134" t="s">
+        <v>246</v>
+      </c>
+      <c r="B24" s="129">
         <f>B11 * IF(B13 &gt; 0,  B23,  B22)</f>
         <v>0.14592027257189422</v>
       </c>
-      <c r="C24" s="135">
+      <c r="C24" s="129">
         <f>B11 * IF(B13 &gt; 0, C23, C22)</f>
         <v>0.1491637148302698</v>
       </c>
-      <c r="D24" s="131"/>
-      <c r="E24" s="137"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="131"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="140" t="s">
-        <v>250</v>
-      </c>
-      <c r="B25" s="135" t="str">
+      <c r="A25" s="134" t="s">
+        <v>247</v>
+      </c>
+      <c r="B25" s="129" t="str">
         <f>IF(B24 &gt; B10,  "Do not reject", "Reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="C25" s="135" t="str">
+      <c r="C25" s="129" t="str">
         <f>IF(C24 &gt; B10, "Do not reject",  "Reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="D25" s="138"/>
-      <c r="F25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="F25" s="126"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="131"/>
-      <c r="F26" s="132"/>
+      <c r="C26" s="125"/>
+      <c r="F26" s="126"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="130"/>
-      <c r="B27" s="136"/>
-      <c r="C27" s="131"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="132"/>
+      <c r="A27" s="124"/>
+      <c r="B27" s="130"/>
+      <c r="C27" s="125"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="130"/>
-      <c r="B28" s="136"/>
-      <c r="C28" s="131"/>
-      <c r="F28" s="132"/>
-      <c r="G28" s="132"/>
+      <c r="A28" s="124"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="125"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="130"/>
-      <c r="B29" s="136"/>
-      <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="132"/>
+      <c r="A29" s="124"/>
+      <c r="B29" s="130"/>
+      <c r="C29" s="125"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
     </row>
     <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="158" t="s">
-        <v>246</v>
-      </c>
-      <c r="B30" s="159"/>
-      <c r="C30" s="159"/>
-      <c r="D30" s="159"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
+      <c r="A30" s="152" t="s">
+        <v>243</v>
+      </c>
+      <c r="B30" s="153"/>
+      <c r="C30" s="153"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Refactored comparison labels probability distributions
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE458E01-464A-3A41-875E-89701A191F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8CD2CE-0DFE-8243-8E40-6B7C7979D9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="262">
   <si>
     <t>E</t>
   </si>
@@ -609,15 +609,6 @@
   </si>
   <si>
     <t>Binomial Probability</t>
-  </si>
-  <si>
-    <t>Exaclty (=)</t>
-  </si>
-  <si>
-    <t>Less than (&lt;)</t>
-  </si>
-  <si>
-    <t>More than (&gt;)</t>
   </si>
   <si>
     <t>Comparison</t>
@@ -710,9 +701,6 @@
     <t>Normal Value</t>
   </si>
   <si>
-    <t>Why times by 0?</t>
-  </si>
-  <si>
     <t>Demand</t>
   </si>
   <si>
@@ -890,10 +878,13 @@
     <t>Bin</t>
   </si>
   <si>
-    <t>&lt;=</t>
-  </si>
-  <si>
     <t>&gt;</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -910,7 +901,7 @@
     <numFmt numFmtId="169" formatCode="#,##0.0000"/>
     <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -980,13 +971,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1020,7 +1004,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1031,12 +1015,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B083"/>
         <bgColor rgb="FFF4B083"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1184,7 +1162,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1372,9 +1350,8 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1387,52 +1364,51 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="9" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1454,23 +1430,23 @@
     <xf numFmtId="4" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1480,77 +1456,76 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -12888,21 +12863,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="142">
+      <c r="C17" s="148">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="143"/>
+      <c r="D17" s="149"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="142">
+      <c r="C18" s="148">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="143"/>
+      <c r="D18" s="149"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -16969,8 +16944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AD4EF6-892A-F84F-8FD1-A47C9BD9CBDB}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16982,34 +16957,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
+      <c r="A1" s="155" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
       <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H2" s="79"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="103" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" s="103" t="s">
+      <c r="A3" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="101" t="s">
         <v>167</v>
       </c>
       <c r="F3" s="79"/>
@@ -17023,15 +16998,15 @@
       <c r="B4" s="81">
         <v>15</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="107">
         <f>B4/$B$9</f>
         <v>0.1875</v>
       </c>
-      <c r="D4" s="119">
+      <c r="D4" s="117">
         <f>A4*C4</f>
         <v>0.1875</v>
       </c>
-      <c r="E4" s="119">
+      <c r="E4" s="117">
         <f>((A4-$D$9)^2)*C4</f>
         <v>0.82687500000000003</v>
       </c>
@@ -17046,15 +17021,15 @@
       <c r="B5" s="81">
         <v>13</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="107">
         <f t="shared" ref="C5:C8" si="0">B5/$B$9</f>
         <v>0.16250000000000001</v>
       </c>
-      <c r="D5" s="119">
+      <c r="D5" s="117">
         <f t="shared" ref="D5:D8" si="1">A5*C5</f>
         <v>0.32500000000000001</v>
       </c>
-      <c r="E5" s="119">
+      <c r="E5" s="117">
         <f t="shared" ref="E5:E8" si="2">((A5-$D$9)^2)*C5</f>
         <v>0.19662500000000005</v>
       </c>
@@ -17069,15 +17044,15 @@
       <c r="B6" s="81">
         <v>18</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="107">
         <f t="shared" si="0"/>
         <v>0.22500000000000001</v>
       </c>
-      <c r="D6" s="119">
+      <c r="D6" s="117">
         <f t="shared" si="1"/>
         <v>0.67500000000000004</v>
       </c>
-      <c r="E6" s="119">
+      <c r="E6" s="117">
         <f t="shared" si="2"/>
         <v>2.2500000000000042E-3</v>
       </c>
@@ -17092,15 +17067,15 @@
       <c r="B7" s="81">
         <v>17</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <f t="shared" si="0"/>
         <v>0.21249999999999999</v>
       </c>
-      <c r="D7" s="119">
+      <c r="D7" s="117">
         <f t="shared" si="1"/>
         <v>0.85</v>
       </c>
-      <c r="E7" s="119">
+      <c r="E7" s="117">
         <f t="shared" si="2"/>
         <v>0.17212499999999997</v>
       </c>
@@ -17115,15 +17090,15 @@
       <c r="B8" s="81">
         <v>17</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <f t="shared" si="0"/>
         <v>0.21249999999999999</v>
       </c>
-      <c r="D8" s="119">
+      <c r="D8" s="117">
         <f t="shared" si="1"/>
         <v>1.0625</v>
       </c>
-      <c r="E8" s="119">
+      <c r="E8" s="117">
         <f t="shared" si="2"/>
         <v>0.76712499999999995</v>
       </c>
@@ -17133,19 +17108,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="79"/>
-      <c r="B9" s="117">
+      <c r="B9" s="116">
         <f>SUM(B4:B8)</f>
         <v>80</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="116">
         <f t="shared" ref="C9" si="3">SUM(C4:C8)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="119">
+      <c r="D9" s="117">
         <f>SUM(D4:D8)</f>
         <v>3.1</v>
       </c>
-      <c r="E9" s="119">
+      <c r="E9" s="117">
         <f>SQRT(SUM(E4:E8))</f>
         <v>1.4017845768876187</v>
       </c>
@@ -17190,15 +17165,15 @@
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="144" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="144"/>
-      <c r="E14" s="144"/>
-      <c r="F14" s="144"/>
-      <c r="G14" s="144"/>
+      <c r="A14" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="155"/>
+      <c r="C14" s="155"/>
+      <c r="D14" s="155"/>
+      <c r="E14" s="155"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="155"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -17211,8 +17186,8 @@
       <c r="H15" s="79"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="106" t="s">
-        <v>189</v>
+      <c r="A16" s="105" t="s">
+        <v>186</v>
       </c>
       <c r="B16" s="83">
         <v>20</v>
@@ -17225,8 +17200,8 @@
       <c r="H16" s="79"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="106" t="s">
-        <v>190</v>
+      <c r="A17" s="105" t="s">
+        <v>187</v>
       </c>
       <c r="B17" s="91">
         <v>42</v>
@@ -17239,10 +17214,10 @@
       <c r="H17" s="79"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="106" t="s">
-        <v>200</v>
-      </c>
-      <c r="B18" s="119">
+      <c r="A18" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" s="117">
         <f>1/(B17-B16)</f>
         <v>4.5454545454545456E-2</v>
       </c>
@@ -17254,10 +17229,10 @@
       <c r="H18" s="79"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="106" t="s">
+      <c r="A19" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="164">
+      <c r="B19" s="146">
         <f>(B17+B16)/2</f>
         <v>31</v>
       </c>
@@ -17269,10 +17244,10 @@
       <c r="H19" s="79"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="106" t="s">
+      <c r="A20" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="164">
+      <c r="B20" s="146">
         <f>(B17-B16)/SQRT(12)</f>
         <v>6.3508529610858835</v>
       </c>
@@ -17285,9 +17260,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="89"/>
-      <c r="C21" s="93" t="s">
-        <v>203</v>
-      </c>
+      <c r="C21" s="90"/>
       <c r="D21" s="90"/>
       <c r="E21" s="90"/>
       <c r="F21" s="79"/>
@@ -17295,41 +17268,41 @@
       <c r="H21" s="79"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="103" t="s">
+      <c r="A22" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="103" t="s">
-        <v>187</v>
+      <c r="C22" s="102" t="s">
+        <v>184</v>
       </c>
       <c r="D22" s="90"/>
-      <c r="E22" s="118" t="s">
+      <c r="E22" s="102" t="s">
+        <v>195</v>
+      </c>
+      <c r="F22" s="102" t="s">
         <v>198</v>
-      </c>
-      <c r="F22" s="118" t="s">
-        <v>201</v>
       </c>
       <c r="G22" s="82"/>
       <c r="H22" s="79"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="106" t="s">
-        <v>182</v>
+      <c r="A23" s="105" t="s">
+        <v>260</v>
       </c>
       <c r="B23" s="83">
         <v>24</v>
       </c>
-      <c r="C23" s="109">
+      <c r="C23" s="108">
         <f>$B$18*0</f>
         <v>0</v>
       </c>
       <c r="D23" s="90"/>
-      <c r="E23" s="156">
+      <c r="E23" s="81">
         <v>70</v>
       </c>
-      <c r="F23" s="107">
+      <c r="F23" s="106">
         <f>((E23/100)/B18) + B16</f>
         <v>35.4</v>
       </c>
@@ -17337,13 +17310,13 @@
       <c r="H23" s="79"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="110" t="s">
-        <v>263</v>
+      <c r="A24" s="109" t="s">
+        <v>261</v>
       </c>
       <c r="B24" s="83">
         <v>31</v>
       </c>
-      <c r="C24" s="109">
+      <c r="C24" s="108">
         <f>$B$18*(B24-B16)</f>
         <v>0.5</v>
       </c>
@@ -17352,13 +17325,13 @@
       <c r="H24" s="79"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="106" t="s">
-        <v>264</v>
+      <c r="A25" s="105" t="s">
+        <v>259</v>
       </c>
       <c r="B25" s="83">
         <v>28</v>
       </c>
-      <c r="C25" s="109">
+      <c r="C25" s="108">
         <f>$B$18*($B$17-B25)</f>
         <v>0.63636363636363635</v>
       </c>
@@ -17367,13 +17340,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="146" t="s">
-        <v>199</v>
+      <c r="A26" s="151" t="s">
+        <v>196</v>
       </c>
       <c r="B26" s="83">
         <v>29</v>
       </c>
-      <c r="C26" s="148">
+      <c r="C26" s="153">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17382,11 +17355,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="147"/>
+      <c r="A27" s="152"/>
       <c r="B27" s="81">
         <v>37</v>
       </c>
-      <c r="C27" s="149"/>
+      <c r="C27" s="154"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17402,15 +17375,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="145" t="s">
-        <v>195</v>
-      </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145"/>
-      <c r="G30" s="145"/>
+      <c r="A30" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="150"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="150"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17419,22 +17392,22 @@
       <c r="H31" s="79"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="106" t="s">
+      <c r="A32" s="105" t="s">
         <v>74</v>
       </c>
       <c r="B32" s="84">
-        <v>16.3</v>
+        <v>236.88</v>
       </c>
       <c r="F32" s="79"/>
       <c r="G32" s="82"/>
       <c r="H32" s="79"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="106" t="s">
+      <c r="A33" s="105" t="s">
         <v>169</v>
       </c>
       <c r="B33" s="84">
-        <v>4.2</v>
+        <v>22.94</v>
       </c>
       <c r="C33" s="79"/>
       <c r="F33" s="79"/>
@@ -17442,8 +17415,8 @@
       <c r="H33" s="79"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="106" t="s">
-        <v>235</v>
+      <c r="A34" s="105" t="s">
+        <v>231</v>
       </c>
       <c r="B34" s="84">
         <v>1</v>
@@ -17462,104 +17435,104 @@
       <c r="H35" s="79"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="B36" s="103" t="s">
+      <c r="A36" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C36" s="103" t="s">
-        <v>187</v>
-      </c>
-      <c r="E36" s="118" t="s">
-        <v>198</v>
-      </c>
-      <c r="F36" s="118" t="s">
-        <v>202</v>
+      <c r="C36" s="102" t="s">
+        <v>184</v>
+      </c>
+      <c r="E36" s="102" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" s="102" t="s">
+        <v>199</v>
       </c>
       <c r="G36" s="82"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="106" t="s">
-        <v>182</v>
+      <c r="A37" s="105" t="s">
+        <v>260</v>
       </c>
       <c r="B37" s="83">
         <v>170</v>
       </c>
-      <c r="C37" s="109">
+      <c r="C37" s="108">
         <f>_xlfn.NORM.DIST(B37,$B$32,$B$33,FALSE)</f>
-        <v>1.4845303686723813E-292</v>
-      </c>
-      <c r="E37" s="156">
-        <v>99.7</v>
-      </c>
-      <c r="F37" s="107">
+        <v>2.4809688142993799E-4</v>
+      </c>
+      <c r="E37" s="81">
+        <v>80</v>
+      </c>
+      <c r="F37" s="106">
         <f>_xlfn.NORM.INV(E37/100, B32, B33)</f>
-        <v>27.840681818868966</v>
+        <v>256.18679109816264</v>
       </c>
       <c r="G37" s="82"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="110" t="s">
-        <v>263</v>
+      <c r="A38" s="109" t="s">
+        <v>261</v>
       </c>
       <c r="B38" s="83">
-        <v>170</v>
-      </c>
-      <c r="C38" s="109">
+        <v>252</v>
+      </c>
+      <c r="C38" s="108">
         <f>_xlfn.NORM.DIST(B38,$B$32,$B$33,TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="E38" s="117" t="s">
-        <v>233</v>
-      </c>
-      <c r="F38" s="107">
+        <v>0.74508766501499035</v>
+      </c>
+      <c r="E38" s="116" t="s">
+        <v>229</v>
+      </c>
+      <c r="F38" s="106">
         <f>B32 - (B34 * B33)</f>
-        <v>12.100000000000001</v>
+        <v>213.94</v>
       </c>
       <c r="G38" s="82"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="106" t="s">
-        <v>264</v>
+      <c r="A39" s="105" t="s">
+        <v>259</v>
       </c>
       <c r="B39" s="83">
-        <v>3</v>
-      </c>
-      <c r="C39" s="109">
+        <v>268</v>
+      </c>
+      <c r="C39" s="108">
         <f>(1-_xlfn.NORM.DIST(B39,$B$32,$B$33,TRUE))</f>
-        <v>0.99922901521552998</v>
+        <v>8.7456970340988316E-2</v>
       </c>
       <c r="D39" s="87"/>
-      <c r="E39" s="113" t="s">
-        <v>234</v>
-      </c>
-      <c r="F39" s="107">
+      <c r="E39" s="112" t="s">
+        <v>230</v>
+      </c>
+      <c r="F39" s="106">
         <f>B32 + (B34 * B33)</f>
-        <v>20.5</v>
+        <v>259.82</v>
       </c>
       <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="146" t="s">
-        <v>199</v>
+      <c r="A40" s="151" t="s">
+        <v>196</v>
       </c>
       <c r="B40" s="83">
-        <v>14</v>
-      </c>
-      <c r="C40" s="148">
+        <v>235</v>
+      </c>
+      <c r="C40" s="153">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
-        <v>0.44786484587392167</v>
+        <v>0.31786094323176883</v>
       </c>
       <c r="F40" s="87"/>
       <c r="G40" s="82"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="147"/>
+      <c r="A41" s="152"/>
       <c r="B41" s="81">
-        <v>19</v>
-      </c>
-      <c r="C41" s="149"/>
+        <v>255</v>
+      </c>
+      <c r="C41" s="154"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
     </row>
@@ -17582,18 +17555,18 @@
       <c r="G44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="145" t="s">
-        <v>194</v>
-      </c>
-      <c r="B46" s="145"/>
-      <c r="C46" s="145"/>
-      <c r="D46" s="145"/>
-      <c r="E46" s="145"/>
-      <c r="F46" s="145"/>
-      <c r="G46" s="145"/>
+      <c r="A46" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="150"/>
+      <c r="C46" s="150"/>
+      <c r="D46" s="150"/>
+      <c r="E46" s="150"/>
+      <c r="F46" s="150"/>
+      <c r="G46" s="150"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="106" t="s">
+      <c r="A48" s="105" t="s">
         <v>168</v>
       </c>
       <c r="B48" s="83">
@@ -17601,7 +17574,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="106" t="s">
+      <c r="A49" s="105" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="83">
@@ -17609,101 +17582,101 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="106" t="s">
+      <c r="A50" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="106">
+      <c r="B50" s="105">
         <f>B49*B48</f>
         <v>6.6499999999999995</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="106" t="s">
+      <c r="A51" s="105" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="106">
+      <c r="B51" s="105">
         <f>B49*(1-B48)*B48</f>
         <v>0.3325000000000003</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="B52" s="110">
+      <c r="B52" s="109">
         <f>SQRT(B51)</f>
         <v>0.57662812973354005</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="163"/>
+      <c r="A53" s="86"/>
       <c r="B53" s="86"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="B55" s="103" t="s">
+      <c r="A55" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B55" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C55" s="103" t="s">
+      <c r="C55" s="102" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="106" t="s">
-        <v>182</v>
+      <c r="A56" s="105" t="s">
+        <v>260</v>
       </c>
       <c r="B56" s="83">
         <v>6</v>
       </c>
-      <c r="C56" s="109">
+      <c r="C56" s="108">
         <f>_xlfn.BINOM.DIST(B56,$B$49,$B$48,FALSE)</f>
         <v>0.25728216171875024</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="110" t="s">
-        <v>263</v>
+      <c r="A57" s="109" t="s">
+        <v>261</v>
       </c>
       <c r="B57" s="83">
-        <v>2</v>
-      </c>
-      <c r="C57" s="109">
+        <v>4</v>
+      </c>
+      <c r="C57" s="108">
         <f>_xlfn.BINOM.DIST(B57, $B$49, $B$48, TRUE)</f>
-        <v>6.0273437500000207E-6</v>
+        <v>3.7570429687500077E-3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="106" t="s">
-        <v>264</v>
+      <c r="A58" s="105" t="s">
+        <v>259</v>
       </c>
       <c r="B58" s="83">
         <v>6</v>
       </c>
-      <c r="C58" s="109">
+      <c r="C58" s="108">
         <f>1 - _xlfn.BINOM.DIST(B58,$B$49,$B$48,TRUE)</f>
         <v>0.69833729609374973</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="146" t="s">
-        <v>199</v>
+      <c r="A59" s="151" t="s">
+        <v>196</v>
       </c>
       <c r="B59" s="83">
         <v>2</v>
       </c>
-      <c r="C59" s="148">
+      <c r="C59" s="153">
         <f>_xlfn.BINOM.DIST(B60,$B$49,$B$48,TRUE) - _xlfn.BINOM.DIST(B59,$B$49,$B$48,TRUE)</f>
         <v>0.30165667656250023</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="147"/>
+      <c r="A60" s="152"/>
       <c r="B60" s="81">
         <v>6</v>
       </c>
-      <c r="C60" s="149"/>
+      <c r="C60" s="154"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="89"/>
@@ -17721,98 +17694,98 @@
       <c r="C63" s="87"/>
     </row>
     <row r="65" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A65" s="145" t="s">
-        <v>196</v>
-      </c>
-      <c r="B65" s="145"/>
-      <c r="C65" s="145"/>
-      <c r="D65" s="145"/>
-      <c r="E65" s="145"/>
-      <c r="F65" s="145"/>
-      <c r="G65" s="145"/>
+      <c r="A65" s="150" t="s">
+        <v>193</v>
+      </c>
+      <c r="B65" s="150"/>
+      <c r="C65" s="150"/>
+      <c r="D65" s="150"/>
+      <c r="E65" s="150"/>
+      <c r="F65" s="150"/>
+      <c r="G65" s="150"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="106" t="s">
-        <v>191</v>
+      <c r="A67" s="105" t="s">
+        <v>188</v>
       </c>
       <c r="B67" s="84">
-        <v>3.4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="106" t="s">
+      <c r="A68" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="B68" s="108">
+      <c r="B68" s="107">
         <f>SQRT(B67)</f>
-        <v>1.8439088914585775</v>
+        <v>3.872983346207417</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="B70" s="103" t="s">
+      <c r="A70" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C70" s="103" t="s">
-        <v>186</v>
+      <c r="C70" s="102" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="106" t="s">
-        <v>182</v>
+      <c r="A71" s="105" t="s">
+        <v>260</v>
       </c>
       <c r="B71" s="83">
         <v>5</v>
       </c>
-      <c r="C71" s="109">
+      <c r="C71" s="108">
         <f>_xlfn.POISSON.DIST(B71,$B$67,FALSE)</f>
-        <v>0.12636072257615658</v>
+        <v>1.9357881219256173E-3</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="110" t="s">
-        <v>263</v>
+      <c r="A72" s="109" t="s">
+        <v>261</v>
       </c>
       <c r="B72" s="83">
-        <v>3</v>
-      </c>
-      <c r="C72" s="109">
+        <v>4</v>
+      </c>
+      <c r="C72" s="108">
         <f>_xlfn.POISSON.DIST(B72,$B$67,TRUE)</f>
-        <v>0.55835705528289536</v>
+        <v>8.5664121077530042E-4</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="106" t="s">
-        <v>264</v>
+      <c r="A73" s="105" t="s">
+        <v>259</v>
       </c>
       <c r="B73" s="83">
         <v>6</v>
       </c>
-      <c r="C73" s="109">
+      <c r="C73" s="108">
         <f>(1 - _xlfn.POISSON.DIST(B73,$B$67,TRUE))</f>
-        <v>5.78532206573662E-2</v>
+        <v>0.99236810036248502</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="146" t="s">
-        <v>199</v>
+      <c r="A74" s="151" t="s">
+        <v>196</v>
       </c>
       <c r="B74" s="83">
         <v>2</v>
       </c>
-      <c r="C74" s="148">
+      <c r="C74" s="153">
         <f>_xlfn.POISSON.DIST(B75,$B$67,TRUE) - _xlfn.POISSON.DIST(B74,$B$67,TRUE)</f>
-        <v>0.53080248168669208</v>
+        <v>2.7531208845164318E-3</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="147"/>
+      <c r="A75" s="152"/>
       <c r="B75" s="81">
         <v>5</v>
       </c>
-      <c r="C75" s="149"/>
+      <c r="C75" s="154"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="89"/>
@@ -17835,27 +17808,27 @@
       <c r="C79" s="87"/>
     </row>
     <row r="80" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A80" s="145" t="s">
-        <v>197</v>
-      </c>
-      <c r="B80" s="145"/>
-      <c r="C80" s="145"/>
-      <c r="D80" s="145"/>
-      <c r="E80" s="145"/>
-      <c r="F80" s="145"/>
-      <c r="G80" s="145"/>
+      <c r="A80" s="150" t="s">
+        <v>194</v>
+      </c>
+      <c r="B80" s="150"/>
+      <c r="C80" s="150"/>
+      <c r="D80" s="150"/>
+      <c r="E80" s="150"/>
+      <c r="F80" s="150"/>
+      <c r="G80" s="150"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B81" s="80"/>
       <c r="C81" s="87"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="106" t="s">
+      <c r="A82" s="105" t="s">
         <v>74</v>
       </c>
       <c r="B82" s="84">
-        <f>6/5</f>
-        <v>1.2</v>
+        <f>15/60</f>
+        <v>0.25</v>
       </c>
       <c r="C82" s="87"/>
     </row>
@@ -17864,75 +17837,74 @@
       <c r="C83" s="87"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="103" t="s">
+      <c r="A84" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="102" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="103" t="s">
-        <v>180</v>
-      </c>
-      <c r="C84" s="103" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="106" t="s">
-        <v>182</v>
+      <c r="A85" s="105" t="s">
+        <v>260</v>
       </c>
       <c r="B85" s="84">
         <v>1</v>
       </c>
-      <c r="C85" s="109">
+      <c r="C85" s="108">
         <f>_xlfn.EXPON.DIST(B85,$B$82,FALSE)</f>
-        <v>0.36143305429464256</v>
+        <v>0.19470019576785122</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="110" t="s">
-        <v>263</v>
+      <c r="A86" s="109" t="s">
+        <v>261</v>
       </c>
       <c r="B86" s="84">
-        <f>2.2/6</f>
-        <v>0.3666666666666667</v>
-      </c>
-      <c r="C86" s="109">
+        <v>0.05</v>
+      </c>
+      <c r="C86" s="108">
         <f>_xlfn.EXPON.DIST(B86,$B$82,TRUE)</f>
-        <v>0.35596357891685859</v>
+        <v>1.2422199506118572E-2</v>
       </c>
       <c r="E86" s="88"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="106" t="s">
-        <v>264</v>
+      <c r="A87" s="105" t="s">
+        <v>259</v>
       </c>
       <c r="B87" s="84">
         <f>2.7/6</f>
         <v>0.45</v>
       </c>
-      <c r="C87" s="109">
+      <c r="C87" s="108">
         <f>1 - _xlfn.EXPON.DIST(B87,$B$82,TRUE)</f>
-        <v>0.58274825237398964</v>
+        <v>0.89359734710851568</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="146" t="s">
-        <v>199</v>
+      <c r="A88" s="151" t="s">
+        <v>196</v>
       </c>
       <c r="B88" s="84">
         <f>2.1/6</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="C88" s="148">
+      <c r="C88" s="153">
         <f>_xlfn.EXPON.DIST(B89,$B$82,TRUE) - _xlfn.EXPON.DIST(B88,$B$82,TRUE)</f>
-        <v>0.25047716007445753</v>
+        <v>8.7189753470477277E-2</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="147"/>
+      <c r="A89" s="152"/>
       <c r="B89" s="81">
         <f>4.5/6</f>
         <v>0.75</v>
       </c>
-      <c r="C89" s="149"/>
+      <c r="C89" s="154"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="89"/>
@@ -17955,15 +17927,15 @@
       <c r="C93" s="87"/>
     </row>
     <row r="94" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A94" s="145" t="s">
+      <c r="A94" s="150" t="s">
         <v>179</v>
       </c>
-      <c r="B94" s="145"/>
-      <c r="C94" s="145"/>
-      <c r="D94" s="145"/>
-      <c r="E94" s="145"/>
-      <c r="F94" s="145"/>
-      <c r="G94" s="145"/>
+      <c r="B94" s="150"/>
+      <c r="C94" s="150"/>
+      <c r="D94" s="150"/>
+      <c r="E94" s="150"/>
+      <c r="F94" s="150"/>
+      <c r="G94" s="150"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D95" s="75"/>
@@ -18002,47 +17974,47 @@
       <c r="F99" s="79"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="102" t="s">
-        <v>204</v>
-      </c>
-      <c r="B100" s="102" t="s">
+      <c r="A100" s="101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="101" t="s">
         <v>174</v>
       </c>
-      <c r="C100" s="102" t="s">
+      <c r="C100" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="D100" s="102" t="s">
+      <c r="D100" s="101" t="s">
         <v>179</v>
       </c>
       <c r="E100" s="85"/>
       <c r="F100" s="79"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="83" t="s">
+      <c r="A101" s="105" t="s">
         <v>176</v>
       </c>
       <c r="B101" s="81">
         <v>7000</v>
       </c>
-      <c r="C101" s="165">
+      <c r="C101" s="147">
         <v>0.3</v>
       </c>
-      <c r="D101" s="102">
+      <c r="D101" s="101">
         <f>B101*C101</f>
         <v>2100</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="83" t="s">
+      <c r="A102" s="105" t="s">
         <v>177</v>
       </c>
       <c r="B102" s="81">
         <v>19000</v>
       </c>
-      <c r="C102" s="165">
+      <c r="C102" s="147">
         <v>0.45</v>
       </c>
-      <c r="D102" s="102">
+      <c r="D102" s="101">
         <f t="shared" ref="D102:D103" si="4">B102*C102</f>
         <v>8550</v>
       </c>
@@ -18050,16 +18022,16 @@
       <c r="F102" s="79"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="83" t="s">
+      <c r="A103" s="105" t="s">
         <v>178</v>
       </c>
       <c r="B103" s="81">
         <v>37000</v>
       </c>
-      <c r="C103" s="165">
+      <c r="C103" s="147">
         <v>0.25</v>
       </c>
-      <c r="D103" s="102">
+      <c r="D103" s="101">
         <f t="shared" si="4"/>
         <v>9250</v>
       </c>
@@ -18070,7 +18042,7 @@
       <c r="A104" s="79"/>
       <c r="B104" s="79"/>
       <c r="C104" s="79"/>
-      <c r="D104" s="102">
+      <c r="D104" s="101">
         <f>SUM(D101:D103)</f>
         <v>19900</v>
       </c>
@@ -18087,7 +18059,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="79" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B106" s="79"/>
       <c r="C106" s="79"/>
@@ -18098,7 +18070,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="79" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B107" s="79"/>
       <c r="C107" s="79"/>
@@ -18109,7 +18081,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="79" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B108" s="79"/>
       <c r="C108" s="79"/>
@@ -18119,7 +18091,7 @@
       <c r="G108" s="79"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="95"/>
+      <c r="A109" s="94"/>
       <c r="B109" s="79"/>
       <c r="C109" s="79"/>
       <c r="D109" s="79"/>
@@ -18128,10 +18100,10 @@
       <c r="G109" s="79"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="106" t="s">
-        <v>208</v>
-      </c>
-      <c r="B110" s="94">
+      <c r="A110" s="105" t="s">
+        <v>204</v>
+      </c>
+      <c r="B110" s="93">
         <v>4</v>
       </c>
       <c r="C110" s="79"/>
@@ -18141,10 +18113,10 @@
       <c r="G110" s="79"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="106" t="s">
-        <v>209</v>
-      </c>
-      <c r="B111" s="94">
+      <c r="A111" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="B111" s="93">
         <v>7</v>
       </c>
       <c r="C111" s="79"/>
@@ -18154,8 +18126,8 @@
       <c r="G111" s="79"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="106" t="s">
-        <v>211</v>
+      <c r="A112" s="105" t="s">
+        <v>207</v>
       </c>
       <c r="B112" s="81">
         <v>75</v>
@@ -18167,10 +18139,10 @@
       <c r="G112" s="79"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="106" t="s">
-        <v>210</v>
-      </c>
-      <c r="B113" s="94">
+      <c r="A113" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="B113" s="162">
         <f>B112*B110</f>
         <v>300</v>
       </c>
@@ -18181,60 +18153,60 @@
       <c r="G113" s="79"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="102" t="s">
-        <v>204</v>
-      </c>
-      <c r="B115" s="102" t="s">
+      <c r="A115" s="101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B115" s="101" t="s">
         <v>175</v>
       </c>
-      <c r="C115" s="102" t="s">
+      <c r="C115" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="D115" s="102" t="s">
+      <c r="D115" s="101" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="83" t="s">
+      <c r="A116" s="105" t="s">
         <v>176</v>
       </c>
       <c r="B116" s="81">
         <v>25</v>
       </c>
-      <c r="C116" s="107">
+      <c r="C116" s="106">
         <v>0.35</v>
       </c>
-      <c r="D116" s="120">
+      <c r="D116" s="118">
         <f>C116*($B$111*MIN($B$112, B116) - $B$113)</f>
         <v>-43.75</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="83" t="s">
+      <c r="A117" s="105" t="s">
         <v>177</v>
       </c>
       <c r="B117" s="81">
         <v>50</v>
       </c>
-      <c r="C117" s="107">
+      <c r="C117" s="106">
         <v>0.2</v>
       </c>
-      <c r="D117" s="120">
+      <c r="D117" s="118">
         <f t="shared" ref="D117:D118" si="5">C117*($B$111*MIN($B$112, B117) - $B$113)</f>
         <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="83" t="s">
+      <c r="A118" s="105" t="s">
         <v>178</v>
       </c>
       <c r="B118" s="81">
         <v>75</v>
       </c>
-      <c r="C118" s="107">
+      <c r="C118" s="106">
         <v>0.45</v>
       </c>
-      <c r="D118" s="120">
+      <c r="D118" s="118">
         <f t="shared" si="5"/>
         <v>101.25</v>
       </c>
@@ -18243,7 +18215,7 @@
       <c r="A119" s="79"/>
       <c r="B119" s="79"/>
       <c r="C119" s="79"/>
-      <c r="D119" s="121">
+      <c r="D119" s="119">
         <f>SUM(D116:D118)</f>
         <v>67.5</v>
       </c>
@@ -18262,6 +18234,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="A94:G94"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
@@ -18272,13 +18251,6 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="C88:C89"/>
     <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -18290,7 +18262,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18301,99 +18273,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
+      <c r="A1" s="150" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="103" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="160" t="s">
+      <c r="B3" s="102" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="98">
+      <c r="D3" s="97">
         <f>AVERAGE(A4:A23)</f>
         <v>34.6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="158">
+      <c r="A4" s="141">
         <v>25</v>
       </c>
       <c r="B4" s="77" cm="1">
         <f t="array" ref="B4:B23">_xlfn._xlws.SORT(A4:A23)</f>
         <v>5</v>
       </c>
-      <c r="C4" s="124"/>
+      <c r="C4" s="122"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="158">
+      <c r="A5" s="141">
         <v>20</v>
       </c>
       <c r="B5" s="77">
         <v>10</v>
       </c>
-      <c r="C5" s="157" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="103" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="102" t="s">
-        <v>214</v>
+      <c r="C5" s="140" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="101" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="158">
+      <c r="A6" s="141">
         <v>5</v>
       </c>
       <c r="B6" s="77">
         <v>15</v>
       </c>
-      <c r="C6" s="161">
+      <c r="C6" s="144">
         <v>5</v>
       </c>
-      <c r="D6" s="104">
+      <c r="D6" s="103">
         <f>AVERAGE(A4:A8)</f>
         <v>20</v>
       </c>
-      <c r="E6" s="105">
+      <c r="E6" s="104">
         <f>D6-$D$3</f>
         <v>-14.600000000000001</v>
       </c>
-      <c r="F6" s="99"/>
+      <c r="F6" s="98"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="158">
+      <c r="A7" s="141">
         <v>17</v>
       </c>
       <c r="B7" s="77">
         <v>17</v>
       </c>
-      <c r="C7" s="162">
+      <c r="C7" s="145">
         <v>10</v>
       </c>
-      <c r="D7" s="104">
+      <c r="D7" s="103">
         <f>AVERAGE(A4:A13)</f>
         <v>28.8</v>
       </c>
-      <c r="E7" s="105">
+      <c r="E7" s="104">
         <f>D7-$D$3</f>
         <v>-5.8000000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="158">
+      <c r="A8" s="141">
         <v>33</v>
       </c>
       <c r="B8" s="77">
@@ -18402,78 +18374,78 @@
       <c r="C8" s="79"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="158">
+      <c r="A9" s="141">
         <v>20</v>
       </c>
       <c r="B9" s="77">
         <v>20</v>
       </c>
-      <c r="C9" s="157" t="s">
-        <v>215</v>
-      </c>
-      <c r="D9" s="103" t="s">
-        <v>231</v>
-      </c>
-      <c r="E9" s="102" t="s">
-        <v>214</v>
+      <c r="C9" s="140" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="101" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="158">
+      <c r="A10" s="141">
         <v>41</v>
       </c>
       <c r="B10" s="77">
         <v>20</v>
       </c>
-      <c r="C10" s="161" t="s">
-        <v>238</v>
-      </c>
-      <c r="D10" s="104">
+      <c r="C10" s="144" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="103">
         <f>AVERAGE(B4:B8)</f>
         <v>13.4</v>
       </c>
-      <c r="E10" s="105">
+      <c r="E10" s="104">
         <f>D10-$D$3</f>
         <v>-21.200000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="158">
+      <c r="A11" s="141">
         <v>53</v>
       </c>
       <c r="B11" s="77">
         <v>24</v>
       </c>
-      <c r="C11" s="162" t="s">
-        <v>239</v>
-      </c>
-      <c r="D11" s="104">
+      <c r="C11" s="145" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="103">
         <f>AVERAGE(B19:B23)</f>
         <v>58.8</v>
       </c>
-      <c r="E11" s="105">
+      <c r="E11" s="104">
         <f>D11-$D$3</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="158">
+      <c r="A12" s="141">
         <v>50</v>
       </c>
       <c r="B12" s="77">
         <v>25</v>
       </c>
       <c r="C12" s="79"/>
-      <c r="D12" s="106" t="s">
-        <v>237</v>
-      </c>
-      <c r="E12" s="107">
+      <c r="D12" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" s="106">
         <f>MAX(ABS(E10), ABS(E11))</f>
         <v>24.199999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="158">
+      <c r="A13" s="141">
         <v>24</v>
       </c>
       <c r="B13" s="77">
@@ -18482,7 +18454,7 @@
       <c r="C13" s="79"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="158">
+      <c r="A14" s="141">
         <v>41</v>
       </c>
       <c r="B14" s="77">
@@ -18491,7 +18463,7 @@
       <c r="C14" s="79"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="158">
+      <c r="A15" s="141">
         <v>52</v>
       </c>
       <c r="B15" s="77">
@@ -18500,7 +18472,7 @@
       <c r="C15" s="79"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="158">
+      <c r="A16" s="141">
         <v>47</v>
       </c>
       <c r="B16" s="77">
@@ -18509,7 +18481,7 @@
       <c r="C16" s="79"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="158">
+      <c r="A17" s="141">
         <v>15</v>
       </c>
       <c r="B17" s="77">
@@ -18518,7 +18490,7 @@
       <c r="C17" s="79"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="158">
+      <c r="A18" s="141">
         <v>44</v>
       </c>
       <c r="B18" s="77">
@@ -18527,7 +18499,7 @@
       <c r="C18" s="79"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="159">
+      <c r="A19" s="142">
         <v>10</v>
       </c>
       <c r="B19" s="77">
@@ -18572,27 +18544,27 @@
       <c r="C23" s="79"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="101"/>
+      <c r="B24" s="100"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="101"/>
+      <c r="B25" s="100"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="101"/>
+      <c r="B26" s="100"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="101"/>
+      <c r="B27" s="100"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="145" t="s">
-        <v>261</v>
-      </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="145"/>
+      <c r="A28" s="150" t="s">
+        <v>257</v>
+      </c>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D29" s="76"/>
@@ -18601,7 +18573,7 @@
       <c r="G29" s="82"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="106" t="s">
+      <c r="A30" s="105" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="84">
@@ -18611,8 +18583,8 @@
       <c r="G30" s="82"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="106" t="s">
-        <v>231</v>
+      <c r="A31" s="105" t="s">
+        <v>227</v>
       </c>
       <c r="B31" s="84">
         <v>1</v>
@@ -18621,7 +18593,7 @@
       <c r="G31" s="82"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="106" t="s">
+      <c r="A32" s="105" t="s">
         <v>169</v>
       </c>
       <c r="B32" s="84">
@@ -18631,8 +18603,8 @@
       <c r="G32" s="82"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="106" t="s">
-        <v>240</v>
+      <c r="A33" s="105" t="s">
+        <v>236</v>
       </c>
       <c r="B33" s="84">
         <v>50.3</v>
@@ -18641,8 +18613,8 @@
       <c r="G33" s="82"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="106" t="s">
-        <v>220</v>
+      <c r="A34" s="105" t="s">
+        <v>216</v>
       </c>
       <c r="B34" s="84">
         <v>0.5</v>
@@ -18653,8 +18625,8 @@
       <c r="G34" s="82"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="106" t="s">
-        <v>232</v>
+      <c r="A35" s="105" t="s">
+        <v>228</v>
       </c>
       <c r="B35" s="84">
         <v>1</v>
@@ -18665,8 +18637,8 @@
       <c r="G35" s="82"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="106" t="s">
-        <v>213</v>
+      <c r="A36" s="105" t="s">
+        <v>209</v>
       </c>
       <c r="B36" s="84">
         <v>25</v>
@@ -18677,8 +18649,8 @@
       <c r="G36" s="82"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="106" t="s">
-        <v>221</v>
+      <c r="A37" s="105" t="s">
+        <v>217</v>
       </c>
       <c r="B37" s="84">
         <v>100</v>
@@ -18689,14 +18661,14 @@
       <c r="G37" s="82"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="106" t="s">
-        <v>226</v>
-      </c>
-      <c r="B38" s="96">
+      <c r="A38" s="105" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="95">
         <v>0.8</v>
       </c>
       <c r="D38" s="76"/>
-      <c r="E38" s="97"/>
+      <c r="E38" s="96"/>
       <c r="F38" s="79"/>
       <c r="G38" s="82"/>
     </row>
@@ -18710,58 +18682,58 @@
       <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="106" t="s">
-        <v>222</v>
-      </c>
-      <c r="B40" s="111">
+      <c r="A40" s="105" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" s="110">
         <f>B32/SQRT(B36)</f>
         <v>1.1199999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="106" t="s">
-        <v>224</v>
-      </c>
-      <c r="B41" s="111">
+      <c r="A41" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="B41" s="110">
         <f>SQRT(B34*(1-B34)/B36)</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="112" t="s">
-        <v>225</v>
-      </c>
-      <c r="B42" s="113">
+      <c r="A42" s="111" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" s="112">
         <f>B41 *  SQRT((B37-B36)/(B37-1))</f>
         <v>8.7038827977848926E-2</v>
       </c>
       <c r="G42" s="82"/>
     </row>
     <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="112" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="113">
+      <c r="A43" s="111" t="s">
+        <v>224</v>
+      </c>
+      <c r="B43" s="112">
         <f>(B31-B30)/(B32/SQRT(B36))</f>
         <v>-350.44642857142861</v>
       </c>
       <c r="G43" s="82"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="106" t="s">
-        <v>218</v>
-      </c>
-      <c r="B44" s="114">
+      <c r="A44" s="105" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" s="113">
         <f>(1-B38)/2</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="G44" s="82"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="106" t="s">
-        <v>219</v>
-      </c>
-      <c r="B45" s="115">
+      <c r="A45" s="105" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="114">
         <f>B38+B44</f>
         <v>0.9</v>
       </c>
@@ -18774,177 +18746,177 @@
       <c r="G47" s="82"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="103"/>
-      <c r="B48" s="103" t="s">
+      <c r="A48" s="102"/>
+      <c r="B48" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C48" s="103" t="s">
-        <v>229</v>
-      </c>
-      <c r="D48" s="103" t="s">
-        <v>223</v>
-      </c>
-      <c r="E48" s="103" t="s">
-        <v>230</v>
-      </c>
-      <c r="F48" s="100"/>
+      <c r="C48" s="102" t="s">
+        <v>225</v>
+      </c>
+      <c r="D48" s="102" t="s">
+        <v>219</v>
+      </c>
+      <c r="E48" s="102" t="s">
+        <v>226</v>
+      </c>
+      <c r="F48" s="99"/>
       <c r="G48" s="79"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="106" t="s">
-        <v>182</v>
-      </c>
-      <c r="B49" s="122">
+      <c r="A49" s="105" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" s="120">
         <v>1</v>
       </c>
-      <c r="C49" s="109">
+      <c r="C49" s="108">
         <f>_xlfn.NORM.DIST(B49, $B$30, $B$40,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="D49" s="109">
+      <c r="D49" s="108">
         <f>_xlfn.NORM.DIST(B49, $B$34, $B$41, FALSE)</f>
         <v>1.4867195147342977E-5</v>
       </c>
-      <c r="E49" s="109">
+      <c r="E49" s="108">
         <f>_xlfn.NORM.DIST(B49/$B$36, $B$34, $B$42,FALSE)</f>
         <v>3.9447003166566339E-6</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="110" t="s">
-        <v>183</v>
-      </c>
-      <c r="B50" s="122">
+      <c r="A50" s="109" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="120">
         <v>1</v>
       </c>
-      <c r="C50" s="109">
+      <c r="C50" s="108">
         <f>_xlfn.NORM.DIST(B50, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D50" s="109">
+      <c r="D50" s="108">
         <f>_xlfn.NORM.DIST(B50, $B$34, $B$41, TRUE)</f>
         <v>0.99999971334842808</v>
       </c>
-      <c r="E50" s="109">
+      <c r="E50" s="108">
         <f>_xlfn.NORM.DIST(B50/$B$36, $B$34, $B$42,TRUE)</f>
         <v>6.2853190747001746E-8</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="106" t="s">
-        <v>184</v>
-      </c>
-      <c r="B51" s="122">
+      <c r="A51" s="105" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" s="120">
         <v>1</v>
       </c>
-      <c r="C51" s="109">
+      <c r="C51" s="108">
         <f>(1-_xlfn.NORM.DIST(B51, $B$30, $B$40,TRUE))</f>
         <v>1</v>
       </c>
-      <c r="D51" s="109">
+      <c r="D51" s="108">
         <f>1 - _xlfn.NORM.DIST(B51, $B$34, $B$41, TRUE)</f>
         <v>2.8665157192353519E-7</v>
       </c>
-      <c r="E51" s="109">
+      <c r="E51" s="108">
         <f>1 - _xlfn.NORM.DIST(B51/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0.99999993714680924</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="146" t="s">
-        <v>199</v>
-      </c>
-      <c r="B52" s="122">
+      <c r="A52" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" s="120">
         <v>1</v>
       </c>
-      <c r="C52" s="148">
+      <c r="C52" s="153">
         <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="150">
+      <c r="D52" s="156">
         <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="148">
+      <c r="E52" s="153">
         <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="147"/>
-      <c r="B53" s="123">
+      <c r="A53" s="152"/>
+      <c r="B53" s="121">
         <v>1</v>
       </c>
-      <c r="C53" s="149"/>
-      <c r="D53" s="151"/>
-      <c r="E53" s="149"/>
+      <c r="C53" s="154"/>
+      <c r="D53" s="157"/>
+      <c r="E53" s="154"/>
       <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G54" s="79"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="102"/>
-      <c r="B55" s="103" t="s">
+      <c r="A55" s="101"/>
+      <c r="B55" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="103" t="s">
-        <v>241</v>
-      </c>
-      <c r="D55" s="116" t="s">
-        <v>220</v>
+      <c r="C55" s="102" t="s">
+        <v>237</v>
+      </c>
+      <c r="D55" s="115" t="s">
+        <v>216</v>
       </c>
       <c r="G55" s="79"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="B56" s="109">
+      <c r="A56" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="B56" s="108">
         <f>_xlfn.NORM.INV(B44, $B$30, $B$40)</f>
         <v>392.06466224659005</v>
       </c>
-      <c r="C56" s="111">
+      <c r="C56" s="110">
         <f>B30-C58</f>
         <v>380.2425705072481</v>
       </c>
-      <c r="D56" s="113">
+      <c r="D56" s="112">
         <f>_xlfn.NORM.INV(B44, B34, B41)</f>
         <v>0.37184484344553992</v>
       </c>
       <c r="G56" s="79"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="106" t="s">
-        <v>217</v>
-      </c>
-      <c r="B57" s="109">
+      <c r="A57" s="105" t="s">
+        <v>213</v>
+      </c>
+      <c r="B57" s="108">
         <f>_xlfn.NORM.INV(B45, $B$30, $B$40)</f>
         <v>394.93533775340995</v>
       </c>
-      <c r="C57" s="111">
+      <c r="C57" s="110">
         <f>B30+C58</f>
         <v>406.7574294927519</v>
       </c>
-      <c r="D57" s="111">
+      <c r="D57" s="110">
         <f>_xlfn.NORM.INV(B45, B34, B41)</f>
         <v>0.62815515655446008</v>
       </c>
       <c r="G57" s="79"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="117" t="s">
-        <v>227</v>
-      </c>
-      <c r="B58" s="109">
+      <c r="A58" s="116" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" s="108">
         <f>_xlfn.CONFIDENCE.NORM(1-B38, B32, B36)</f>
         <v>1.4353377534099525</v>
       </c>
-      <c r="C58" s="111">
+      <c r="C58" s="110">
         <f>_xlfn.CONFIDENCE.T(1-B38, B33, B36)</f>
         <v>13.257429492751886</v>
       </c>
-      <c r="D58" s="111">
+      <c r="D58" s="110">
         <f>_xlfn.CONFIDENCE.NORM(1-B38, B35, B36)</f>
         <v>0.25631031310892011</v>
       </c>
@@ -18995,362 +18967,362 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="75" customWidth="1"/>
-    <col min="2" max="4" width="22.6640625" style="131" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22.6640625" style="129" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="22.6640625" style="75" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="75"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="152" t="s">
-        <v>242</v>
-      </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
+      <c r="A1" s="158" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="124"/>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
+      <c r="A2" s="122"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="128">
+      <c r="B3" s="126">
         <v>30</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="127" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" s="128">
+      <c r="A4" s="125" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="126">
         <v>31</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="127" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" s="128">
+      <c r="A5" s="125" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" s="126">
         <v>0</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="127" t="s">
-        <v>252</v>
-      </c>
-      <c r="B6" s="128">
+      <c r="A6" s="125" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="126">
         <v>0</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="127" t="s">
-        <v>249</v>
-      </c>
-      <c r="B7" s="128">
+      <c r="A7" s="125" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7" s="126">
         <v>6</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="136" t="s">
-        <v>248</v>
-      </c>
-      <c r="B8" s="128">
+      <c r="A8" s="134" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="126">
         <v>0</v>
       </c>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="124"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="127" t="s">
-        <v>213</v>
-      </c>
-      <c r="B9" s="128">
+      <c r="A9" s="125" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="126">
         <v>40</v>
       </c>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="127" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="128">
+      <c r="A10" s="125" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="126">
         <v>0.05</v>
       </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="124"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="127" t="s">
-        <v>257</v>
-      </c>
-      <c r="B11" s="128">
+      <c r="A11" s="125" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="126">
         <v>1</v>
       </c>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="126"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="80"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="83" t="s">
-        <v>259</v>
-      </c>
-      <c r="B13" s="137">
+        <v>255</v>
+      </c>
+      <c r="B13" s="135">
         <f>B14</f>
         <v>1.0540925533894598</v>
       </c>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="134" t="s">
-        <v>259</v>
-      </c>
-      <c r="B14" s="129">
+      <c r="A14" s="132" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" s="127">
         <f>(B4-B3)/(IF(B8&gt;0, B8, B7)/SQRT(B9))</f>
         <v>1.0540925533894598</v>
       </c>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="134" t="s">
-        <v>260</v>
-      </c>
-      <c r="B15" s="135">
+      <c r="A15" s="132" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="133">
         <f>IF(B5 &gt; 0, (B6-B5)/SQRT(B5*(1-B5)/B9), 0)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="126"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="134" t="s">
-        <v>253</v>
-      </c>
-      <c r="B16" s="135">
+      <c r="A16" s="132" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="133">
         <f>B3 + B21 * (B7/SQRT(B9))</f>
         <v>31.560445163626671</v>
       </c>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="134" t="s">
-        <v>254</v>
-      </c>
-      <c r="B17" s="135">
+      <c r="A17" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="133">
         <f>_xlfn.NORM.DIST(B16,B4, B7/SQRT(B9), TRUE)</f>
         <v>0.72265973985512544</v>
       </c>
-      <c r="C17" s="125"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
     </row>
     <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="155" t="s">
-        <v>256</v>
-      </c>
-      <c r="B19" s="155"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
+      <c r="A19" s="161" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="161"/>
+      <c r="C19" s="161"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="139"/>
-      <c r="B20" s="140" t="s">
-        <v>250</v>
-      </c>
-      <c r="C20" s="140" t="s">
+      <c r="A20" s="137"/>
+      <c r="B20" s="138" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" s="138" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="132" t="s">
         <v>251</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="126"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="134" t="s">
-        <v>255</v>
-      </c>
-      <c r="B21" s="141">
+      <c r="B21" s="139">
         <f>_xlfn.NORM.S.INV(1-B10)</f>
         <v>1.6448536269514715</v>
       </c>
-      <c r="C21" s="129">
+      <c r="C21" s="127">
         <f>_xlfn.T.INV(IF(B11=1, 1-B10, B10/B11), B9 -1)</f>
         <v>1.6848751217112248</v>
       </c>
       <c r="D21" s="75"/>
-      <c r="E21" s="126"/>
+      <c r="E21" s="124"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="134" t="s">
-        <v>244</v>
-      </c>
-      <c r="B22" s="129">
+      <c r="A22" s="132" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="127">
         <f>_xlfn.NORM.S.DIST(IF(B15 &gt; 0, B15, B13), TRUE)</f>
         <v>0.85407972742810578</v>
       </c>
-      <c r="C22" s="129">
+      <c r="C22" s="127">
         <f>_xlfn.T.DIST(IF(B15 &gt; B15, B15, B13), (B9-1), TRUE)</f>
         <v>0.8508362851697302</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="138"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="136"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="134" t="s">
-        <v>245</v>
-      </c>
-      <c r="B23" s="129">
+      <c r="A23" s="132" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23" s="127">
         <f>1-B22</f>
         <v>0.14592027257189422</v>
       </c>
-      <c r="C23" s="129">
+      <c r="C23" s="127">
         <f>1-C22</f>
         <v>0.1491637148302698</v>
       </c>
-      <c r="D23" s="125"/>
-      <c r="F23" s="126"/>
+      <c r="D23" s="123"/>
+      <c r="F23" s="124"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="134" t="s">
-        <v>246</v>
-      </c>
-      <c r="B24" s="129">
+      <c r="A24" s="132" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="127">
         <f>B11 * IF(B13 &gt; 0,  B23,  B22)</f>
         <v>0.14592027257189422</v>
       </c>
-      <c r="C24" s="129">
+      <c r="C24" s="127">
         <f>B11 * IF(B13 &gt; 0, C23, C22)</f>
         <v>0.1491637148302698</v>
       </c>
-      <c r="D24" s="125"/>
-      <c r="E24" s="131"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="129"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="134" t="s">
-        <v>247</v>
-      </c>
-      <c r="B25" s="129" t="str">
+      <c r="A25" s="132" t="s">
+        <v>243</v>
+      </c>
+      <c r="B25" s="127" t="str">
         <f>IF(B24 &gt; B10,  "Do not reject", "Reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="C25" s="129" t="str">
+      <c r="C25" s="127" t="str">
         <f>IF(C24 &gt; B10, "Do not reject",  "Reject")</f>
         <v>Do not reject</v>
       </c>
-      <c r="D25" s="132"/>
-      <c r="F25" s="126"/>
+      <c r="D25" s="130"/>
+      <c r="F25" s="124"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="125"/>
-      <c r="F26" s="126"/>
+      <c r="C26" s="123"/>
+      <c r="F26" s="124"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="124"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="125"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="126"/>
+      <c r="A27" s="122"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="123"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="124"/>
-      <c r="B28" s="130"/>
-      <c r="C28" s="125"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="126"/>
+      <c r="A28" s="122"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="123"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="124"/>
-      <c r="B29" s="130"/>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="126"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="126"/>
+      <c r="A29" s="122"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="123"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="124"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
     </row>
     <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="152" t="s">
-        <v>243</v>
-      </c>
-      <c r="B30" s="153"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
+      <c r="A30" s="158" t="s">
+        <v>239</v>
+      </c>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Refactor cells to hightligh color based if is editable or not
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8CD2CE-0DFE-8243-8E40-6B7C7979D9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED3E83-133B-A74D-897A-4A648546F6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="264">
   <si>
     <t>E</t>
   </si>
@@ -758,18 +758,9 @@
     <t>std error mean</t>
   </si>
   <si>
-    <t xml:space="preserve">P(sample) </t>
-  </si>
-  <si>
-    <t>std error sample</t>
-  </si>
-  <si>
     <t>std error population</t>
   </si>
   <si>
-    <t>confidence level</t>
-  </si>
-  <si>
     <t>margin error</t>
   </si>
   <si>
@@ -884,7 +875,22 @@
     <t>=</t>
   </si>
   <si>
-    <t>&lt;</t>
+    <t>std error proportion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(proportion) </t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>confidence interval</t>
+  </si>
+  <si>
+    <t>Sample Size</t>
+  </si>
+  <si>
+    <t>Z value</t>
   </si>
 </sst>
 </file>
@@ -901,7 +907,7 @@
     <numFmt numFmtId="169" formatCode="#,##0.0000"/>
     <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1002,6 +1008,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1157,12 +1175,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1487,6 +1508,19 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1507,6 +1541,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1522,17 +1557,16 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{47997285-B3F5-F244-B205-73B85F68F6F7}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{B9995DE2-6BC8-2D45-B0CA-8CAD653AB999}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent 2" xfId="4" xr:uid="{FD7D5D8B-C45B-C54F-92D6-932DA4275992}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1560,6 +1594,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8584,8 +8628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M984"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G216" sqref="G216"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12863,21 +12907,21 @@
       <c r="B17" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="148">
+      <c r="C17" s="155">
         <f>_xlfn.COVARIANCE.S(E3:E7,F3:F7)</f>
         <v>10.25</v>
       </c>
-      <c r="D17" s="149"/>
+      <c r="D17" s="156"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="148">
+      <c r="C18" s="155">
         <f>CORREL(E3:E7,F3:F7)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D18" s="149"/>
+      <c r="D18" s="156"/>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -16944,8 +16988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AD4EF6-892A-F84F-8FD1-A47C9BD9CBDB}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16957,15 +17001,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="162" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
       <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -16973,7 +17017,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="102" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B3" s="102" t="s">
         <v>5</v>
@@ -16993,22 +17037,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="81">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C4" s="107">
         <f>B4/$B$9</f>
-        <v>0.1875</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="D4" s="117">
         <f>A4*C4</f>
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="E4" s="117">
         <f>((A4-$D$9)^2)*C4</f>
-        <v>0.82687500000000003</v>
+        <v>0.44227635200000004</v>
       </c>
       <c r="F4" s="79"/>
       <c r="G4" s="80"/>
@@ -17016,22 +17060,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="81">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C5" s="107">
         <f t="shared" ref="C5:C8" si="0">B5/$B$9</f>
-        <v>0.16250000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D5" s="117">
         <f t="shared" ref="D5:D8" si="1">A5*C5</f>
-        <v>0.32500000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E5" s="117">
         <f t="shared" ref="E5:E8" si="2">((A5-$D$9)^2)*C5</f>
-        <v>0.19662500000000005</v>
+        <v>6.4511999999999827E-4</v>
       </c>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
@@ -17039,22 +17083,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="81">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="107">
         <f t="shared" si="0"/>
-        <v>0.22500000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="D6" s="117">
         <f t="shared" si="1"/>
-        <v>0.67500000000000004</v>
+        <v>0.16</v>
       </c>
       <c r="E6" s="117">
         <f t="shared" si="2"/>
-        <v>2.2500000000000042E-3</v>
+        <v>8.786432000000001E-2</v>
       </c>
       <c r="F6" s="79"/>
       <c r="G6" s="79"/>
@@ -17062,22 +17106,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="81">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" s="107">
         <f t="shared" si="0"/>
-        <v>0.21249999999999999</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D7" s="117">
         <f t="shared" si="1"/>
-        <v>0.85</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="E7" s="117">
         <f t="shared" si="2"/>
-        <v>0.17212499999999997</v>
+        <v>0.402653184</v>
       </c>
       <c r="F7" s="79"/>
       <c r="G7" s="82"/>
@@ -17085,22 +17129,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="81">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="81">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C8" s="107">
         <f t="shared" si="0"/>
-        <v>0.21249999999999999</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="D8" s="117">
         <f t="shared" si="1"/>
-        <v>1.0625</v>
+        <v>0.224</v>
       </c>
       <c r="E8" s="117">
         <f t="shared" si="2"/>
-        <v>0.76712499999999995</v>
+        <v>0.52025702400000007</v>
       </c>
       <c r="F8" s="79"/>
       <c r="G8" s="82"/>
@@ -17110,7 +17154,7 @@
       <c r="A9" s="79"/>
       <c r="B9" s="116">
         <f>SUM(B4:B8)</f>
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="C9" s="116">
         <f t="shared" ref="C9" si="3">SUM(C4:C8)</f>
@@ -17118,11 +17162,11 @@
       </c>
       <c r="D9" s="117">
         <f>SUM(D4:D8)</f>
-        <v>3.1</v>
+        <v>0.95200000000000007</v>
       </c>
       <c r="E9" s="117">
         <f>SQRT(SUM(E4:E8))</f>
-        <v>1.4017845768876187</v>
+        <v>1.2056931616294422</v>
       </c>
       <c r="F9" s="79"/>
       <c r="G9" s="82"/>
@@ -17165,15 +17209,15 @@
       <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="155" t="s">
+      <c r="A14" s="162" t="s">
         <v>189</v>
       </c>
-      <c r="B14" s="155"/>
-      <c r="C14" s="155"/>
-      <c r="D14" s="155"/>
-      <c r="E14" s="155"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="155"/>
+      <c r="B14" s="162"/>
+      <c r="C14" s="162"/>
+      <c r="D14" s="162"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -17289,7 +17333,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="105" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B23" s="83">
         <v>24</v>
@@ -17311,7 +17355,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="109" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B24" s="83">
         <v>31</v>
@@ -17326,7 +17370,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="105" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B25" s="83">
         <v>28</v>
@@ -17340,13 +17384,13 @@
       <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="151" t="s">
+      <c r="A26" s="158" t="s">
         <v>196</v>
       </c>
       <c r="B26" s="83">
         <v>29</v>
       </c>
-      <c r="C26" s="153">
+      <c r="C26" s="160">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -17355,11 +17399,11 @@
       <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="152"/>
+      <c r="A27" s="159"/>
       <c r="B27" s="81">
         <v>37</v>
       </c>
-      <c r="C27" s="154"/>
+      <c r="C27" s="161"/>
       <c r="F27" s="79"/>
       <c r="G27" s="82"/>
       <c r="H27" s="79"/>
@@ -17375,15 +17419,15 @@
       <c r="H29" s="79"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="150" t="s">
+      <c r="A30" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="B30" s="150"/>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="157"/>
       <c r="H30" s="79"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -17396,7 +17440,7 @@
         <v>74</v>
       </c>
       <c r="B32" s="84">
-        <v>236.88</v>
+        <v>92.1</v>
       </c>
       <c r="F32" s="79"/>
       <c r="G32" s="82"/>
@@ -17407,7 +17451,7 @@
         <v>169</v>
       </c>
       <c r="B33" s="84">
-        <v>22.94</v>
+        <v>3.8</v>
       </c>
       <c r="C33" s="79"/>
       <c r="F33" s="79"/>
@@ -17416,7 +17460,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="105" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B34" s="84">
         <v>1</v>
@@ -17454,85 +17498,85 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="105" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B37" s="83">
         <v>170</v>
       </c>
       <c r="C37" s="108">
         <f>_xlfn.NORM.DIST(B37,$B$32,$B$33,FALSE)</f>
-        <v>2.4809688142993799E-4</v>
+        <v>5.8210115268694259E-93</v>
       </c>
       <c r="E37" s="81">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="F37" s="106">
         <f>_xlfn.NORM.INV(E37/100, B32, B33)</f>
-        <v>256.18679109816264</v>
+        <v>90.635782227651234</v>
       </c>
       <c r="G37" s="82"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="109" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B38" s="83">
-        <v>252</v>
+        <v>170</v>
       </c>
       <c r="C38" s="108">
         <f>_xlfn.NORM.DIST(B38,$B$32,$B$33,TRUE)</f>
-        <v>0.74508766501499035</v>
+        <v>1</v>
       </c>
       <c r="E38" s="116" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F38" s="106">
         <f>B32 - (B34 * B33)</f>
-        <v>213.94</v>
+        <v>88.3</v>
       </c>
       <c r="G38" s="82"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="105" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B39" s="83">
-        <v>268</v>
+        <v>90</v>
       </c>
       <c r="C39" s="108">
         <f>(1-_xlfn.NORM.DIST(B39,$B$32,$B$33,TRUE))</f>
-        <v>8.7456970340988316E-2</v>
+        <v>0.70974214320182194</v>
       </c>
       <c r="D39" s="87"/>
       <c r="E39" s="112" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F39" s="106">
         <f>B32 + (B34 * B33)</f>
-        <v>259.82</v>
+        <v>95.899999999999991</v>
       </c>
       <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="151" t="s">
+      <c r="A40" s="158" t="s">
         <v>196</v>
       </c>
       <c r="B40" s="83">
-        <v>235</v>
-      </c>
-      <c r="C40" s="153">
+        <v>14</v>
+      </c>
+      <c r="C40" s="160">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
-        <v>0.31786094323176883</v>
+        <v>9.0980992495193636E-83</v>
       </c>
       <c r="F40" s="87"/>
       <c r="G40" s="82"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="152"/>
+      <c r="A41" s="159"/>
       <c r="B41" s="81">
-        <v>255</v>
-      </c>
-      <c r="C41" s="154"/>
+        <v>19</v>
+      </c>
+      <c r="C41" s="161"/>
       <c r="F41" s="79"/>
       <c r="G41" s="79"/>
     </row>
@@ -17555,22 +17599,22 @@
       <c r="G44" s="79"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="150" t="s">
+      <c r="A46" s="157" t="s">
         <v>191</v>
       </c>
-      <c r="B46" s="150"/>
-      <c r="C46" s="150"/>
-      <c r="D46" s="150"/>
-      <c r="E46" s="150"/>
-      <c r="F46" s="150"/>
-      <c r="G46" s="150"/>
+      <c r="B46" s="157"/>
+      <c r="C46" s="157"/>
+      <c r="D46" s="157"/>
+      <c r="E46" s="157"/>
+      <c r="F46" s="157"/>
+      <c r="G46" s="157"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="105" t="s">
         <v>168</v>
       </c>
       <c r="B48" s="83">
-        <v>0.95</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -17578,7 +17622,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="83">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -17587,7 +17631,7 @@
       </c>
       <c r="B50" s="105">
         <f>B49*B48</f>
-        <v>6.6499999999999995</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -17596,7 +17640,7 @@
       </c>
       <c r="B51" s="105">
         <f>B49*(1-B48)*B48</f>
-        <v>0.3325000000000003</v>
+        <v>6.5958999999999994</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -17605,7 +17649,7 @@
       </c>
       <c r="B52" s="109">
         <f>SQRT(B51)</f>
-        <v>0.57662812973354005</v>
+        <v>2.568248430350927</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -17625,58 +17669,58 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="105" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B56" s="83">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C56" s="108">
         <f>_xlfn.BINOM.DIST(B56,$B$49,$B$48,FALSE)</f>
-        <v>0.25728216171875024</v>
+        <v>4.8396508822861123E-3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="109" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B57" s="83">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C57" s="108">
         <f>_xlfn.BINOM.DIST(B57, $B$49, $B$48, TRUE)</f>
-        <v>3.7570429687500077E-3</v>
+        <v>5.4728953427993282E-3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="105" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B58" s="83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" s="108">
         <f>1 - _xlfn.BINOM.DIST(B58,$B$49,$B$48,TRUE)</f>
-        <v>0.69833729609374973</v>
+        <v>0.72148233135432849</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="151" t="s">
+      <c r="A59" s="158" t="s">
         <v>196</v>
       </c>
       <c r="B59" s="83">
         <v>2</v>
       </c>
-      <c r="C59" s="153">
+      <c r="C59" s="160">
         <f>_xlfn.BINOM.DIST(B60,$B$49,$B$48,TRUE) - _xlfn.BINOM.DIST(B59,$B$49,$B$48,TRUE)</f>
-        <v>0.30165667656250023</v>
+        <v>0.40516176722632513</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="152"/>
+      <c r="A60" s="159"/>
       <c r="B60" s="81">
         <v>6</v>
       </c>
-      <c r="C60" s="154"/>
+      <c r="C60" s="161"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="89"/>
@@ -17694,22 +17738,23 @@
       <c r="C63" s="87"/>
     </row>
     <row r="65" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A65" s="150" t="s">
+      <c r="A65" s="157" t="s">
         <v>193</v>
       </c>
-      <c r="B65" s="150"/>
-      <c r="C65" s="150"/>
-      <c r="D65" s="150"/>
-      <c r="E65" s="150"/>
-      <c r="F65" s="150"/>
-      <c r="G65" s="150"/>
+      <c r="B65" s="157"/>
+      <c r="C65" s="157"/>
+      <c r="D65" s="157"/>
+      <c r="E65" s="157"/>
+      <c r="F65" s="157"/>
+      <c r="G65" s="157"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="105" t="s">
         <v>188</v>
       </c>
       <c r="B67" s="84">
-        <v>15</v>
+        <f>1/3.4</f>
+        <v>0.29411764705882354</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -17718,7 +17763,7 @@
       </c>
       <c r="B68" s="107">
         <f>SQRT(B67)</f>
-        <v>3.872983346207417</v>
+        <v>0.54232614454664041</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -17734,58 +17779,58 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="105" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B71" s="83">
         <v>5</v>
       </c>
       <c r="C71" s="108">
         <f>_xlfn.POISSON.DIST(B71,$B$67,FALSE)</f>
-        <v>1.9357881219256173E-3</v>
+        <v>1.3667544531873795E-5</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="109" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B72" s="83">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="C72" s="108">
         <f>_xlfn.POISSON.DIST(B72,$B$67,TRUE)</f>
-        <v>8.5664121077530042E-4</v>
+        <v>0.9965933487048797</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="105" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B73" s="83">
         <v>6</v>
       </c>
       <c r="C73" s="108">
         <f>(1 - _xlfn.POISSON.DIST(B73,$B$67,TRUE))</f>
-        <v>0.99236810036248502</v>
+        <v>2.9220104225124999E-8</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="151" t="s">
+      <c r="A74" s="158" t="s">
         <v>196</v>
       </c>
       <c r="B74" s="83">
         <v>2</v>
       </c>
-      <c r="C74" s="153">
+      <c r="C74" s="160">
         <f>_xlfn.POISSON.DIST(B75,$B$67,TRUE) - _xlfn.POISSON.DIST(B74,$B$67,TRUE)</f>
-        <v>2.7531208845164318E-3</v>
+        <v>3.4059520973428459E-3</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="152"/>
+      <c r="A75" s="159"/>
       <c r="B75" s="81">
         <v>5</v>
       </c>
-      <c r="C75" s="154"/>
+      <c r="C75" s="161"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="89"/>
@@ -17808,15 +17853,15 @@
       <c r="C79" s="87"/>
     </row>
     <row r="80" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A80" s="150" t="s">
+      <c r="A80" s="157" t="s">
         <v>194</v>
       </c>
-      <c r="B80" s="150"/>
-      <c r="C80" s="150"/>
-      <c r="D80" s="150"/>
-      <c r="E80" s="150"/>
-      <c r="F80" s="150"/>
-      <c r="G80" s="150"/>
+      <c r="B80" s="157"/>
+      <c r="C80" s="157"/>
+      <c r="D80" s="157"/>
+      <c r="E80" s="157"/>
+      <c r="F80" s="157"/>
+      <c r="G80" s="157"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B81" s="80"/>
@@ -17827,8 +17872,8 @@
         <v>74</v>
       </c>
       <c r="B82" s="84">
-        <f>15/60</f>
-        <v>0.25</v>
+        <f>1/5</f>
+        <v>0.2</v>
       </c>
       <c r="C82" s="87"/>
     </row>
@@ -17849,62 +17894,59 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="105" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B85" s="84">
         <v>1</v>
       </c>
       <c r="C85" s="108">
         <f>_xlfn.EXPON.DIST(B85,$B$82,FALSE)</f>
-        <v>0.19470019576785122</v>
+        <v>0.16374615061559639</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="109" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B86" s="84">
-        <v>0.05</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C86" s="108">
         <f>_xlfn.EXPON.DIST(B86,$B$82,TRUE)</f>
-        <v>1.2422199506118572E-2</v>
+        <v>0.35596357891685865</v>
       </c>
       <c r="E86" s="88"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="105" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B87" s="84">
-        <f>2.7/6</f>
-        <v>0.45</v>
+        <v>2.7</v>
       </c>
       <c r="C87" s="108">
         <f>1 - _xlfn.EXPON.DIST(B87,$B$82,TRUE)</f>
-        <v>0.89359734710851568</v>
+        <v>0.58274825237398964</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="151" t="s">
+      <c r="A88" s="158" t="s">
         <v>196</v>
       </c>
       <c r="B88" s="84">
-        <f>2.1/6</f>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="C88" s="153">
+        <v>2.1</v>
+      </c>
+      <c r="C88" s="160">
         <f>_xlfn.EXPON.DIST(B89,$B$82,TRUE) - _xlfn.EXPON.DIST(B88,$B$82,TRUE)</f>
-        <v>8.7189753470477277E-2</v>
+        <v>0.25047716007445764</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="152"/>
-      <c r="B89" s="81">
-        <f>4.5/6</f>
-        <v>0.75</v>
-      </c>
-      <c r="C89" s="154"/>
+      <c r="A89" s="159"/>
+      <c r="B89" s="149">
+        <v>4.5</v>
+      </c>
+      <c r="C89" s="161"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="89"/>
@@ -17927,15 +17969,15 @@
       <c r="C93" s="87"/>
     </row>
     <row r="94" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A94" s="150" t="s">
+      <c r="A94" s="157" t="s">
         <v>179</v>
       </c>
-      <c r="B94" s="150"/>
-      <c r="C94" s="150"/>
-      <c r="D94" s="150"/>
-      <c r="E94" s="150"/>
-      <c r="F94" s="150"/>
-      <c r="G94" s="150"/>
+      <c r="B94" s="157"/>
+      <c r="C94" s="157"/>
+      <c r="D94" s="157"/>
+      <c r="E94" s="157"/>
+      <c r="F94" s="157"/>
+      <c r="G94" s="157"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D95" s="75"/>
@@ -18142,7 +18184,7 @@
       <c r="A113" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="B113" s="162">
+      <c r="B113" s="148">
         <f>B112*B110</f>
         <v>300</v>
       </c>
@@ -18173,7 +18215,7 @@
       <c r="B116" s="81">
         <v>25</v>
       </c>
-      <c r="C116" s="106">
+      <c r="C116" s="147">
         <v>0.35</v>
       </c>
       <c r="D116" s="118">
@@ -18188,7 +18230,7 @@
       <c r="B117" s="81">
         <v>50</v>
       </c>
-      <c r="C117" s="106">
+      <c r="C117" s="147">
         <v>0.2</v>
       </c>
       <c r="D117" s="118">
@@ -18203,7 +18245,7 @@
       <c r="B118" s="81">
         <v>75</v>
       </c>
-      <c r="C118" s="106">
+      <c r="C118" s="147">
         <v>0.45</v>
       </c>
       <c r="D118" s="118">
@@ -18259,10 +18301,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E279595A-CDC1-E441-A6DF-F172F4F13CC6}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18273,22 +18315,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="157" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="101" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="102" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C3" s="143" t="s">
         <v>74</v>
@@ -18319,7 +18361,7 @@
         <v>211</v>
       </c>
       <c r="D5" s="102" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E5" s="101" t="s">
         <v>210</v>
@@ -18384,7 +18426,7 @@
         <v>211</v>
       </c>
       <c r="D9" s="102" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E9" s="101" t="s">
         <v>210</v>
@@ -18398,7 +18440,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="144" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D10" s="103">
         <f>AVERAGE(B4:B8)</f>
@@ -18417,7 +18459,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="145" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D11" s="103">
         <f>AVERAGE(B19:B23)</f>
@@ -18437,7 +18479,7 @@
       </c>
       <c r="C12" s="79"/>
       <c r="D12" s="105" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E12" s="106">
         <f>MAX(ABS(E10), ABS(E11))</f>
@@ -18544,413 +18586,557 @@
       <c r="C23" s="79"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="100"/>
+      <c r="A24" s="85"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="79"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="100"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="79"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="100"/>
+      <c r="A26" s="85"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="79"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="100"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="79"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="150" t="s">
-        <v>257</v>
-      </c>
-      <c r="B28" s="150"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="150"/>
-      <c r="G28" s="150"/>
+      <c r="A28" s="157" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28" s="157"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="157"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="157"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="82"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="79"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="105" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="84">
-        <v>393.5</v>
-      </c>
-      <c r="D30" s="76"/>
-      <c r="G30" s="82"/>
+      <c r="A30" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="83">
+        <v>70</v>
+      </c>
+      <c r="C30" s="79"/>
+      <c r="D30" s="116" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="83">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="105" t="s">
-        <v>227</v>
-      </c>
-      <c r="B31" s="84">
-        <v>1</v>
-      </c>
-      <c r="D31" s="76"/>
-      <c r="G31" s="82"/>
+      <c r="A31" s="116" t="s">
+        <v>220</v>
+      </c>
+      <c r="B31" s="83">
+        <v>14</v>
+      </c>
+      <c r="D31" s="116" t="s">
+        <v>220</v>
+      </c>
+      <c r="E31" s="154">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="B32" s="84">
-        <v>5.6</v>
-      </c>
-      <c r="D32" s="76"/>
-      <c r="G32" s="82"/>
+        <v>261</v>
+      </c>
+      <c r="B32" s="95">
+        <v>0.99</v>
+      </c>
+      <c r="D32" s="105" t="s">
+        <v>261</v>
+      </c>
+      <c r="E32" s="95">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="105" t="s">
-        <v>236</v>
-      </c>
-      <c r="B33" s="84">
-        <v>50.3</v>
-      </c>
-      <c r="D33" s="76"/>
-      <c r="G33" s="82"/>
+        <v>263</v>
+      </c>
+      <c r="B33" s="152">
+        <f>_xlfn.NORM.S.INV((1-B32)/2)</f>
+        <v>-2.5758293035488999</v>
+      </c>
+      <c r="D33" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" s="152">
+        <f>_xlfn.NORM.S.INV((1-E32)/2)</f>
+        <v>-1.9599639845400536</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="105" t="s">
-        <v>216</v>
-      </c>
-      <c r="B34" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="D34" s="76"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="82"/>
+      <c r="A34" s="116" t="s">
+        <v>209</v>
+      </c>
+      <c r="B34" s="153">
+        <f>((B33*B30)/B31)^2</f>
+        <v>165.87241502553027</v>
+      </c>
+      <c r="D34" s="116" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" s="153">
+        <f>(E33^2*E30*(1-E30))/E31^2</f>
+        <v>553.17007017995377</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="105" t="s">
-        <v>228</v>
-      </c>
-      <c r="B35" s="84">
-        <v>1</v>
-      </c>
-      <c r="D35" s="76"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="82"/>
+      <c r="B35" s="100"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="105" t="s">
-        <v>209</v>
-      </c>
-      <c r="B36" s="84">
-        <v>25</v>
-      </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="82"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="105" t="s">
-        <v>217</v>
-      </c>
-      <c r="B37" s="84">
-        <v>100</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="82"/>
+      <c r="B36" s="100"/>
+    </row>
+    <row r="37" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A37" s="157" t="s">
+        <v>254</v>
+      </c>
+      <c r="B37" s="157"/>
+      <c r="C37" s="157"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="157"/>
+      <c r="F37" s="157"/>
+      <c r="G37" s="157"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="105" t="s">
-        <v>222</v>
-      </c>
-      <c r="B38" s="95">
-        <v>0.8</v>
-      </c>
       <c r="D38" s="76"/>
-      <c r="E38" s="96"/>
+      <c r="E38" s="76"/>
       <c r="F38" s="79"/>
       <c r="G38" s="82"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="79"/>
-      <c r="B39" s="79"/>
-      <c r="C39" s="79"/>
+      <c r="A39" s="105" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="84">
+        <v>282.5</v>
+      </c>
       <c r="D39" s="76"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
       <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="105" t="s">
-        <v>218</v>
-      </c>
-      <c r="B40" s="110">
-        <f>B32/SQRT(B36)</f>
-        <v>1.1199999999999999</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B40" s="84">
+        <v>0</v>
+      </c>
+      <c r="D40" s="76"/>
+      <c r="G40" s="82"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="105" t="s">
-        <v>220</v>
-      </c>
-      <c r="B41" s="110">
-        <f>SQRT(B34*(1-B34)/B36)</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="111" t="s">
-        <v>221</v>
-      </c>
-      <c r="B42" s="112">
-        <f>B41 *  SQRT((B37-B36)/(B37-1))</f>
-        <v>8.7038827977848926E-2</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B41" s="84">
+        <v>12.2</v>
+      </c>
+      <c r="D41" s="76"/>
+      <c r="G41" s="82"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" s="84">
+        <v>4.2</v>
+      </c>
+      <c r="D42" s="76"/>
       <c r="G42" s="82"/>
     </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="111" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="112">
-        <f>(B31-B30)/(B32/SQRT(B36))</f>
-        <v>-350.44642857142861</v>
-      </c>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="105" t="s">
+        <v>216</v>
+      </c>
+      <c r="B43" s="84">
+        <v>0.79</v>
+      </c>
+      <c r="D43" s="76"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="82"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="105" t="s">
-        <v>214</v>
-      </c>
-      <c r="B44" s="113">
-        <f>(1-B38)/2</f>
-        <v>9.9999999999999978E-2</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="B44" s="84">
+        <f>B45</f>
+        <v>0.40730823708832603</v>
+      </c>
+      <c r="D44" s="76"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="86"/>
       <c r="G44" s="82"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="105" t="s">
-        <v>215</v>
-      </c>
-      <c r="B45" s="114">
-        <f>B38+B44</f>
-        <v>0.9</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="B45" s="109">
+        <f>SQRT(B43 * (1 - B43))</f>
+        <v>0.40730823708832603</v>
+      </c>
+      <c r="D45" s="76"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="86"/>
       <c r="G45" s="82"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="B46" s="84">
+        <v>30</v>
+      </c>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="79"/>
       <c r="G46" s="82"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="105" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="84">
+        <v>100</v>
+      </c>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="79"/>
       <c r="G47" s="82"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="102"/>
-      <c r="B48" s="102" t="s">
-        <v>180</v>
-      </c>
-      <c r="C48" s="102" t="s">
-        <v>225</v>
-      </c>
-      <c r="D48" s="102" t="s">
-        <v>219</v>
-      </c>
-      <c r="E48" s="102" t="s">
-        <v>226</v>
-      </c>
-      <c r="F48" s="99"/>
-      <c r="G48" s="79"/>
+      <c r="A48" s="105" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" s="95">
+        <v>0.8</v>
+      </c>
+      <c r="D48" s="76"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="82"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="105" t="s">
-        <v>260</v>
-      </c>
-      <c r="B49" s="120">
-        <v>1</v>
-      </c>
-      <c r="C49" s="108">
-        <f>_xlfn.NORM.DIST(B49, $B$30, $B$40,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="108">
-        <f>_xlfn.NORM.DIST(B49, $B$34, $B$41, FALSE)</f>
-        <v>1.4867195147342977E-5</v>
-      </c>
-      <c r="E49" s="108">
-        <f>_xlfn.NORM.DIST(B49/$B$36, $B$34, $B$42,FALSE)</f>
-        <v>3.9447003166566339E-6</v>
-      </c>
+      <c r="A49" s="79"/>
+      <c r="B49" s="79"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="82"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="109" t="s">
-        <v>261</v>
-      </c>
-      <c r="B50" s="120">
-        <v>1</v>
-      </c>
-      <c r="C50" s="108">
-        <f>_xlfn.NORM.DIST(B50, $B$30, $B$40,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="108">
-        <f>_xlfn.NORM.DIST(B50, $B$34, $B$41, TRUE)</f>
-        <v>0.99999971334842808</v>
-      </c>
-      <c r="E50" s="108">
-        <f>_xlfn.NORM.DIST(B50/$B$36, $B$34, $B$42,TRUE)</f>
-        <v>6.2853190747001746E-8</v>
+      <c r="A50" s="105" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" s="110">
+        <f>B41/SQRT(B46)</f>
+        <v>2.2274050671876755</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="B51" s="110">
+        <f>SQRT(B43*(1-B43)/B46)</f>
+        <v>7.4363969770312829E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="111" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="112">
+        <f>B51 *  SQRT((B47-B46)/(B47-1))</f>
+        <v>6.2530800491445895E-2</v>
+      </c>
+      <c r="G52" s="82"/>
+    </row>
+    <row r="53" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="111" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" s="112">
+        <f>(B40-B39)/(B41/SQRT(B46))</f>
+        <v>-126.8291987665651</v>
+      </c>
+      <c r="G53" s="82"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="105" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" s="113">
+        <f>(1-B48)/2</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="G54" s="82"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="105" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" s="114">
+        <f>B48+B54</f>
+        <v>0.9</v>
+      </c>
+      <c r="G55" s="82"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="82"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="82"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="102"/>
+      <c r="B58" s="102" t="s">
+        <v>180</v>
+      </c>
+      <c r="C58" s="102" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58" s="102" t="s">
         <v>259</v>
       </c>
-      <c r="B51" s="120">
+      <c r="E58" s="102" t="s">
+        <v>223</v>
+      </c>
+      <c r="F58" s="99"/>
+      <c r="G58" s="79"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="105" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" s="120">
         <v>1</v>
       </c>
-      <c r="C51" s="108">
-        <f>(1-_xlfn.NORM.DIST(B51, $B$30, $B$40,TRUE))</f>
+      <c r="C59" s="108">
+        <f>_xlfn.NORM.DIST(B59, $B$39, $B$50,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="108">
+        <f>_xlfn.NORM.DIST(B59, $B$43, $B$51, FALSE)</f>
+        <v>9.9510056096036179E-2</v>
+      </c>
+      <c r="E59" s="108">
+        <f>_xlfn.NORM.DIST(B59/$B$46, $B$43, $B$52,FALSE)</f>
+        <v>1.0199816782484256E-31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="109" t="s">
+        <v>260</v>
+      </c>
+      <c r="B60" s="120">
+        <v>279</v>
+      </c>
+      <c r="C60" s="108">
+        <f>_xlfn.NORM.DIST(B60, $B$39, $B$50,TRUE)</f>
+        <v>5.8052403829567452E-2</v>
+      </c>
+      <c r="D60" s="108">
+        <f>_xlfn.NORM.DIST(B60, $B$43, $B$51, TRUE)</f>
         <v>1</v>
       </c>
-      <c r="D51" s="108">
-        <f>1 - _xlfn.NORM.DIST(B51, $B$34, $B$41, TRUE)</f>
-        <v>2.8665157192353519E-7</v>
-      </c>
-      <c r="E51" s="108">
-        <f>1 - _xlfn.NORM.DIST(B51/$B$36, $B$34, $B$42,TRUE)</f>
-        <v>0.99999993714680924</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="151" t="s">
+      <c r="E60" s="108">
+        <f>_xlfn.NORM.DIST(B60/$B$46, $B$43, $B$52,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="B61" s="120">
+        <v>0.74</v>
+      </c>
+      <c r="C61" s="108">
+        <f>(1-_xlfn.NORM.DIST(B61, $B$39, $B$50,TRUE))</f>
+        <v>1</v>
+      </c>
+      <c r="D61" s="108">
+        <f>1 - _xlfn.NORM.DIST(B61, $B$43, $B$51, TRUE)</f>
+        <v>0.7493254737662115</v>
+      </c>
+      <c r="E61" s="108">
+        <f>1 - _xlfn.NORM.DIST(B61/$B$46, $B$43, $B$52,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="158" t="s">
         <v>196</v>
       </c>
-      <c r="B52" s="120">
-        <v>1</v>
-      </c>
-      <c r="C52" s="153">
-        <f>_xlfn.NORM.DIST(B53, $B$30, $B$40,TRUE) - _xlfn.NORM.DIST(B52, $B$30, $B$40,TRUE)</f>
+      <c r="B62" s="120">
+        <v>14</v>
+      </c>
+      <c r="C62" s="160">
+        <f>_xlfn.NORM.DIST(B63, $B$39, $B$50,TRUE) - _xlfn.NORM.DIST(B62, $B$39, $B$50,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="156">
-        <f>_xlfn.NORM.DIST(B53, $B$34, $B$41, TRUE) - _xlfn.NORM.DIST(B52, $B$34, $B$41, TRUE)</f>
+      <c r="D62" s="164">
+        <f>_xlfn.NORM.DIST(B63, $B$43, $B$51, TRUE) - _xlfn.NORM.DIST(B62, $B$43, $B$51, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="153">
-        <f>_xlfn.NORM.DIST(B53/$B$36, $B$34, $B$42,TRUE) - _xlfn.NORM.DIST(B52/$B$36, $B$34, $B$42,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="152"/>
-      <c r="B53" s="121">
-        <v>1</v>
-      </c>
-      <c r="C53" s="154"/>
-      <c r="D53" s="157"/>
-      <c r="E53" s="154"/>
-      <c r="G53" s="79"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G54" s="79"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="101"/>
-      <c r="B55" s="102" t="s">
+      <c r="E62" s="160">
+        <f>_xlfn.NORM.DIST(B63/$B$46, $B$43, $B$52,TRUE) - _xlfn.NORM.DIST(B62/$B$46, $B$43, $B$52,TRUE)</f>
+        <v>6.1149796065439257E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="159"/>
+      <c r="B63" s="121">
+        <v>19</v>
+      </c>
+      <c r="C63" s="161"/>
+      <c r="D63" s="165"/>
+      <c r="E63" s="161"/>
+      <c r="G63" s="79"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="79"/>
+      <c r="B64" s="79"/>
+      <c r="C64" s="79"/>
+      <c r="D64" s="79"/>
+      <c r="E64" s="79"/>
+      <c r="G64" s="79"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="163" t="s">
+        <v>249</v>
+      </c>
+      <c r="B65" s="163"/>
+      <c r="C65" s="163"/>
+      <c r="D65" s="163"/>
+      <c r="G65" s="79"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="101"/>
+      <c r="B66" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="102" t="s">
-        <v>237</v>
-      </c>
-      <c r="D55" s="115" t="s">
+      <c r="C66" s="115" t="s">
         <v>216</v>
       </c>
-      <c r="G55" s="79"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="105" t="s">
+      <c r="D66" s="102" t="s">
+        <v>234</v>
+      </c>
+      <c r="G66" s="79"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="105" t="s">
         <v>212</v>
       </c>
-      <c r="B56" s="108">
-        <f>_xlfn.NORM.INV(B44, $B$30, $B$40)</f>
-        <v>392.06466224659005</v>
-      </c>
-      <c r="C56" s="110">
-        <f>B30-C58</f>
-        <v>380.2425705072481</v>
-      </c>
-      <c r="D56" s="112">
-        <f>_xlfn.NORM.INV(B44, B34, B41)</f>
-        <v>0.37184484344553992</v>
-      </c>
-      <c r="G56" s="79"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="105" t="s">
+      <c r="B67" s="108">
+        <f>_xlfn.NORM.INV(B54, $B$39, $B$50)</f>
+        <v>279.64546554904365</v>
+      </c>
+      <c r="C67" s="112">
+        <f>_xlfn.NORM.INV(B54, B43, B51)</f>
+        <v>0.69469873812074423</v>
+      </c>
+      <c r="D67" s="110">
+        <f>B39-D69</f>
+        <v>281.49437749218231</v>
+      </c>
+      <c r="G67" s="79"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="105" t="s">
         <v>213</v>
       </c>
-      <c r="B57" s="108">
-        <f>_xlfn.NORM.INV(B45, $B$30, $B$40)</f>
-        <v>394.93533775340995</v>
-      </c>
-      <c r="C57" s="110">
-        <f>B30+C58</f>
-        <v>406.7574294927519</v>
-      </c>
-      <c r="D57" s="110">
-        <f>_xlfn.NORM.INV(B45, B34, B41)</f>
-        <v>0.62815515655446008</v>
-      </c>
-      <c r="G57" s="79"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="116" t="s">
-        <v>223</v>
-      </c>
-      <c r="B58" s="108">
-        <f>_xlfn.CONFIDENCE.NORM(1-B38, B32, B36)</f>
-        <v>1.4353377534099525</v>
-      </c>
-      <c r="C58" s="110">
-        <f>_xlfn.CONFIDENCE.T(1-B38, B33, B36)</f>
-        <v>13.257429492751886</v>
-      </c>
-      <c r="D58" s="110">
-        <f>_xlfn.CONFIDENCE.NORM(1-B38, B35, B36)</f>
-        <v>0.25631031310892011</v>
-      </c>
-      <c r="G58" s="79"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C59" s="92"/>
-      <c r="D59" s="76"/>
-      <c r="G59" s="79"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="79"/>
-      <c r="G60" s="79"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="79"/>
-      <c r="G61" s="79"/>
+      <c r="B68" s="108">
+        <f>_xlfn.NORM.INV(B55, $B$39, $B$50)</f>
+        <v>285.35453445095635</v>
+      </c>
+      <c r="C68" s="110">
+        <f>_xlfn.NORM.INV(B55, B43, B51)</f>
+        <v>0.88530126187925584</v>
+      </c>
+      <c r="D68" s="110">
+        <f>B39+D69</f>
+        <v>283.50562250781769</v>
+      </c>
+      <c r="G68" s="79"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="116" t="s">
+        <v>220</v>
+      </c>
+      <c r="B69" s="108">
+        <f>_xlfn.CONFIDENCE.NORM(1-B48, B41, B46)</f>
+        <v>2.8545344509563417</v>
+      </c>
+      <c r="C69" s="110">
+        <f>_xlfn.CONFIDENCE.NORM(1-B48, B44, B46)</f>
+        <v>9.5301261879255764E-2</v>
+      </c>
+      <c r="D69" s="110">
+        <f>_xlfn.CONFIDENCE.T(1-B48, B42, B46)</f>
+        <v>1.0056225078176664</v>
+      </c>
+      <c r="G69" s="79"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C70" s="92"/>
+      <c r="D70" s="76"/>
+      <c r="G70" s="79"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="79"/>
+      <c r="G71" s="79"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C72" s="150"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="79"/>
+      <c r="G72" s="79"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C73" s="151"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B23">
     <sortCondition ref="B4:B23"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A28:G28"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D62:D63"/>
   </mergeCells>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
+      <formula>$B$45</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -18961,7 +19147,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18973,15 +19159,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="158" t="s">
-        <v>238</v>
-      </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
+      <c r="A1" s="166" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="122"/>
@@ -18997,7 +19183,7 @@
         <v>74</v>
       </c>
       <c r="B3" s="126">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C3" s="123"/>
       <c r="D3" s="123"/>
@@ -19007,10 +19193,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B4" s="126">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C4" s="123"/>
       <c r="D4" s="123"/>
@@ -19033,7 +19219,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="125" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B6" s="126">
         <v>0</v>
@@ -19046,10 +19232,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="125" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B7" s="126">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="123"/>
       <c r="D7" s="123"/>
@@ -19059,7 +19245,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="134" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B8" s="126">
         <v>0</v>
@@ -19075,7 +19261,7 @@
         <v>209</v>
       </c>
       <c r="B9" s="126">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" s="123"/>
       <c r="D9" s="123"/>
@@ -19085,10 +19271,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="125" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B10" s="126">
-        <v>0.05</v>
+        <v>0.9</v>
       </c>
       <c r="C10" s="123"/>
       <c r="D10" s="123"/>
@@ -19098,7 +19284,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="125" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B11" s="126">
         <v>1</v>
@@ -19120,11 +19306,11 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="83" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B13" s="135">
         <f>B14</f>
-        <v>1.0540925533894598</v>
+        <v>0</v>
       </c>
       <c r="C13" s="123"/>
       <c r="D13" s="123"/>
@@ -19134,11 +19320,11 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="132" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B14" s="127">
         <f>(B4-B3)/(IF(B8&gt;0, B8, B7)/SQRT(B9))</f>
-        <v>1.0540925533894598</v>
+        <v>0</v>
       </c>
       <c r="C14" s="123"/>
       <c r="D14" s="123"/>
@@ -19148,7 +19334,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="132" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B15" s="133">
         <f>IF(B5 &gt; 0, (B6-B5)/SQRT(B5*(1-B5)/B9), 0)</f>
@@ -19162,11 +19348,11 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="132" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B16" s="133">
         <f>B3 + B21 * (B7/SQRT(B9))</f>
-        <v>31.560445163626671</v>
+        <v>20.932040362046166</v>
       </c>
       <c r="C16" s="123"/>
       <c r="D16" s="123"/>
@@ -19176,11 +19362,11 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="132" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B17" s="133">
         <f>_xlfn.NORM.DIST(B16,B4, B7/SQRT(B9), TRUE)</f>
-        <v>0.72265973985512544</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="C17" s="123"/>
       <c r="D17" s="123"/>
@@ -19190,11 +19376,11 @@
     </row>
     <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="161" t="s">
-        <v>252</v>
-      </c>
-      <c r="B19" s="161"/>
-      <c r="C19" s="161"/>
+      <c r="A19" s="163" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" s="163"/>
+      <c r="C19" s="163"/>
       <c r="D19" s="123"/>
       <c r="E19" s="124"/>
       <c r="F19" s="124"/>
@@ -19202,10 +19388,10 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="137"/>
       <c r="B20" s="138" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C20" s="138" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D20" s="123"/>
       <c r="E20" s="123"/>
@@ -19213,75 +19399,75 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="132" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B21" s="139">
         <f>_xlfn.NORM.S.INV(1-B10)</f>
-        <v>1.6448536269514715</v>
+        <v>-1.2815515655446006</v>
       </c>
       <c r="C21" s="127">
         <f>_xlfn.T.INV(IF(B11=1, 1-B10, B10/B11), B9 -1)</f>
-        <v>1.6848751217112248</v>
+        <v>-1.3062118020160358</v>
       </c>
       <c r="D21" s="75"/>
       <c r="E21" s="124"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="132" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B22" s="127">
         <f>_xlfn.NORM.S.DIST(IF(B15 &gt; 0, B15, B13), TRUE)</f>
-        <v>0.85407972742810578</v>
+        <v>0.5</v>
       </c>
       <c r="C22" s="127">
         <f>_xlfn.T.DIST(IF(B15 &gt; B15, B15, B13), (B9-1), TRUE)</f>
-        <v>0.8508362851697302</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="123"/>
       <c r="E22" s="136"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="132" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B23" s="127">
         <f>1-B22</f>
-        <v>0.14592027257189422</v>
+        <v>0.5</v>
       </c>
       <c r="C23" s="127">
         <f>1-C22</f>
-        <v>0.1491637148302698</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="123"/>
       <c r="F23" s="124"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="132" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B24" s="127">
         <f>B11 * IF(B13 &gt; 0,  B23,  B22)</f>
-        <v>0.14592027257189422</v>
+        <v>0.5</v>
       </c>
       <c r="C24" s="127">
         <f>B11 * IF(B13 &gt; 0, C23, C22)</f>
-        <v>0.1491637148302698</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="123"/>
       <c r="E24" s="129"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="132" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B25" s="127" t="str">
-        <f>IF(B24 &gt; B10,  "Do not reject", "Reject")</f>
-        <v>Do not reject</v>
+        <f>IF(B24 &gt;= B10,  "Do not reject", "Reject")</f>
+        <v>Reject</v>
       </c>
       <c r="C25" s="127" t="str">
-        <f>IF(C24 &gt; B10, "Do not reject",  "Reject")</f>
-        <v>Do not reject</v>
+        <f>IF(C24 &gt;= B10, "Do not reject",  "Reject")</f>
+        <v>Reject</v>
       </c>
       <c r="D25" s="130"/>
       <c r="F25" s="124"/>
@@ -19314,15 +19500,15 @@
       <c r="G29" s="124"/>
     </row>
     <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="158" t="s">
-        <v>239</v>
-      </c>
-      <c r="B30" s="159"/>
-      <c r="C30" s="159"/>
-      <c r="D30" s="159"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
+      <c r="A30" s="166" t="s">
+        <v>236</v>
+      </c>
+      <c r="B30" s="167"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="168"/>
+      <c r="F30" s="168"/>
+      <c r="G30" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added formula for hypothesis with two sample populations
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0DF55F-1AA6-DD40-9015-22F584B4D25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B4F9DF-8F78-F44B-B903-62D4B2606BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="233">
   <si>
     <t>E</t>
   </si>
@@ -785,6 +785,18 @@
   </si>
   <si>
     <t>Z value</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t>Hypothesis Test Two Populations</t>
+  </si>
+  <si>
+    <t>F critial value</t>
+  </si>
+  <si>
+    <t>F score</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1089,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1384,13 +1396,13 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1404,6 +1416,7 @@
     <xf numFmtId="166" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1420,7 +1433,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="11" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -8169,7 +8185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E428" sqref="E428"/>
     </sheetView>
   </sheetViews>
@@ -10212,11 +10228,11 @@
       <c r="B271" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C271" s="142">
+      <c r="C271" s="143">
         <f>_xlfn.COVARIANCE.S(F257:F261,G257:G261)</f>
         <v>10.25</v>
       </c>
-      <c r="D271" s="143"/>
+      <c r="D271" s="144"/>
       <c r="E271"/>
       <c r="F271"/>
       <c r="G271"/>
@@ -10227,11 +10243,11 @@
       <c r="B272" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C272" s="142">
+      <c r="C272" s="143">
         <f>CORREL(F257:F261,G257:G261)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D272" s="143"/>
+      <c r="D272" s="144"/>
       <c r="E272"/>
       <c r="F272"/>
       <c r="G272"/>
@@ -11901,23 +11917,23 @@
       <c r="A406" s="57">
         <v>191</v>
       </c>
-      <c r="B406" s="156">
+      <c r="B406" s="142">
         <f>MIN(A394:A408)</f>
         <v>179</v>
       </c>
-      <c r="C406" s="156">
+      <c r="C406" s="142">
         <f>_xlfn.QUARTILE.EXC(A394:A408, 1)</f>
         <v>196</v>
       </c>
-      <c r="D406" s="156">
+      <c r="D406" s="142">
         <f>_xlfn.QUARTILE.EXC(A394:A408, 2)</f>
         <v>223</v>
       </c>
-      <c r="E406" s="156">
+      <c r="E406" s="142">
         <f>_xlfn.QUARTILE.EXC(A394:A408, 3)</f>
         <v>249</v>
       </c>
-      <c r="F406" s="156">
+      <c r="F406" s="142">
         <f>MAX(A394:A408)</f>
         <v>267</v>
       </c>
@@ -15550,15 +15566,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="150" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
       <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -15758,15 +15774,15 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="150" t="s">
         <v>155</v>
       </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="144"/>
-      <c r="E14" s="144"/>
-      <c r="F14" s="144"/>
-      <c r="G14" s="144"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="150"/>
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -16825,6 +16841,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="A94:G94"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
@@ -16835,13 +16858,6 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="C88:C89"/>
     <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16867,12 +16883,12 @@
       <c r="A1" s="145" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
@@ -17543,7 +17559,7 @@
         <f>_xlfn.NORM.DIST(B63, $B$39, $B$50,TRUE) - _xlfn.NORM.DIST(B62, $B$39, $B$50,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D62" s="151">
+      <c r="D62" s="152">
         <f>_xlfn.NORM.DIST(B63, $B$43, $B$51, TRUE) - _xlfn.NORM.DIST(B62, $B$43, $B$51, TRUE)</f>
         <v>0</v>
       </c>
@@ -17558,7 +17574,7 @@
         <v>19</v>
       </c>
       <c r="C63" s="149"/>
-      <c r="D63" s="152"/>
+      <c r="D63" s="153"/>
       <c r="E63" s="149"/>
       <c r="G63" s="66"/>
     </row>
@@ -17571,12 +17587,12 @@
       <c r="G64" s="66"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="150" t="s">
+      <c r="A65" s="151" t="s">
         <v>214</v>
       </c>
-      <c r="B65" s="150"/>
-      <c r="C65" s="150"/>
-      <c r="D65" s="150"/>
+      <c r="B65" s="151"/>
+      <c r="C65" s="151"/>
+      <c r="D65" s="151"/>
       <c r="G65" s="66"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -17693,10 +17709,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17708,15 +17724,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="154" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="109"/>
@@ -17925,11 +17941,11 @@
     </row>
     <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="151" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="150"/>
-      <c r="C19" s="150"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="151"/>
       <c r="D19" s="110"/>
       <c r="E19" s="111"/>
       <c r="F19" s="111"/>
@@ -18043,15 +18059,50 @@
       <c r="A29" s="109"/>
       <c r="B29" s="115"/>
       <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="111"/>
       <c r="F29" s="111"/>
       <c r="G29" s="111"/>
     </row>
+    <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A30" s="154" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30" s="158"/>
+      <c r="C30" s="158"/>
+      <c r="D30" s="158"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="B32" s="157">
+        <v>11.734883999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="B33" s="157">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="68" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="157">
+        <f>_xlfn.F.INV.RT(B33, 1, 3)</f>
+        <v>10.127964486013932</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B6">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">

</xml_diff>

<commit_message>
Added formulas to calculate t and f critical values for hyphiesis with two populations
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B4F9DF-8F78-F44B-B903-62D4B2606BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F6BC51-A766-E64F-974F-AE862C3C5A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="236">
   <si>
     <t>E</t>
   </si>
@@ -793,10 +793,19 @@
     <t>Hypothesis Test Two Populations</t>
   </si>
   <si>
-    <t>F critial value</t>
-  </si>
-  <si>
-    <t>F score</t>
+    <t>DF Model</t>
+  </si>
+  <si>
+    <t>DF Error</t>
+  </si>
+  <si>
+    <t>T-Critical value</t>
+  </si>
+  <si>
+    <t>F-Critical value</t>
+  </si>
+  <si>
+    <t>DF Slope</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1098,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1397,6 +1406,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1433,10 +1443,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="11" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -10228,11 +10238,11 @@
       <c r="B271" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C271" s="143">
+      <c r="C271" s="144">
         <f>_xlfn.COVARIANCE.S(F257:F261,G257:G261)</f>
         <v>10.25</v>
       </c>
-      <c r="D271" s="144"/>
+      <c r="D271" s="145"/>
       <c r="E271"/>
       <c r="F271"/>
       <c r="G271"/>
@@ -10243,11 +10253,11 @@
       <c r="B272" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C272" s="143">
+      <c r="C272" s="144">
         <f>CORREL(F257:F261,G257:G261)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D272" s="144"/>
+      <c r="D272" s="145"/>
       <c r="E272"/>
       <c r="F272"/>
       <c r="G272"/>
@@ -15566,15 +15576,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
       <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -15774,15 +15784,15 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="150" t="s">
+      <c r="A14" s="151" t="s">
         <v>155</v>
       </c>
-      <c r="B14" s="150"/>
-      <c r="C14" s="150"/>
-      <c r="D14" s="150"/>
-      <c r="E14" s="150"/>
-      <c r="F14" s="150"/>
-      <c r="G14" s="150"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="151"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="151"/>
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -15949,13 +15959,13 @@
       <c r="H25" s="66"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="146" t="s">
+      <c r="A26" s="147" t="s">
         <v>162</v>
       </c>
       <c r="B26" s="70">
         <v>29</v>
       </c>
-      <c r="C26" s="148">
+      <c r="C26" s="149">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -15964,11 +15974,11 @@
       <c r="H26" s="66"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="147"/>
+      <c r="A27" s="148"/>
       <c r="B27" s="68">
         <v>37</v>
       </c>
-      <c r="C27" s="149"/>
+      <c r="C27" s="150"/>
       <c r="F27" s="66"/>
       <c r="G27" s="69"/>
       <c r="H27" s="66"/>
@@ -15984,15 +15994,15 @@
       <c r="H29" s="66"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="145" t="s">
+      <c r="A30" s="146" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145"/>
-      <c r="G30" s="145"/>
+      <c r="B30" s="146"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="146"/>
+      <c r="E30" s="146"/>
+      <c r="F30" s="146"/>
+      <c r="G30" s="146"/>
       <c r="H30" s="66"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -16123,13 +16133,13 @@
       <c r="G39" s="69"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="146" t="s">
+      <c r="A40" s="147" t="s">
         <v>162</v>
       </c>
       <c r="B40" s="70">
         <v>14</v>
       </c>
-      <c r="C40" s="148">
+      <c r="C40" s="149">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
         <v>9.0980992495193636E-83</v>
       </c>
@@ -16137,11 +16147,11 @@
       <c r="G40" s="69"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="147"/>
+      <c r="A41" s="148"/>
       <c r="B41" s="68">
         <v>19</v>
       </c>
-      <c r="C41" s="149"/>
+      <c r="C41" s="150"/>
       <c r="F41" s="66"/>
       <c r="G41" s="66"/>
     </row>
@@ -16164,15 +16174,15 @@
       <c r="G44" s="66"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="145" t="s">
+      <c r="A46" s="146" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="145"/>
-      <c r="C46" s="145"/>
-      <c r="D46" s="145"/>
-      <c r="E46" s="145"/>
-      <c r="F46" s="145"/>
-      <c r="G46" s="145"/>
+      <c r="B46" s="146"/>
+      <c r="C46" s="146"/>
+      <c r="D46" s="146"/>
+      <c r="E46" s="146"/>
+      <c r="F46" s="146"/>
+      <c r="G46" s="146"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="92" t="s">
@@ -16269,23 +16279,23 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="146" t="s">
+      <c r="A59" s="147" t="s">
         <v>162</v>
       </c>
       <c r="B59" s="70">
         <v>2</v>
       </c>
-      <c r="C59" s="148">
+      <c r="C59" s="149">
         <f>_xlfn.BINOM.DIST(B60,$B$49,$B$48,TRUE) - _xlfn.BINOM.DIST(B59,$B$49,$B$48,TRUE)</f>
         <v>0.40516176722632513</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="147"/>
+      <c r="A60" s="148"/>
       <c r="B60" s="68">
         <v>6</v>
       </c>
-      <c r="C60" s="149"/>
+      <c r="C60" s="150"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="76"/>
@@ -16303,15 +16313,15 @@
       <c r="C63" s="74"/>
     </row>
     <row r="65" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A65" s="145" t="s">
+      <c r="A65" s="146" t="s">
         <v>159</v>
       </c>
-      <c r="B65" s="145"/>
-      <c r="C65" s="145"/>
-      <c r="D65" s="145"/>
-      <c r="E65" s="145"/>
-      <c r="F65" s="145"/>
-      <c r="G65" s="145"/>
+      <c r="B65" s="146"/>
+      <c r="C65" s="146"/>
+      <c r="D65" s="146"/>
+      <c r="E65" s="146"/>
+      <c r="F65" s="146"/>
+      <c r="G65" s="146"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="92" t="s">
@@ -16379,23 +16389,23 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="146" t="s">
+      <c r="A74" s="147" t="s">
         <v>162</v>
       </c>
       <c r="B74" s="70">
         <v>2</v>
       </c>
-      <c r="C74" s="148">
+      <c r="C74" s="149">
         <f>_xlfn.POISSON.DIST(B75,$B$67,TRUE) - _xlfn.POISSON.DIST(B74,$B$67,TRUE)</f>
         <v>3.4059520973428459E-3</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="147"/>
+      <c r="A75" s="148"/>
       <c r="B75" s="68">
         <v>5</v>
       </c>
-      <c r="C75" s="149"/>
+      <c r="C75" s="150"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="76"/>
@@ -16418,15 +16428,15 @@
       <c r="C79" s="74"/>
     </row>
     <row r="80" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A80" s="145" t="s">
+      <c r="A80" s="146" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="145"/>
-      <c r="C80" s="145"/>
-      <c r="D80" s="145"/>
-      <c r="E80" s="145"/>
-      <c r="F80" s="145"/>
-      <c r="G80" s="145"/>
+      <c r="B80" s="146"/>
+      <c r="C80" s="146"/>
+      <c r="D80" s="146"/>
+      <c r="E80" s="146"/>
+      <c r="F80" s="146"/>
+      <c r="G80" s="146"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B81" s="67"/>
@@ -16495,23 +16505,23 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="146" t="s">
+      <c r="A88" s="147" t="s">
         <v>162</v>
       </c>
       <c r="B88" s="71">
         <v>2.1</v>
       </c>
-      <c r="C88" s="148">
+      <c r="C88" s="149">
         <f>_xlfn.EXPON.DIST(B89,$B$82,TRUE) - _xlfn.EXPON.DIST(B88,$B$82,TRUE)</f>
         <v>0.25047716007445764</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="147"/>
+      <c r="A89" s="148"/>
       <c r="B89" s="136">
         <v>4.5</v>
       </c>
-      <c r="C89" s="149"/>
+      <c r="C89" s="150"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="76"/>
@@ -16534,15 +16544,15 @@
       <c r="C93" s="74"/>
     </row>
     <row r="94" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A94" s="145" t="s">
+      <c r="A94" s="146" t="s">
         <v>145</v>
       </c>
-      <c r="B94" s="145"/>
-      <c r="C94" s="145"/>
-      <c r="D94" s="145"/>
-      <c r="E94" s="145"/>
-      <c r="F94" s="145"/>
-      <c r="G94" s="145"/>
+      <c r="B94" s="146"/>
+      <c r="C94" s="146"/>
+      <c r="D94" s="146"/>
+      <c r="E94" s="146"/>
+      <c r="F94" s="146"/>
+      <c r="G94" s="146"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D95" s="62"/>
@@ -16880,15 +16890,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
@@ -17171,15 +17181,15 @@
       <c r="C27" s="66"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="145" t="s">
+      <c r="A28" s="146" t="s">
         <v>227</v>
       </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="72"/>
@@ -17268,15 +17278,15 @@
       <c r="B36" s="87"/>
     </row>
     <row r="37" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A37" s="145" t="s">
+      <c r="A37" s="146" t="s">
         <v>219</v>
       </c>
-      <c r="B37" s="145"/>
-      <c r="C37" s="145"/>
-      <c r="D37" s="145"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="145"/>
-      <c r="G37" s="145"/>
+      <c r="B37" s="146"/>
+      <c r="C37" s="146"/>
+      <c r="D37" s="146"/>
+      <c r="E37" s="146"/>
+      <c r="F37" s="146"/>
+      <c r="G37" s="146"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D38" s="63"/>
@@ -17549,33 +17559,33 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="146" t="s">
+      <c r="A62" s="147" t="s">
         <v>162</v>
       </c>
       <c r="B62" s="107">
         <v>14</v>
       </c>
-      <c r="C62" s="148">
+      <c r="C62" s="149">
         <f>_xlfn.NORM.DIST(B63, $B$39, $B$50,TRUE) - _xlfn.NORM.DIST(B62, $B$39, $B$50,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D62" s="152">
+      <c r="D62" s="153">
         <f>_xlfn.NORM.DIST(B63, $B$43, $B$51, TRUE) - _xlfn.NORM.DIST(B62, $B$43, $B$51, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E62" s="148">
+      <c r="E62" s="149">
         <f>_xlfn.NORM.DIST(B63/$B$46, $B$43, $B$52,TRUE) - _xlfn.NORM.DIST(B62/$B$46, $B$43, $B$52,TRUE)</f>
         <v>6.1149796065439257E-3</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="147"/>
+      <c r="A63" s="148"/>
       <c r="B63" s="108">
         <v>19</v>
       </c>
-      <c r="C63" s="149"/>
-      <c r="D63" s="153"/>
-      <c r="E63" s="149"/>
+      <c r="C63" s="150"/>
+      <c r="D63" s="154"/>
+      <c r="E63" s="150"/>
       <c r="G63" s="66"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -17587,12 +17597,12 @@
       <c r="G64" s="66"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="151" t="s">
+      <c r="A65" s="152" t="s">
         <v>214</v>
       </c>
-      <c r="B65" s="151"/>
-      <c r="C65" s="151"/>
-      <c r="D65" s="151"/>
+      <c r="B65" s="152"/>
+      <c r="C65" s="152"/>
+      <c r="D65" s="152"/>
       <c r="G65" s="66"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -17709,10 +17719,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17724,15 +17734,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="155" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="109"/>
@@ -17941,11 +17951,11 @@
     </row>
     <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="152" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="151"/>
-      <c r="C19" s="151"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="152"/>
       <c r="D19" s="110"/>
       <c r="E19" s="111"/>
       <c r="F19" s="111"/>
@@ -18063,29 +18073,21 @@
       <c r="G29" s="111"/>
     </row>
     <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="154" t="s">
+      <c r="A30" s="155" t="s">
         <v>230</v>
       </c>
       <c r="B30" s="158"/>
       <c r="C30" s="158"/>
       <c r="D30" s="158"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="68" t="s">
-        <v>232</v>
-      </c>
-      <c r="B32" s="157">
-        <v>11.734883999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="68" t="s">
         <v>229</v>
       </c>
-      <c r="B33" s="157">
+      <c r="B32" s="143">
         <v>0.05</v>
       </c>
     </row>
@@ -18093,9 +18095,42 @@
       <c r="A34" s="68" t="s">
         <v>231</v>
       </c>
-      <c r="B34" s="157">
-        <f>_xlfn.F.INV.RT(B33, 1, 3)</f>
+      <c r="B34" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="68" t="s">
+        <v>234</v>
+      </c>
+      <c r="B36" s="143">
+        <f>_xlfn.F.INV.RT(B32, B34, B35)</f>
         <v>10.127964486013932</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="143" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" s="68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="68" t="s">
+        <v>233</v>
+      </c>
+      <c r="B39" s="143">
+        <f>_xlfn.T.INV.2T(B32, B38)</f>
+        <v>3.1824463052837091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added formulas for simple linear regression
</commit_message>
<xml_diff>
--- a/Cheat Sheet.xlsx
+++ b/Cheat Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnova/Projects/business-statistics-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F6BC51-A766-E64F-974F-AE862C3C5A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C281F9-697A-0744-8ED4-EA409446DD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="28800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptive Statistics" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="240">
   <si>
     <t>E</t>
   </si>
@@ -806,6 +806,18 @@
   </si>
   <si>
     <t>DF Slope</t>
+  </si>
+  <si>
+    <t>m (slope)</t>
+  </si>
+  <si>
+    <t>b (y-intercept)</t>
+  </si>
+  <si>
+    <t>average mean</t>
+  </si>
+  <si>
+    <t>x (value)</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1110,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1407,12 +1419,14 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1426,7 +1440,6 @@
     <xf numFmtId="166" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1446,7 +1459,9 @@
     <xf numFmtId="169" fontId="11" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -10238,11 +10253,11 @@
       <c r="B271" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C271" s="144">
+      <c r="C271" s="145">
         <f>_xlfn.COVARIANCE.S(F257:F261,G257:G261)</f>
         <v>10.25</v>
       </c>
-      <c r="D271" s="145"/>
+      <c r="D271" s="146"/>
       <c r="E271"/>
       <c r="F271"/>
       <c r="G271"/>
@@ -10253,11 +10268,11 @@
       <c r="B272" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C272" s="144">
+      <c r="C272" s="145">
         <f>CORREL(F257:F261,G257:G261)</f>
         <v>0.67770909502996846</v>
       </c>
-      <c r="D272" s="145"/>
+      <c r="D272" s="146"/>
       <c r="E272"/>
       <c r="F272"/>
       <c r="G272"/>
@@ -15576,15 +15591,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
       <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -15784,15 +15799,15 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="151" t="s">
+      <c r="A14" s="147" t="s">
         <v>155</v>
       </c>
-      <c r="B14" s="151"/>
-      <c r="C14" s="151"/>
-      <c r="D14" s="151"/>
-      <c r="E14" s="151"/>
-      <c r="F14" s="151"/>
-      <c r="G14" s="151"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="147"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="147"/>
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -15959,13 +15974,13 @@
       <c r="H25" s="66"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="149" t="s">
         <v>162</v>
       </c>
       <c r="B26" s="70">
         <v>29</v>
       </c>
-      <c r="C26" s="149">
+      <c r="C26" s="151">
         <f>$B$18*($B$17-B26) - $B$18*($B$17-B27)</f>
         <v>0.36363636363636365</v>
       </c>
@@ -15974,11 +15989,11 @@
       <c r="H26" s="66"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="148"/>
+      <c r="A27" s="150"/>
       <c r="B27" s="68">
         <v>37</v>
       </c>
-      <c r="C27" s="150"/>
+      <c r="C27" s="152"/>
       <c r="F27" s="66"/>
       <c r="G27" s="69"/>
       <c r="H27" s="66"/>
@@ -15994,15 +16009,15 @@
       <c r="H29" s="66"/>
     </row>
     <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="146" t="s">
+      <c r="A30" s="148" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="146"/>
-      <c r="C30" s="146"/>
-      <c r="D30" s="146"/>
-      <c r="E30" s="146"/>
-      <c r="F30" s="146"/>
-      <c r="G30" s="146"/>
+      <c r="B30" s="148"/>
+      <c r="C30" s="148"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
+      <c r="G30" s="148"/>
       <c r="H30" s="66"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -16133,13 +16148,13 @@
       <c r="G39" s="69"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="147" t="s">
+      <c r="A40" s="149" t="s">
         <v>162</v>
       </c>
       <c r="B40" s="70">
         <v>14</v>
       </c>
-      <c r="C40" s="149">
+      <c r="C40" s="151">
         <f>_xlfn.NORM.DIST(B41,$B$32,$B$33,TRUE) - _xlfn.NORM.DIST(B40,$B$32,$B$33,TRUE)</f>
         <v>9.0980992495193636E-83</v>
       </c>
@@ -16147,11 +16162,11 @@
       <c r="G40" s="69"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="148"/>
+      <c r="A41" s="150"/>
       <c r="B41" s="68">
         <v>19</v>
       </c>
-      <c r="C41" s="150"/>
+      <c r="C41" s="152"/>
       <c r="F41" s="66"/>
       <c r="G41" s="66"/>
     </row>
@@ -16174,15 +16189,15 @@
       <c r="G44" s="66"/>
     </row>
     <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="146" t="s">
+      <c r="A46" s="148" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="146"/>
-      <c r="C46" s="146"/>
-      <c r="D46" s="146"/>
-      <c r="E46" s="146"/>
-      <c r="F46" s="146"/>
-      <c r="G46" s="146"/>
+      <c r="B46" s="148"/>
+      <c r="C46" s="148"/>
+      <c r="D46" s="148"/>
+      <c r="E46" s="148"/>
+      <c r="F46" s="148"/>
+      <c r="G46" s="148"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="92" t="s">
@@ -16279,23 +16294,23 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="147" t="s">
+      <c r="A59" s="149" t="s">
         <v>162</v>
       </c>
       <c r="B59" s="70">
         <v>2</v>
       </c>
-      <c r="C59" s="149">
+      <c r="C59" s="151">
         <f>_xlfn.BINOM.DIST(B60,$B$49,$B$48,TRUE) - _xlfn.BINOM.DIST(B59,$B$49,$B$48,TRUE)</f>
         <v>0.40516176722632513</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="148"/>
+      <c r="A60" s="150"/>
       <c r="B60" s="68">
         <v>6</v>
       </c>
-      <c r="C60" s="150"/>
+      <c r="C60" s="152"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="76"/>
@@ -16313,15 +16328,15 @@
       <c r="C63" s="74"/>
     </row>
     <row r="65" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A65" s="146" t="s">
+      <c r="A65" s="148" t="s">
         <v>159</v>
       </c>
-      <c r="B65" s="146"/>
-      <c r="C65" s="146"/>
-      <c r="D65" s="146"/>
-      <c r="E65" s="146"/>
-      <c r="F65" s="146"/>
-      <c r="G65" s="146"/>
+      <c r="B65" s="148"/>
+      <c r="C65" s="148"/>
+      <c r="D65" s="148"/>
+      <c r="E65" s="148"/>
+      <c r="F65" s="148"/>
+      <c r="G65" s="148"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="92" t="s">
@@ -16389,23 +16404,23 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="147" t="s">
+      <c r="A74" s="149" t="s">
         <v>162</v>
       </c>
       <c r="B74" s="70">
         <v>2</v>
       </c>
-      <c r="C74" s="149">
+      <c r="C74" s="151">
         <f>_xlfn.POISSON.DIST(B75,$B$67,TRUE) - _xlfn.POISSON.DIST(B74,$B$67,TRUE)</f>
         <v>3.4059520973428459E-3</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="148"/>
+      <c r="A75" s="150"/>
       <c r="B75" s="68">
         <v>5</v>
       </c>
-      <c r="C75" s="150"/>
+      <c r="C75" s="152"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="76"/>
@@ -16428,15 +16443,15 @@
       <c r="C79" s="74"/>
     </row>
     <row r="80" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A80" s="146" t="s">
+      <c r="A80" s="148" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="146"/>
-      <c r="C80" s="146"/>
-      <c r="D80" s="146"/>
-      <c r="E80" s="146"/>
-      <c r="F80" s="146"/>
-      <c r="G80" s="146"/>
+      <c r="B80" s="148"/>
+      <c r="C80" s="148"/>
+      <c r="D80" s="148"/>
+      <c r="E80" s="148"/>
+      <c r="F80" s="148"/>
+      <c r="G80" s="148"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B81" s="67"/>
@@ -16505,23 +16520,23 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="147" t="s">
+      <c r="A88" s="149" t="s">
         <v>162</v>
       </c>
       <c r="B88" s="71">
         <v>2.1</v>
       </c>
-      <c r="C88" s="149">
+      <c r="C88" s="151">
         <f>_xlfn.EXPON.DIST(B89,$B$82,TRUE) - _xlfn.EXPON.DIST(B88,$B$82,TRUE)</f>
         <v>0.25047716007445764</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="148"/>
+      <c r="A89" s="150"/>
       <c r="B89" s="136">
         <v>4.5</v>
       </c>
-      <c r="C89" s="150"/>
+      <c r="C89" s="152"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="76"/>
@@ -16544,15 +16559,15 @@
       <c r="C93" s="74"/>
     </row>
     <row r="94" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A94" s="146" t="s">
+      <c r="A94" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="B94" s="146"/>
-      <c r="C94" s="146"/>
-      <c r="D94" s="146"/>
-      <c r="E94" s="146"/>
-      <c r="F94" s="146"/>
-      <c r="G94" s="146"/>
+      <c r="B94" s="148"/>
+      <c r="C94" s="148"/>
+      <c r="D94" s="148"/>
+      <c r="E94" s="148"/>
+      <c r="F94" s="148"/>
+      <c r="G94" s="148"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D95" s="62"/>
@@ -16851,13 +16866,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
     <mergeCell ref="A94:G94"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
@@ -16868,6 +16876,13 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="C88:C89"/>
     <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16890,15 +16905,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="148" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
@@ -17181,15 +17196,15 @@
       <c r="C27" s="66"/>
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="146" t="s">
+      <c r="A28" s="148" t="s">
         <v>227</v>
       </c>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
+      <c r="B28" s="148"/>
+      <c r="C28" s="148"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="148"/>
+      <c r="F28" s="148"/>
+      <c r="G28" s="148"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="72"/>
@@ -17278,15 +17293,15 @@
       <c r="B36" s="87"/>
     </row>
     <row r="37" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A37" s="146" t="s">
+      <c r="A37" s="148" t="s">
         <v>219</v>
       </c>
-      <c r="B37" s="146"/>
-      <c r="C37" s="146"/>
-      <c r="D37" s="146"/>
-      <c r="E37" s="146"/>
-      <c r="F37" s="146"/>
-      <c r="G37" s="146"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="148"/>
+      <c r="D37" s="148"/>
+      <c r="E37" s="148"/>
+      <c r="F37" s="148"/>
+      <c r="G37" s="148"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D38" s="63"/>
@@ -17559,33 +17574,33 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="147" t="s">
+      <c r="A62" s="149" t="s">
         <v>162</v>
       </c>
       <c r="B62" s="107">
         <v>14</v>
       </c>
-      <c r="C62" s="149">
+      <c r="C62" s="151">
         <f>_xlfn.NORM.DIST(B63, $B$39, $B$50,TRUE) - _xlfn.NORM.DIST(B62, $B$39, $B$50,TRUE)</f>
         <v>0</v>
       </c>
-      <c r="D62" s="153">
+      <c r="D62" s="154">
         <f>_xlfn.NORM.DIST(B63, $B$43, $B$51, TRUE) - _xlfn.NORM.DIST(B62, $B$43, $B$51, TRUE)</f>
         <v>0</v>
       </c>
-      <c r="E62" s="149">
+      <c r="E62" s="151">
         <f>_xlfn.NORM.DIST(B63/$B$46, $B$43, $B$52,TRUE) - _xlfn.NORM.DIST(B62/$B$46, $B$43, $B$52,TRUE)</f>
         <v>6.1149796065439257E-3</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="148"/>
+      <c r="A63" s="150"/>
       <c r="B63" s="108">
         <v>19</v>
       </c>
-      <c r="C63" s="150"/>
-      <c r="D63" s="154"/>
-      <c r="E63" s="150"/>
+      <c r="C63" s="152"/>
+      <c r="D63" s="155"/>
+      <c r="E63" s="152"/>
       <c r="G63" s="66"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -17597,12 +17612,12 @@
       <c r="G64" s="66"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="152" t="s">
+      <c r="A65" s="153" t="s">
         <v>214</v>
       </c>
-      <c r="B65" s="152"/>
-      <c r="C65" s="152"/>
-      <c r="D65" s="152"/>
+      <c r="B65" s="153"/>
+      <c r="C65" s="153"/>
+      <c r="D65" s="153"/>
       <c r="G65" s="66"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -17719,10 +17734,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0329EBD4-6806-254B-8444-3A8691549E0B}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17734,15 +17749,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="109"/>
@@ -17951,11 +17966,11 @@
     </row>
     <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="152" t="s">
+      <c r="A19" s="153" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="152"/>
-      <c r="C19" s="152"/>
+      <c r="B19" s="153"/>
+      <c r="C19" s="153"/>
       <c r="D19" s="110"/>
       <c r="E19" s="111"/>
       <c r="F19" s="111"/>
@@ -18073,18 +18088,18 @@
       <c r="G29" s="111"/>
     </row>
     <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A30" s="155" t="s">
+      <c r="A30" s="156" t="s">
         <v>230</v>
       </c>
-      <c r="B30" s="158"/>
-      <c r="C30" s="158"/>
-      <c r="D30" s="158"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="160" t="s">
         <v>229</v>
       </c>
       <c r="B32" s="143">
@@ -18092,45 +18107,78 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="68" t="s">
+      <c r="A34" s="160" t="s">
         <v>231</v>
       </c>
-      <c r="B34" s="159">
+      <c r="B34" s="144">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="68" t="s">
+      <c r="A35" s="160" t="s">
         <v>232</v>
       </c>
-      <c r="B35" s="159">
+      <c r="B35" s="144">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="160" t="s">
         <v>234</v>
       </c>
-      <c r="B36" s="143">
+      <c r="B36" s="161">
         <f>_xlfn.F.INV.RT(B32, B34, B35)</f>
         <v>10.127964486013932</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="143" t="s">
+      <c r="A38" s="161" t="s">
         <v>235</v>
       </c>
-      <c r="B38" s="68">
+      <c r="B38" s="162">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="68" t="s">
+      <c r="A39" s="160" t="s">
         <v>233</v>
       </c>
-      <c r="B39" s="143">
+      <c r="B39" s="161">
         <f>_xlfn.T.INV.2T(B32, B38)</f>
         <v>3.1824463052837091</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="160" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" s="143">
+        <v>1.2597</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="160" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" s="143">
+        <v>-28.917999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="160" t="s">
+        <v>239</v>
+      </c>
+      <c r="B43" s="84">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="160" t="s">
+        <v>238</v>
+      </c>
+      <c r="B44" s="161">
+        <f>B41*B43+B42</f>
+        <v>59.261000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>